<commit_message>
se agregaron las actividades, y comentarios en la descripcion de funciones del la estructura de manu
</commit_message>
<xml_diff>
--- a/00-Documentacion/Listado_Modulos2.xlsx
+++ b/00-Documentacion/Listado_Modulos2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\source\repos\migracion_spooler\00-Documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\pc\raul\Net\migracion_spooler\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88BFA5B3-8BC0-407C-A942-C793355FEC12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{948A81AE-9AA1-491F-8B54-6834EE202F7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="859" activeTab="3" xr2:uid="{9A494972-654C-41EC-A971-3BEDBD7DDBA9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="859" activeTab="1" xr2:uid="{9A494972-654C-41EC-A971-3BEDBD7DDBA9}"/>
   </bookViews>
   <sheets>
     <sheet name="Opción de Menú vs Funcion param" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="779" uniqueCount="592">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="613">
   <si>
     <t>Opción de Menú</t>
   </si>
@@ -1818,6 +1818,73 @@
   </si>
   <si>
     <t>listado expedientes de que se tiene enviar por  ws (son generados por el modulo), al portal CISE -190 archivos</t>
+  </si>
+  <si>
+    <t>anexo24_cnh</t>
+  </si>
+  <si>
+    <t>cfd_logis_reporteador</t>
+  </si>
+  <si>
+    <t>trading_genera_GSK</t>
+  </si>
+  <si>
+    <t>trading_genera_TLN</t>
+  </si>
+  <si>
+    <t>trading_genera_TMS</t>
+  </si>
+  <si>
+    <t>Carga_Requisitos</t>
+  </si>
+  <si>
+    <t>email_digit_clientes</t>
+  </si>
+  <si>
+    <t>fusion_trac_disponer</t>
+  </si>
+  <si>
+    <t>facturas_txt</t>
+  </si>
+  <si>
+    <t>facturas_cargos</t>
+  </si>
+  <si>
+    <t>factura_pedimento</t>
+  </si>
+  <si>
+    <t>ftp_digit_talon</t>
+  </si>
+  <si>
+    <t>mi_ocp_consulta</t>
+  </si>
+  <si>
+    <t>ocp_generacion_xml</t>
+  </si>
+  <si>
+    <t>Contemplar las funciones o proceso de webservices, envio de correo y los 5 sql que esta de forma secuencial</t>
+  </si>
+  <si>
+    <t>Tema</t>
+  </si>
+  <si>
+    <t>Descripcion</t>
+  </si>
+  <si>
+    <t>prueba del proceso de generacion de pdf</t>
+  </si>
+  <si>
+    <t>Solicitud de envió de exe de genera pdf (prubas)   Solicita archivos de configuración
+   CA60.dll
+   CORE40.dll
+   ORA805.dll
+   NLSRTL33.dll</t>
+  </si>
+  <si>
+    <t>estrutura de objetos</t>
+  </si>
+  <si>
+    <t>reunion con lulu verificacion  de estrutura de objetos de bD</t>
   </si>
 </sst>
 </file>
@@ -1912,7 +1979,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1940,6 +2007,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF8EA9DB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2059,7 +2132,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2171,6 +2244,13 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2548,10 +2628,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2793532-E55B-4B24-AE52-361B14773BDB}">
-  <dimension ref="A1:I314"/>
+  <dimension ref="A1:I317"/>
   <sheetViews>
-    <sheetView topLeftCell="B301" workbookViewId="0">
-      <selection activeCell="G310" sqref="G310"/>
+    <sheetView topLeftCell="A271" workbookViewId="0">
+      <selection activeCell="D288" sqref="D288"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2745,6 +2825,9 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>13</v>
+      </c>
       <c r="C12" s="4" t="s">
         <v>321</v>
       </c>
@@ -2754,7 +2837,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>13</v>
@@ -2768,7 +2851,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>14</v>
@@ -2782,7 +2865,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>15</v>
@@ -2796,7 +2879,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>16</v>
@@ -2810,7 +2893,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>17</v>
@@ -2827,7 +2910,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>18</v>
@@ -2841,7 +2924,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>19</v>
@@ -2855,7 +2938,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>20</v>
@@ -2872,7 +2955,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>21</v>
@@ -2886,7 +2969,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>22</v>
@@ -2900,7 +2983,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>23</v>
@@ -2914,7 +2997,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>24</v>
@@ -2928,7 +3011,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>25</v>
@@ -2942,7 +3025,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>26</v>
@@ -2956,7 +3039,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>27</v>
@@ -2970,7 +3053,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>28</v>
@@ -2984,7 +3067,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>29</v>
@@ -2998,7 +3081,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>30</v>
@@ -3015,7 +3098,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>31</v>
@@ -3029,7 +3112,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>32</v>
@@ -3043,7 +3126,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>33</v>
@@ -3057,7 +3140,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>34</v>
@@ -3071,7 +3154,7 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>35</v>
@@ -3085,7 +3168,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>36</v>
@@ -3102,7 +3185,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>37</v>
@@ -3116,7 +3199,7 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>38</v>
@@ -3130,7 +3213,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>39</v>
@@ -3144,7 +3227,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>40</v>
@@ -3158,7 +3241,7 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>41</v>
@@ -3172,7 +3255,7 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>42</v>
@@ -3186,7 +3269,7 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>43</v>
@@ -3200,7 +3283,7 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>44</v>
@@ -3223,7 +3306,7 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>45</v>
@@ -3237,7 +3320,7 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>46</v>
@@ -3254,7 +3337,7 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>47</v>
@@ -3268,7 +3351,7 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>48</v>
@@ -3282,7 +3365,7 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>49</v>
@@ -3296,7 +3379,7 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>50</v>
@@ -3310,7 +3393,7 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>51</v>
@@ -3324,7 +3407,7 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>52</v>
@@ -3338,7 +3421,7 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>53</v>
@@ -3352,7 +3435,7 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>54</v>
@@ -3366,7 +3449,7 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>55</v>
@@ -3380,7 +3463,7 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>56</v>
@@ -3394,7 +3477,7 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>57</v>
@@ -3408,7 +3491,7 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>58</v>
@@ -3422,7 +3505,7 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>59</v>
@@ -3436,7 +3519,7 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>60</v>
@@ -3450,7 +3533,7 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>61</v>
@@ -3464,7 +3547,7 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>62</v>
@@ -3478,7 +3561,7 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>63</v>
@@ -3495,7 +3578,7 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>64</v>
@@ -3509,7 +3592,7 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>65</v>
@@ -3523,7 +3606,7 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>66</v>
@@ -3537,7 +3620,7 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>67</v>
@@ -3554,7 +3637,7 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>68</v>
@@ -3571,7 +3654,7 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>69</v>
@@ -3585,7 +3668,7 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>70</v>
@@ -3599,7 +3682,7 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>71</v>
@@ -3616,7 +3699,7 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>72</v>
@@ -3630,7 +3713,7 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>73</v>
@@ -3644,7 +3727,7 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>74</v>
@@ -3658,7 +3741,7 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>75</v>
@@ -3672,7 +3755,7 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>76</v>
@@ -3686,7 +3769,7 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>77</v>
@@ -3700,7 +3783,7 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>78</v>
@@ -3714,7 +3797,7 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>79</v>
@@ -3728,7 +3811,7 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>80</v>
@@ -3742,7 +3825,7 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>81</v>
@@ -3756,7 +3839,7 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>82</v>
@@ -3770,7 +3853,7 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>83</v>
@@ -3784,7 +3867,7 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>84</v>
@@ -3798,7 +3881,7 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>85</v>
@@ -3812,7 +3895,7 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>86</v>
@@ -3826,7 +3909,7 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>87</v>
@@ -3843,7 +3926,7 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>88</v>
@@ -3860,7 +3943,7 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>89</v>
@@ -3874,7 +3957,7 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>90</v>
@@ -3888,7 +3971,7 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>91</v>
@@ -3902,7 +3985,7 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>92</v>
@@ -3916,7 +3999,7 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>93</v>
@@ -3930,7 +4013,7 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>94</v>
@@ -3944,7 +4027,7 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>95</v>
@@ -3958,7 +4041,7 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>96</v>
@@ -3972,7 +4055,7 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>97</v>
@@ -3989,7 +4072,7 @@
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>98</v>
@@ -4003,7 +4086,7 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>99</v>
@@ -4017,7 +4100,7 @@
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>100</v>
@@ -4031,7 +4114,7 @@
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>101</v>
@@ -4045,7 +4128,7 @@
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>102</v>
@@ -4059,7 +4142,7 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>103</v>
@@ -4073,7 +4156,7 @@
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>104</v>
@@ -4087,7 +4170,7 @@
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>105</v>
@@ -4101,7 +4184,7 @@
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>106</v>
@@ -4115,7 +4198,7 @@
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C107" s="1" t="s">
         <v>107</v>
@@ -4132,7 +4215,7 @@
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>108</v>
@@ -4149,7 +4232,7 @@
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="2">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C109" s="1" t="s">
         <v>109</v>
@@ -4166,7 +4249,7 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="2">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>110</v>
@@ -4183,7 +4266,7 @@
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="2">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>111</v>
@@ -4200,7 +4283,7 @@
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="2">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>112</v>
@@ -4214,7 +4297,7 @@
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="2">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>113</v>
@@ -4231,7 +4314,7 @@
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="2">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>114</v>
@@ -4245,7 +4328,7 @@
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="2">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>115</v>
@@ -4265,7 +4348,7 @@
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="2">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C116" s="1" t="s">
         <v>116</v>
@@ -4279,7 +4362,7 @@
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="2">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C117" s="1" t="s">
         <v>117</v>
@@ -4293,7 +4376,7 @@
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="2">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C118" s="1" t="s">
         <v>118</v>
@@ -4307,7 +4390,7 @@
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="2">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C119" s="1" t="s">
         <v>119</v>
@@ -4321,7 +4404,7 @@
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="2">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C120" s="1" t="s">
         <v>120</v>
@@ -4335,7 +4418,7 @@
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" s="2">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C121" s="1" t="s">
         <v>121</v>
@@ -4349,7 +4432,7 @@
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" s="2">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C122" s="1" t="s">
         <v>122</v>
@@ -4363,7 +4446,7 @@
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" s="2">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C123" s="1" t="s">
         <v>124</v>
@@ -4377,7 +4460,7 @@
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" s="2">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>326</v>
@@ -4394,7 +4477,7 @@
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" s="2">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C125" s="1" t="s">
         <v>126</v>
@@ -4411,7 +4494,7 @@
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" s="2">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C126" s="1" t="s">
         <v>127</v>
@@ -4428,7 +4511,7 @@
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" s="2">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C127" s="1" t="s">
         <v>128</v>
@@ -4448,7 +4531,7 @@
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" s="2">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C128" s="1" t="s">
         <v>129</v>
@@ -4468,7 +4551,7 @@
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" s="2">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C129" s="1" t="s">
         <v>130</v>
@@ -4485,7 +4568,7 @@
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" s="2">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C130" s="1" t="s">
         <v>131</v>
@@ -4499,7 +4582,7 @@
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" s="2">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C131" s="1" t="s">
         <v>132</v>
@@ -4513,7 +4596,7 @@
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" s="2">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C132" s="1" t="s">
         <v>133</v>
@@ -4527,7 +4610,7 @@
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" s="2">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C133" s="1" t="s">
         <v>134</v>
@@ -4541,7 +4624,7 @@
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" s="2">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C134" s="1" t="s">
         <v>135</v>
@@ -4558,7 +4641,7 @@
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" s="2">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C135" s="1" t="s">
         <v>136</v>
@@ -4584,7 +4667,7 @@
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" s="2">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C136" s="1" t="s">
         <v>137</v>
@@ -4610,7 +4693,7 @@
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" s="2">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C137" s="1" t="s">
         <v>138</v>
@@ -4624,7 +4707,7 @@
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" s="2">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C138" s="1" t="s">
         <v>139</v>
@@ -4644,7 +4727,7 @@
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" s="2">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C139" s="1" t="s">
         <v>140</v>
@@ -4664,7 +4747,7 @@
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" s="2">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C140" s="1" t="s">
         <v>141</v>
@@ -4678,7 +4761,7 @@
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" s="2">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C141" s="1" t="s">
         <v>142</v>
@@ -4692,7 +4775,7 @@
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" s="2">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C142" s="1" t="s">
         <v>143</v>
@@ -4706,7 +4789,7 @@
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" s="2">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C143" s="1" t="s">
         <v>144</v>
@@ -4723,7 +4806,7 @@
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" s="2">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C144" s="1" t="s">
         <v>145</v>
@@ -4737,7 +4820,7 @@
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" s="2">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C145" s="1" t="s">
         <v>146</v>
@@ -4751,7 +4834,7 @@
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" s="2">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C146" s="1" t="s">
         <v>147</v>
@@ -4768,7 +4851,7 @@
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" s="2">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C147" s="1" t="s">
         <v>148</v>
@@ -4782,7 +4865,7 @@
     </row>
     <row r="148" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A148" s="2">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C148" s="1" t="s">
         <v>149</v>
@@ -4796,7 +4879,7 @@
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" s="2">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C149" s="1" t="s">
         <v>150</v>
@@ -4813,7 +4896,7 @@
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150" s="2">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C150" s="1" t="s">
         <v>151</v>
@@ -4827,7 +4910,7 @@
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151" s="2">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C151" s="1" t="s">
         <v>152</v>
@@ -4841,7 +4924,7 @@
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152" s="2">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C152" s="1" t="s">
         <v>153</v>
@@ -4858,7 +4941,7 @@
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C153" s="1" t="s">
         <v>154</v>
@@ -4878,7 +4961,7 @@
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" s="2">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C154" s="1" t="s">
         <v>155</v>
@@ -4892,7 +4975,7 @@
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" s="2">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C155" s="1" t="s">
         <v>156</v>
@@ -4906,7 +4989,7 @@
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" s="2">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C156" s="1" t="s">
         <v>157</v>
@@ -4920,7 +5003,7 @@
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" s="2">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C157" s="1" t="s">
         <v>158</v>
@@ -4934,7 +5017,7 @@
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158" s="2">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C158" s="1" t="s">
         <v>159</v>
@@ -4948,7 +5031,7 @@
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159" s="2">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C159" s="1" t="s">
         <v>160</v>
@@ -4962,7 +5045,7 @@
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160" s="2">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C160" s="1" t="s">
         <v>161</v>
@@ -4976,7 +5059,7 @@
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="2">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C161" s="1" t="s">
         <v>162</v>
@@ -4990,7 +5073,7 @@
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="2">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C162" s="1" t="s">
         <v>163</v>
@@ -5004,7 +5087,7 @@
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="2">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C163" s="1" t="s">
         <v>164</v>
@@ -5018,7 +5101,7 @@
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" s="2">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C164" s="1" t="s">
         <v>165</v>
@@ -5032,7 +5115,7 @@
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="2">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C165" s="1" t="s">
         <v>166</v>
@@ -5046,7 +5129,7 @@
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="2">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C166" s="1" t="s">
         <v>167</v>
@@ -5060,7 +5143,7 @@
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="2">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C167" s="1" t="s">
         <v>168</v>
@@ -5074,7 +5157,7 @@
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="2">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C168" s="1" t="s">
         <v>169</v>
@@ -5088,7 +5171,7 @@
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="2">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C169" s="1" t="s">
         <v>170</v>
@@ -5102,7 +5185,7 @@
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" s="2">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C170" s="1" t="s">
         <v>171</v>
@@ -5116,7 +5199,7 @@
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" s="2">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C171" s="1" t="s">
         <v>172</v>
@@ -5130,7 +5213,7 @@
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" s="2">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C172" s="1" t="s">
         <v>173</v>
@@ -5144,7 +5227,7 @@
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" s="2">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C173" s="1" t="s">
         <v>174</v>
@@ -5158,7 +5241,7 @@
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" s="2">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C174" s="1" t="s">
         <v>175</v>
@@ -5172,7 +5255,7 @@
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" s="2">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C175" s="1" t="s">
         <v>176</v>
@@ -5186,7 +5269,7 @@
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" s="2">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C176" s="1" t="s">
         <v>177</v>
@@ -5200,7 +5283,7 @@
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" s="2">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C177" s="1" t="s">
         <v>178</v>
@@ -5214,7 +5297,7 @@
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" s="2">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C178" s="1" t="s">
         <v>179</v>
@@ -5228,7 +5311,7 @@
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" s="2">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C179" s="1" t="s">
         <v>180</v>
@@ -5242,7 +5325,7 @@
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" s="2">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C180" s="1" t="s">
         <v>181</v>
@@ -5256,7 +5339,7 @@
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" s="2">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C181" s="1" t="s">
         <v>182</v>
@@ -5270,7 +5353,7 @@
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" s="2">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B182" s="1" t="s">
         <v>326</v>
@@ -5287,7 +5370,7 @@
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" s="2">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C183" s="1" t="s">
         <v>184</v>
@@ -5301,7 +5384,7 @@
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" s="2">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C184" s="1" t="s">
         <v>185</v>
@@ -5315,7 +5398,7 @@
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" s="2">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C185" s="1" t="s">
         <v>186</v>
@@ -5329,7 +5412,7 @@
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" s="2">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C186" s="1" t="s">
         <v>187</v>
@@ -5343,7 +5426,7 @@
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" s="2">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C187" s="1" t="s">
         <v>188</v>
@@ -5357,7 +5440,7 @@
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" s="2">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C188" s="1" t="s">
         <v>189</v>
@@ -5371,7 +5454,7 @@
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" s="2">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C189" s="1" t="s">
         <v>190</v>
@@ -5385,7 +5468,7 @@
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" s="2">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C190" s="1" t="s">
         <v>191</v>
@@ -5399,7 +5482,7 @@
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" s="2">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C191" s="1" t="s">
         <v>192</v>
@@ -5413,7 +5496,7 @@
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" s="2">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C192" s="1" t="s">
         <v>193</v>
@@ -5427,7 +5510,7 @@
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A193" s="2">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C193" s="1" t="s">
         <v>194</v>
@@ -5441,7 +5524,7 @@
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A194" s="2">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C194" s="1" t="s">
         <v>195</v>
@@ -5455,7 +5538,7 @@
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A195" s="2">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C195" s="1" t="s">
         <v>196</v>
@@ -5469,7 +5552,7 @@
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A196" s="2">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C196" s="1" t="s">
         <v>197</v>
@@ -5483,7 +5566,7 @@
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A197" s="2">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C197" s="1" t="s">
         <v>198</v>
@@ -5497,7 +5580,7 @@
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A198" s="2">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C198" s="1" t="s">
         <v>199</v>
@@ -5511,7 +5594,7 @@
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199" s="2">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C199" s="1" t="s">
         <v>200</v>
@@ -5525,7 +5608,7 @@
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A200" s="2">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C200" s="1" t="s">
         <v>201</v>
@@ -5542,7 +5625,7 @@
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A201" s="2">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C201" s="1" t="s">
         <v>202</v>
@@ -5556,7 +5639,7 @@
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A202" s="2">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="C202" s="1" t="s">
         <v>203</v>
@@ -5570,7 +5653,7 @@
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A203" s="2">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C203" s="1" t="s">
         <v>204</v>
@@ -5584,7 +5667,7 @@
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A204" s="2">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C204" s="1" t="s">
         <v>205</v>
@@ -5598,7 +5681,7 @@
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A205" s="2">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C205" s="1" t="s">
         <v>206</v>
@@ -5612,7 +5695,7 @@
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A206" s="2">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C206" s="1" t="s">
         <v>207</v>
@@ -5626,7 +5709,7 @@
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A207" s="2">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C207" s="1" t="s">
         <v>208</v>
@@ -5640,7 +5723,7 @@
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A208" s="2">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C208" s="1" t="s">
         <v>209</v>
@@ -5654,7 +5737,7 @@
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A209" s="2">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C209" s="1" t="s">
         <v>210</v>
@@ -5668,7 +5751,7 @@
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A210" s="2">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C210" s="1" t="s">
         <v>211</v>
@@ -5682,7 +5765,7 @@
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A211" s="2">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C211" s="1" t="s">
         <v>212</v>
@@ -5695,6 +5778,9 @@
       </c>
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A212" s="2">
+        <v>213</v>
+      </c>
       <c r="D212" s="1" t="s">
         <v>456</v>
       </c>
@@ -5704,7 +5790,7 @@
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A213" s="2">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C213" s="1" t="s">
         <v>213</v>
@@ -5718,7 +5804,7 @@
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A214" s="2">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C214" s="1" t="s">
         <v>214</v>
@@ -5732,15 +5818,18 @@
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A215" s="2">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C215" s="1" t="s">
         <v>215</v>
       </c>
+      <c r="D215" s="1" t="s">
+        <v>326</v>
+      </c>
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A216" s="2">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C216" s="1" t="s">
         <v>216</v>
@@ -5754,7 +5843,7 @@
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A217" s="2">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C217" s="1" t="s">
         <v>217</v>
@@ -5768,7 +5857,7 @@
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A218" s="2">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C218" s="1" t="s">
         <v>218</v>
@@ -5782,7 +5871,7 @@
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A219" s="2">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C219" s="1" t="s">
         <v>219</v>
@@ -5799,7 +5888,7 @@
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A220" s="2">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C220" s="1" t="s">
         <v>220</v>
@@ -5813,7 +5902,7 @@
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A221" s="2">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C221" s="1" t="s">
         <v>221</v>
@@ -5827,7 +5916,7 @@
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A222" s="2">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C222" s="1" t="s">
         <v>222</v>
@@ -5844,7 +5933,7 @@
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A223" s="2">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C223" s="1" t="s">
         <v>223</v>
@@ -5858,7 +5947,7 @@
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A224" s="2">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C224" s="1" t="s">
         <v>224</v>
@@ -5872,7 +5961,7 @@
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A225" s="2">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C225" s="1" t="s">
         <v>225</v>
@@ -5886,7 +5975,7 @@
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A226" s="2">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C226" s="1" t="s">
         <v>226</v>
@@ -5900,7 +5989,7 @@
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A227" s="2">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C227" s="1" t="s">
         <v>227</v>
@@ -5914,7 +6003,7 @@
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A228" s="2">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C228" s="1" t="s">
         <v>228</v>
@@ -5928,7 +6017,7 @@
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A229" s="2">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C229" s="1" t="s">
         <v>229</v>
@@ -5942,7 +6031,7 @@
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A230" s="2">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C230" s="1" t="s">
         <v>230</v>
@@ -5956,7 +6045,7 @@
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A231" s="2">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C231" s="1" t="s">
         <v>231</v>
@@ -5970,7 +6059,7 @@
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A232" s="2">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C232" s="1" t="s">
         <v>232</v>
@@ -5984,7 +6073,7 @@
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A233" s="2">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C233" s="1" t="s">
         <v>233</v>
@@ -5998,7 +6087,7 @@
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A234" s="2">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C234" s="1" t="s">
         <v>234</v>
@@ -6012,7 +6101,7 @@
     </row>
     <row r="235" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A235" s="2">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C235" s="1" t="s">
         <v>235</v>
@@ -6026,7 +6115,7 @@
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A236" s="2">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C236" s="1" t="s">
         <v>236</v>
@@ -6040,7 +6129,7 @@
     </row>
     <row r="237" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A237" s="2">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C237" s="1" t="s">
         <v>237</v>
@@ -6057,7 +6146,7 @@
     </row>
     <row r="238" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A238" s="2">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C238" s="1" t="s">
         <v>238</v>
@@ -6071,7 +6160,7 @@
     </row>
     <row r="239" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A239" s="2">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C239" s="1" t="s">
         <v>239</v>
@@ -6085,7 +6174,7 @@
     </row>
     <row r="240" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A240" s="2">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C240" s="1" t="s">
         <v>240</v>
@@ -6099,7 +6188,7 @@
     </row>
     <row r="241" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A241" s="2">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C241" s="1" t="s">
         <v>241</v>
@@ -6113,7 +6202,7 @@
     </row>
     <row r="242" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A242" s="2">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C242" s="1" t="s">
         <v>242</v>
@@ -6127,7 +6216,7 @@
     </row>
     <row r="243" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A243" s="2">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C243" s="1" t="s">
         <v>243</v>
@@ -6141,7 +6230,7 @@
     </row>
     <row r="244" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A244" s="2">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C244" s="1" t="s">
         <v>244</v>
@@ -6155,7 +6244,7 @@
     </row>
     <row r="245" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A245" s="2">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C245" s="1" t="s">
         <v>245</v>
@@ -6169,7 +6258,7 @@
     </row>
     <row r="246" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A246" s="2">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C246" s="1" t="s">
         <v>246</v>
@@ -6183,7 +6272,7 @@
     </row>
     <row r="247" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A247" s="2">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C247" s="1" t="s">
         <v>247</v>
@@ -6200,7 +6289,7 @@
     </row>
     <row r="248" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A248" s="2">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C248" s="1" t="s">
         <v>248</v>
@@ -6217,7 +6306,7 @@
     </row>
     <row r="249" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A249" s="2">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C249" s="1" t="s">
         <v>249</v>
@@ -6231,7 +6320,7 @@
     </row>
     <row r="250" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A250" s="2">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C250" s="1" t="s">
         <v>250</v>
@@ -6244,6 +6333,9 @@
       </c>
     </row>
     <row r="251" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A251" s="2">
+        <v>252</v>
+      </c>
       <c r="D251" s="1" t="s">
         <v>576</v>
       </c>
@@ -6252,6 +6344,9 @@
       </c>
     </row>
     <row r="252" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A252" s="2">
+        <v>253</v>
+      </c>
       <c r="D252" s="1" t="s">
         <v>577</v>
       </c>
@@ -6261,7 +6356,7 @@
     </row>
     <row r="253" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A253" s="2">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C253" s="1" t="s">
         <v>251</v>
@@ -6275,7 +6370,7 @@
     </row>
     <row r="254" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A254" s="2">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C254" s="1" t="s">
         <v>252</v>
@@ -6289,7 +6384,7 @@
     </row>
     <row r="255" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A255" s="2">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C255" s="1" t="s">
         <v>253</v>
@@ -6303,7 +6398,7 @@
     </row>
     <row r="256" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A256" s="2">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C256" s="1" t="s">
         <v>254</v>
@@ -6315,49 +6410,79 @@
         <v>8</v>
       </c>
     </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A257" s="2">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C257" s="1" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D257" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="E257" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A258" s="2">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C258" s="1" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D258" s="1" t="s">
+        <v>592</v>
+      </c>
+      <c r="E258" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A259" s="2">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C259" s="1" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D259" s="1" t="s">
+        <v>593</v>
+      </c>
+      <c r="E259" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A260" s="2">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C260" s="1" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="261" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D260" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="E260" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A261" s="2">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C261" s="1" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D261" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="E261" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A262" s="2">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B262" s="1" t="s">
         <v>326</v>
@@ -6365,446 +6490,614 @@
       <c r="C262" s="1" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="263" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D262" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="E262" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A263" s="2">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C263" s="1" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="264" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D263" s="1" t="s">
+        <v>594</v>
+      </c>
+      <c r="E263" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A264" s="2">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C264" s="1" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="265" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D264" s="1" t="s">
+        <v>595</v>
+      </c>
+      <c r="E264" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A265" s="2">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C265" s="1" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="266" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D265" s="1" t="s">
+        <v>596</v>
+      </c>
+      <c r="E265" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A266" s="2">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C266" s="1" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="267" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D266" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="E266" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A267" s="2">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C267" s="1" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="268" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D267" s="1" t="s">
+        <v>597</v>
+      </c>
+      <c r="E267" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A268" s="2">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C268" s="1" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="269" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D268" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="E268" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A269" s="2">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C269" s="1" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="270" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D269" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="E269" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A270" s="2">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C270" s="1" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="271" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D270" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="E270" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A271" s="2">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C271" s="1" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="272" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D271" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="E271" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A272" s="2">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C272" s="1" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="273" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D272" s="1" t="s">
+        <v>598</v>
+      </c>
+      <c r="E272" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A273" s="2">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C273" s="1" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="274" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D273" s="1" t="s">
+        <v>599</v>
+      </c>
+      <c r="E273" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A274" s="2">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C274" s="1" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="275" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D274" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="E274" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A275" s="2">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C275" s="1" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="276" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D275" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="E275" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A276" s="2">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C276" s="1" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="277" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D276" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="E276" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A277" s="2">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C277" s="1" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="278" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D277" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="E277" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A278" s="2">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C278" s="1" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="279" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D278" s="1" t="s">
+        <v>600</v>
+      </c>
+      <c r="E278" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A279" s="2">
+        <v>280</v>
+      </c>
+      <c r="D279" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="E279" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A280" s="2">
         <v>281</v>
       </c>
-      <c r="C279" s="1" t="s">
+      <c r="C280" s="1" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="280" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A280" s="2">
+      <c r="D280" s="1" t="s">
+        <v>602</v>
+      </c>
+      <c r="E280" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A281" s="2">
         <v>282</v>
       </c>
-      <c r="C280" s="1" t="s">
+      <c r="C281" s="1" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="281" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A281" s="2">
+      <c r="D281" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="E281" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A282" s="2">
         <v>283</v>
       </c>
-      <c r="C281" s="1" t="s">
+      <c r="C282" s="1" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="282" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A282" s="2">
+      <c r="D282" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="E282" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A283" s="2">
         <v>284</v>
       </c>
-      <c r="C282" s="1" t="s">
+      <c r="C283" s="1" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="283" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A283" s="2">
+      <c r="D283" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="E283" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A284" s="2">
         <v>285</v>
       </c>
-      <c r="C283" s="1" t="s">
+      <c r="C284" s="1" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="284" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A284" s="2">
+      <c r="D284" s="1" t="s">
+        <v>604</v>
+      </c>
+      <c r="E284" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A285" s="2">
         <v>286</v>
       </c>
-      <c r="C284" s="1" t="s">
+      <c r="C285" s="1" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="285" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A285" s="2">
+      <c r="D285" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="E285" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A286" s="2">
         <v>287</v>
       </c>
-      <c r="C285" s="1" t="s">
+      <c r="D286" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="E286" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A287" s="2">
+        <v>288</v>
+      </c>
+      <c r="C287" s="1" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="286" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A286" s="2">
+    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A288" s="2">
+        <v>289</v>
+      </c>
+      <c r="C288" s="1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="289" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A289" s="2">
+        <v>290</v>
+      </c>
+      <c r="C289" s="1" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="290" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A290" s="2">
+        <v>291</v>
+      </c>
+      <c r="C290" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="291" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A291" s="2">
+        <v>292</v>
+      </c>
+      <c r="C291" s="1" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="292" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A292" s="2">
+        <v>293</v>
+      </c>
+      <c r="C292" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="C286" s="1" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="287" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A287" s="2">
+    </row>
+    <row r="293" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A293" s="2">
+        <v>294</v>
+      </c>
+      <c r="C293" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="C287" s="1" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="288" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A288" s="2">
+    </row>
+    <row r="294" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A294" s="2">
+        <v>295</v>
+      </c>
+      <c r="B294" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="C294" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="C288" s="1" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A289" s="2">
+    </row>
+    <row r="295" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A295" s="2">
+        <v>296</v>
+      </c>
+      <c r="C295" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="C289" s="1" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A290" s="2">
+    </row>
+    <row r="296" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A296" s="2">
+        <v>297</v>
+      </c>
+      <c r="C296" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="C290" s="1" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A291" s="2">
+    </row>
+    <row r="297" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A297" s="2">
+        <v>298</v>
+      </c>
+      <c r="C297" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="C291" s="1" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A292" s="2">
+    </row>
+    <row r="298" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A298" s="2">
+        <v>299</v>
+      </c>
+      <c r="C298" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="B292" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="C292" s="1" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A293" s="2">
+    </row>
+    <row r="299" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A299" s="2">
+        <v>300</v>
+      </c>
+      <c r="C299" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="C293" s="1" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A294" s="2">
+    </row>
+    <row r="300" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A300" s="2">
+        <v>301</v>
+      </c>
+      <c r="C300" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="C294" s="1" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A295" s="2">
+    </row>
+    <row r="301" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A301" s="2">
+        <v>302</v>
+      </c>
+      <c r="C301" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="C295" s="1" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A296" s="2">
+    </row>
+    <row r="302" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A302" s="2">
+        <v>303</v>
+      </c>
+      <c r="C302" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="C296" s="1" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A297" s="2">
+    </row>
+    <row r="303" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A303" s="2">
+        <v>304</v>
+      </c>
+      <c r="C303" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="C297" s="1" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A298" s="2">
+    </row>
+    <row r="304" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A304" s="2">
+        <v>305</v>
+      </c>
+      <c r="C304" s="1" t="s">
         <v>300</v>
-      </c>
-      <c r="C298" s="1" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A299" s="2">
-        <v>301</v>
-      </c>
-      <c r="C299" s="1" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A300" s="2">
-        <v>302</v>
-      </c>
-      <c r="C300" s="1" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A301" s="2">
-        <v>303</v>
-      </c>
-      <c r="C301" s="1" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="302" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A302" s="2">
-        <v>304</v>
-      </c>
-      <c r="C302" s="1" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="303" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A303" s="2">
-        <v>305</v>
-      </c>
-      <c r="C303" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="D303" s="1" t="s">
-        <v>457</v>
-      </c>
-      <c r="E303" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="304" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A304" s="2">
-        <v>306</v>
-      </c>
-      <c r="B304" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="C304" s="1" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="305" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A305" s="2">
+        <v>306</v>
+      </c>
+      <c r="C305" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="D305" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="E305" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="306" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A306" s="2">
         <v>307</v>
       </c>
-      <c r="C305" s="1" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="306" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A306" s="7">
-        <v>308</v>
-      </c>
-      <c r="B306" s="5"/>
-      <c r="C306" s="5" t="s">
-        <v>304</v>
-      </c>
-      <c r="D306" s="5" t="s">
-        <v>304</v>
-      </c>
-      <c r="E306" s="5">
-        <v>5</v>
+      <c r="B306" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="C306" s="1" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="307" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A307" s="2">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C307" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="308" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A308" s="2">
-        <v>310</v>
-      </c>
-      <c r="C308" s="1" t="s">
-        <v>306</v>
+        <v>309</v>
+      </c>
+      <c r="B308" s="5"/>
+      <c r="C308" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="D308" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="E308" s="5">
+        <v>5</v>
       </c>
     </row>
     <row r="309" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A309" s="2">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C309" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="310" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A310" s="2">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C310" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="311" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A311" s="2">
+        <v>312</v>
+      </c>
+      <c r="C311" s="1" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="312" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A312" s="2">
         <v>313</v>
       </c>
-      <c r="C311" s="1" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="312" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A312" s="7">
-        <v>314</v>
-      </c>
-      <c r="B312" s="5"/>
-      <c r="C312" s="5" t="s">
-        <v>310</v>
-      </c>
-      <c r="D312" s="5" t="s">
-        <v>310</v>
-      </c>
-      <c r="E312" s="5">
-        <v>7</v>
+      <c r="C312" s="1" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="313" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A313" s="2">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C313" s="1" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="314" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A314" s="2">
+        <v>315</v>
+      </c>
+      <c r="B314" s="5"/>
+      <c r="C314" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="D314" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="E314" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="315" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A315" s="2">
         <v>316</v>
       </c>
-      <c r="C314" s="1" t="s">
+      <c r="C315" s="1" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="316" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A316" s="2">
+        <v>317</v>
+      </c>
+      <c r="C316" s="1" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="317" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A317" s="2">
+        <v>317</v>
+      </c>
+      <c r="C317" s="1" t="s">
         <v>312</v>
       </c>
     </row>
@@ -6816,10 +7109,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A24CCD5-B140-49E1-9D6E-67F75307E332}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6837,6 +7130,12 @@
       <c r="B1" t="s">
         <v>585</v>
       </c>
+      <c r="C1" t="s">
+        <v>607</v>
+      </c>
+      <c r="D1" t="s">
+        <v>608</v>
+      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="38">
@@ -6850,6 +7149,34 @@
       </c>
       <c r="D2" t="s">
         <v>584</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A3" s="38">
+        <v>45411</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>609</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="38">
+        <v>45411</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>611</v>
+      </c>
+      <c r="D4" t="s">
+        <v>612</v>
       </c>
     </row>
   </sheetData>
@@ -7008,8 +7335,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD54439F-40DB-4068-9758-9F0A5DA03583}">
   <dimension ref="A1:O18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7117,7 +7444,14 @@
         <v>403</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="39"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="40" t="s">
+        <v>606</v>
+      </c>
+      <c r="E3" s="41"/>
       <c r="F3" t="s">
         <v>463</v>
       </c>
@@ -7399,11 +7733,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="45" t="s">
         <v>499</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="44"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="47"/>
     </row>
     <row r="2" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
@@ -7431,9 +7765,9 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="45"/>
-      <c r="B4" s="46"/>
-      <c r="C4" s="47"/>
+      <c r="A4" s="48"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="50"/>
     </row>
     <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
@@ -7469,9 +7803,9 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="45"/>
-      <c r="B8" s="46"/>
-      <c r="C8" s="47"/>
+      <c r="A8" s="48"/>
+      <c r="B8" s="49"/>
+      <c r="C8" s="50"/>
     </row>
     <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
@@ -7488,9 +7822,9 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="45"/>
-      <c r="B10" s="46"/>
-      <c r="C10" s="47"/>
+      <c r="A10" s="48"/>
+      <c r="B10" s="49"/>
+      <c r="C10" s="50"/>
     </row>
     <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
@@ -7507,9 +7841,9 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="45"/>
-      <c r="B12" s="46"/>
-      <c r="C12" s="47"/>
+      <c r="A12" s="48"/>
+      <c r="B12" s="49"/>
+      <c r="C12" s="50"/>
     </row>
     <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="13" t="s">
@@ -7523,9 +7857,9 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="45"/>
-      <c r="B14" s="46"/>
-      <c r="C14" s="47"/>
+      <c r="A14" s="48"/>
+      <c r="B14" s="49"/>
+      <c r="C14" s="50"/>
     </row>
     <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="21" t="s">
@@ -7539,9 +7873,9 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="39"/>
-      <c r="B16" s="40"/>
-      <c r="C16" s="41"/>
+      <c r="A16" s="42"/>
+      <c r="B16" s="43"/>
+      <c r="C16" s="44"/>
     </row>
     <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="13" t="s">
@@ -7555,9 +7889,9 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="39"/>
-      <c r="B18" s="40"/>
-      <c r="C18" s="41"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="43"/>
+      <c r="C18" s="44"/>
     </row>
     <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="13" t="s">
@@ -7571,9 +7905,9 @@
       </c>
     </row>
     <row r="20" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="39"/>
-      <c r="B20" s="40"/>
-      <c r="C20" s="41"/>
+      <c r="A20" s="42"/>
+      <c r="B20" s="43"/>
+      <c r="C20" s="44"/>
     </row>
     <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="13" t="s">
@@ -7587,9 +7921,9 @@
       </c>
     </row>
     <row r="22" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="39"/>
-      <c r="B22" s="40"/>
-      <c r="C22" s="41"/>
+      <c r="A22" s="42"/>
+      <c r="B22" s="43"/>
+      <c r="C22" s="44"/>
     </row>
     <row r="23" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="13" t="s">
@@ -7635,11 +7969,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="45" t="s">
         <v>521</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="44"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="47"/>
     </row>
     <row r="2" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
@@ -7660,13 +7994,13 @@
       <c r="C3" s="23"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="55" t="s">
         <v>525</v>
       </c>
       <c r="B4" s="24" t="s">
         <v>526</v>
       </c>
-      <c r="C4" s="54" t="s">
+      <c r="C4" s="57" t="s">
         <v>527</v>
       </c>
       <c r="D4" s="7">
@@ -7674,11 +8008,11 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="53"/>
+      <c r="A5" s="56"/>
       <c r="B5" s="25" t="s">
         <v>528</v>
       </c>
-      <c r="C5" s="55"/>
+      <c r="C5" s="58"/>
     </row>
     <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="26" t="s">
@@ -7692,40 +8026,40 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="56" t="s">
+      <c r="A7" s="59" t="s">
         <v>532</v>
       </c>
       <c r="B7" s="29" t="s">
         <v>533</v>
       </c>
-      <c r="C7" s="58" t="s">
+      <c r="C7" s="61" t="s">
         <v>534</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="57"/>
+      <c r="A8" s="60"/>
       <c r="B8" s="30" t="s">
         <v>535</v>
       </c>
-      <c r="C8" s="59"/>
+      <c r="C8" s="62"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="56" t="s">
+      <c r="A9" s="59" t="s">
         <v>536</v>
       </c>
       <c r="B9" s="29" t="s">
         <v>533</v>
       </c>
-      <c r="C9" s="58" t="s">
+      <c r="C9" s="61" t="s">
         <v>534</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="57"/>
+      <c r="A10" s="60"/>
       <c r="B10" s="30" t="s">
         <v>535</v>
       </c>
-      <c r="C10" s="59"/>
+      <c r="C10" s="62"/>
     </row>
     <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="26" t="s">
@@ -7809,22 +8143,22 @@
       <c r="C19" s="35"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="48" t="s">
+      <c r="A20" s="51" t="s">
         <v>547</v>
       </c>
       <c r="B20" s="36" t="s">
         <v>548</v>
       </c>
-      <c r="C20" s="50" t="s">
+      <c r="C20" s="53" t="s">
         <v>534</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="49"/>
+      <c r="A21" s="52"/>
       <c r="B21" s="16" t="s">
         <v>549</v>
       </c>
-      <c r="C21" s="51"/>
+      <c r="C21" s="54"/>
     </row>
     <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="32"/>

</xml_diff>

<commit_message>
actualizacion de documentacion bosch
bosh  (ftp_digit_bosch) Definición de funciones contempladas en total 24  funciones , documentación de la funcionalidad,  pendiente agregar consultas generadas y relaciones ,
- Reunión con Ricardo explicación de  bosh
- Documentación  de spooler  (command vs función principal con numero de parámetros) , se llevan documentados 305
</commit_message>
<xml_diff>
--- a/00-Documentacion/Listado_Modulos2.xlsx
+++ b/00-Documentacion/Listado_Modulos2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\pc\raul\Net\migracion_spooler\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{948A81AE-9AA1-491F-8B54-6834EE202F7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40BE315D-69C1-43B3-BA73-7EF50C3A5F90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="859" activeTab="1" xr2:uid="{9A494972-654C-41EC-A971-3BEDBD7DDBA9}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="613">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="903" uniqueCount="671">
   <si>
     <t>Opción de Menú</t>
   </si>
@@ -1413,9 +1413,6 @@
   </si>
   <si>
     <t>reprograma_ejecucion_reporte</t>
-  </si>
-  <si>
-    <t>ftp_digit_tupperware</t>
   </si>
   <si>
     <t>rotacion_personal</t>
@@ -1885,6 +1882,183 @@
   </si>
   <si>
     <t>reunion con lulu verificacion  de estrutura de objetos de bD</t>
+  </si>
+  <si>
+    <t>generacion de expediente  aduanal bosch , se envia mediante ftp (consumo a de exe externo para timbrar), el cual en base al cliente se le asigna una nomeclatura archivos enviados</t>
+  </si>
+  <si>
+    <t>M:\Orfeo2\Bin\conv_xml_pdf2.exe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M:\Orfeo2\Bin\edocs_acuses_sat.exe </t>
+  </si>
+  <si>
+    <t>SQL_PED_1</t>
+  </si>
+  <si>
+    <t>myZip.Init</t>
+  </si>
+  <si>
+    <t>Recupera los posibles archivos PEDIMENTO a enviar, filtro por fecha</t>
+  </si>
+  <si>
+    <t>SQL_PED</t>
+  </si>
+  <si>
+    <t>Recupera los posibles archivos PEDIMENTO a enviar</t>
+  </si>
+  <si>
+    <t>SQL_CONTACTOS</t>
+  </si>
+  <si>
+    <t>genera informacion de correo en base al id_cron, según el proceso</t>
+  </si>
+  <si>
+    <t>send_mail</t>
+  </si>
+  <si>
+    <t>Proceso que recibe parametro origen, destino, archivos para enviar la informacion, envioa correo al area de sistemas</t>
+  </si>
+  <si>
+    <t>get_cli_ftp_server</t>
+  </si>
+  <si>
+    <t>toma la funcion de variables.bas</t>
+  </si>
+  <si>
+    <t>valida el tipo de informacion a enviar y relaciona los parametros con los clientes para el envio</t>
+  </si>
+  <si>
+    <t>conexion_ftp</t>
+  </si>
+  <si>
+    <t>valida el tipo de conexión va realiza ftp o sftp, y valida la conexión</t>
+  </si>
+  <si>
+    <t>Archivo_Validacion</t>
+  </si>
+  <si>
+    <t>recolecta los archvios por validar</t>
+  </si>
+  <si>
+    <t>valida tamaño del archivo del pedido</t>
+  </si>
+  <si>
+    <t>add_file_to_list</t>
+  </si>
+  <si>
+    <t>añade los archivos a enviar</t>
+  </si>
+  <si>
+    <t>selecciona los formatos que deberia enviarse de los documento emitidos por sat por clave de sat</t>
+  </si>
+  <si>
+    <t>todos archvios cove cfdi, facturas , etc</t>
+  </si>
+  <si>
+    <t>SQL_PED_DATOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">forma nombre del archivo pedimento .pdf en base rdf </t>
+  </si>
+  <si>
+    <t>SQL_ACUSE_SAT_COVE</t>
+  </si>
+  <si>
+    <t>documentos del sat  cfdi median el sgeclave(llave de documento del expediente)</t>
+  </si>
+  <si>
+    <t>SQL_ACUSE_SAT_EDOC</t>
+  </si>
+  <si>
+    <t>documentos del sat digitalizados  median el sgeclave(llave de documento del expediente)</t>
+  </si>
+  <si>
+    <t>SQL_NAME_FILE</t>
+  </si>
+  <si>
+    <t>Arma nombre del archivo</t>
+  </si>
+  <si>
+    <t>set_real_files</t>
+  </si>
+  <si>
+    <t>guarda los pendientes enviados para mandar un resumen de los archivos que se enviaron ZIP</t>
+  </si>
+  <si>
+    <t>save_files_1</t>
+  </si>
+  <si>
+    <t>guarda los pendientes enviados para mandar un resumen de los archivos que se enviaron</t>
+  </si>
+  <si>
+    <t>send_error_mail</t>
+  </si>
+  <si>
+    <t>etiquea de error para envio de correo</t>
+  </si>
+  <si>
+    <t>SQL_GET_FOLIO</t>
+  </si>
+  <si>
+    <t>Obtine el folio del pedimento</t>
+  </si>
+  <si>
+    <t>ftp_put_file</t>
+  </si>
+  <si>
+    <t>envio de archivos ftp</t>
+  </si>
+  <si>
+    <t>save_files</t>
+  </si>
+  <si>
+    <t>deconexion_ftp</t>
+  </si>
+  <si>
+    <t>desconecta la session</t>
+  </si>
+  <si>
+    <t>operaciones_aduanales</t>
+  </si>
+  <si>
+    <t>Bosch_Pedimentos3_xls</t>
+  </si>
+  <si>
+    <t>Ing_egr_gar_pend_fact</t>
+  </si>
+  <si>
+    <t>Fondo_fijo</t>
+  </si>
+  <si>
+    <t>funcion genera pdf</t>
+  </si>
+  <si>
+    <t>- bosh  (ftp_digit_bosch) Definición de funciones contempladas en total 24  funciones , documentación de la funcionalidad,  pendiente agregar consultas generadas ,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bosh  (ftp_digit_bosch) </t>
+  </si>
+  <si>
+    <t>Reunión con Ricardo explicación de  bosh </t>
+  </si>
+  <si>
+    <t>DOUMENTACION</t>
+  </si>
+  <si>
+    <t>scj_pedimentos_pagados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Documentación  de spooler  (command vs función principal con numero de parámetros) , se llevan documentados 305 </t>
+  </si>
+  <si>
+    <t>Generación aplicación  para validar la ejecución en servidor  “Hola mundo”  se cambió por “Main Spooler”</t>
+  </si>
+  <si>
+    <t>SPOOLER</t>
+  </si>
+  <si>
+    <t>reunion con lulu verificacion  de estrutura de objetos de Bd , se rediseño por el tamaño de los objeto, se envio el excel a lulu</t>
   </si>
 </sst>
 </file>
@@ -2630,8 +2804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2793532-E55B-4B24-AE52-361B14773BDB}">
   <dimension ref="A1:I317"/>
   <sheetViews>
-    <sheetView topLeftCell="A271" workbookViewId="0">
-      <selection activeCell="D288" sqref="D288"/>
+    <sheetView topLeftCell="A292" workbookViewId="0">
+      <selection activeCell="D316" sqref="D316"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5810,7 +5984,7 @@
         <v>214</v>
       </c>
       <c r="D214" s="1" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="E214" s="1">
         <v>5</v>
@@ -5953,7 +6127,7 @@
         <v>224</v>
       </c>
       <c r="D224" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="E224" s="1">
         <v>5</v>
@@ -5967,7 +6141,7 @@
         <v>225</v>
       </c>
       <c r="D225" s="1" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="E225" s="1">
         <v>4</v>
@@ -5981,7 +6155,7 @@
         <v>226</v>
       </c>
       <c r="D226" s="1" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="E226" s="1">
         <v>4</v>
@@ -5995,7 +6169,7 @@
         <v>227</v>
       </c>
       <c r="D227" s="1" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="E227" s="1">
         <v>6</v>
@@ -6135,7 +6309,7 @@
         <v>237</v>
       </c>
       <c r="D237" s="1" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="E237" s="1">
         <v>8</v>
@@ -6222,7 +6396,7 @@
         <v>243</v>
       </c>
       <c r="D243" s="1" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="E243" s="1">
         <v>6</v>
@@ -6236,7 +6410,7 @@
         <v>244</v>
       </c>
       <c r="D244" s="1" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="E244" s="1">
         <v>6</v>
@@ -6250,7 +6424,7 @@
         <v>245</v>
       </c>
       <c r="D245" s="1" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E245" s="1">
         <v>6</v>
@@ -6312,7 +6486,7 @@
         <v>249</v>
       </c>
       <c r="D249" s="1" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E249" s="1">
         <v>5</v>
@@ -6326,7 +6500,7 @@
         <v>250</v>
       </c>
       <c r="D250" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="E250" s="1">
         <v>7</v>
@@ -6337,7 +6511,7 @@
         <v>252</v>
       </c>
       <c r="D251" s="1" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="E251" s="1">
         <v>7</v>
@@ -6348,7 +6522,7 @@
         <v>253</v>
       </c>
       <c r="D252" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="E252" s="1">
         <v>6</v>
@@ -6362,7 +6536,7 @@
         <v>251</v>
       </c>
       <c r="D253" s="1" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="E253" s="1">
         <v>6</v>
@@ -6376,7 +6550,7 @@
         <v>252</v>
       </c>
       <c r="D254" s="1" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="E254" s="1">
         <v>5</v>
@@ -6404,7 +6578,7 @@
         <v>254</v>
       </c>
       <c r="D256" s="1" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="E256" s="1">
         <v>8</v>
@@ -6432,7 +6606,7 @@
         <v>256</v>
       </c>
       <c r="D258" s="1" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="E258" s="1">
         <v>5</v>
@@ -6446,7 +6620,7 @@
         <v>257</v>
       </c>
       <c r="D259" s="1" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="E259" s="1">
         <v>1</v>
@@ -6505,7 +6679,7 @@
         <v>261</v>
       </c>
       <c r="D263" s="1" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="E263" s="1">
         <v>7</v>
@@ -6519,7 +6693,7 @@
         <v>262</v>
       </c>
       <c r="D264" s="1" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="E264" s="1">
         <v>7</v>
@@ -6533,7 +6707,7 @@
         <v>263</v>
       </c>
       <c r="D265" s="1" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="E265" s="1">
         <v>7</v>
@@ -6561,7 +6735,7 @@
         <v>265</v>
       </c>
       <c r="D267" s="1" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="E267" s="1">
         <v>6</v>
@@ -6631,7 +6805,7 @@
         <v>270</v>
       </c>
       <c r="D272" s="1" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E272" s="1">
         <v>2</v>
@@ -6645,7 +6819,7 @@
         <v>271</v>
       </c>
       <c r="D273" s="1" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="E273" s="1">
         <v>6</v>
@@ -6715,7 +6889,7 @@
         <v>276</v>
       </c>
       <c r="D278" s="1" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="E278" s="1">
         <v>9</v>
@@ -6726,7 +6900,7 @@
         <v>280</v>
       </c>
       <c r="D279" s="1" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="E279" s="1">
         <v>7</v>
@@ -6740,7 +6914,7 @@
         <v>277</v>
       </c>
       <c r="D280" s="1" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="E280" s="1">
         <v>5</v>
@@ -6754,7 +6928,7 @@
         <v>278</v>
       </c>
       <c r="D281" s="1" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="E281" s="1">
         <v>5</v>
@@ -6796,7 +6970,7 @@
         <v>281</v>
       </c>
       <c r="D284" s="1" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="E284" s="1">
         <v>1</v>
@@ -6810,7 +6984,7 @@
         <v>282</v>
       </c>
       <c r="D285" s="1" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="E285" s="1">
         <v>4</v>
@@ -6834,6 +7008,12 @@
       <c r="C287" s="1" t="s">
         <v>283</v>
       </c>
+      <c r="D287" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="E287" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="288" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A288" s="2">
@@ -6842,48 +7022,84 @@
       <c r="C288" s="1" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="289" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D288" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="E288" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A289" s="2">
         <v>290</v>
       </c>
       <c r="C289" s="1" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="290" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D289" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="E289" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A290" s="2">
         <v>291</v>
       </c>
       <c r="C290" s="1" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="291" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D290" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="E290" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A291" s="2">
         <v>292</v>
       </c>
       <c r="C291" s="1" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="292" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D291" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="E291" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A292" s="2">
         <v>293</v>
       </c>
       <c r="C292" s="1" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="293" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D292" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="E292" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A293" s="2">
         <v>294</v>
       </c>
       <c r="C293" s="1" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="294" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D293" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="E293" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A294" s="2">
         <v>295</v>
       </c>
@@ -6893,85 +7109,145 @@
       <c r="C294" s="1" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="295" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D294" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="E294" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A295" s="2">
         <v>296</v>
       </c>
       <c r="C295" s="1" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="296" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D295" s="1" t="s">
+        <v>657</v>
+      </c>
+      <c r="E295" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A296" s="2">
         <v>297</v>
       </c>
       <c r="C296" s="1" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="297" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D296" s="1" t="s">
+        <v>658</v>
+      </c>
+      <c r="E296" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A297" s="2">
         <v>298</v>
       </c>
       <c r="C297" s="1" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="298" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D297" s="1" t="s">
+        <v>659</v>
+      </c>
+      <c r="E297" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A298" s="2">
         <v>299</v>
       </c>
       <c r="C298" s="1" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="299" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D298" s="1" t="s">
+        <v>660</v>
+      </c>
+      <c r="E298" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A299" s="2">
         <v>300</v>
       </c>
       <c r="C299" s="1" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="300" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D299" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="E299" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A300" s="2">
         <v>301</v>
       </c>
-      <c r="C300" s="1" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="301" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D300" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="E300" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A301" s="2">
         <v>302</v>
       </c>
       <c r="C301" s="1" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="302" spans="1:3" x14ac:dyDescent="0.25">
+        <v>296</v>
+      </c>
+      <c r="D301" s="1" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="302" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A302" s="2">
         <v>303</v>
       </c>
       <c r="C302" s="1" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="303" spans="1:3" x14ac:dyDescent="0.25">
+        <v>297</v>
+      </c>
+      <c r="D302" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="E302" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="303" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A303" s="2">
         <v>304</v>
       </c>
       <c r="C303" s="1" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="304" spans="1:3" x14ac:dyDescent="0.25">
+        <v>298</v>
+      </c>
+      <c r="D303" s="1" t="s">
+        <v>666</v>
+      </c>
+      <c r="E303" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="304" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A304" s="2">
         <v>305</v>
       </c>
       <c r="C304" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
+      </c>
+      <c r="D304" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="E304" s="1">
+        <v>7</v>
       </c>
     </row>
     <row r="305" spans="1:5" x14ac:dyDescent="0.25">
@@ -6979,63 +7255,53 @@
         <v>306</v>
       </c>
       <c r="C305" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="D305" s="1" t="s">
-        <v>457</v>
-      </c>
-      <c r="E305" s="1">
-        <v>3</v>
+        <v>300</v>
       </c>
     </row>
     <row r="306" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A306" s="2">
         <v>307</v>
       </c>
-      <c r="B306" s="1" t="s">
-        <v>326</v>
-      </c>
       <c r="C306" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="307" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A307" s="2">
         <v>308</v>
       </c>
+      <c r="B307" s="1" t="s">
+        <v>326</v>
+      </c>
       <c r="C307" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="308" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A308" s="2">
         <v>309</v>
       </c>
-      <c r="B308" s="5"/>
-      <c r="C308" s="5" t="s">
-        <v>304</v>
-      </c>
-      <c r="D308" s="5" t="s">
-        <v>304</v>
-      </c>
-      <c r="E308" s="5">
-        <v>5</v>
+      <c r="C308" s="1" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="309" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A309" s="2">
         <v>310</v>
       </c>
-      <c r="C309" s="1" t="s">
-        <v>305</v>
-      </c>
+      <c r="B309" s="5"/>
+      <c r="C309" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="D309" s="5"/>
+      <c r="E309" s="5"/>
     </row>
     <row r="310" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A310" s="2">
         <v>311</v>
       </c>
       <c r="C310" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="311" spans="1:5" x14ac:dyDescent="0.25">
@@ -7043,7 +7309,7 @@
         <v>312</v>
       </c>
       <c r="C311" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="312" spans="1:5" x14ac:dyDescent="0.25">
@@ -7051,7 +7317,7 @@
         <v>313</v>
       </c>
       <c r="C312" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="313" spans="1:5" x14ac:dyDescent="0.25">
@@ -7059,43 +7325,39 @@
         <v>314</v>
       </c>
       <c r="C313" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="314" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A314" s="2">
         <v>315</v>
       </c>
-      <c r="B314" s="5"/>
-      <c r="C314" s="5" t="s">
-        <v>310</v>
-      </c>
-      <c r="D314" s="5" t="s">
-        <v>310</v>
-      </c>
-      <c r="E314" s="5">
-        <v>7</v>
+      <c r="C314" s="1" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="315" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A315" s="2">
         <v>316</v>
       </c>
-      <c r="C315" s="1" t="s">
-        <v>311</v>
-      </c>
+      <c r="B315" s="5"/>
+      <c r="C315" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="D315" s="5"/>
+      <c r="E315" s="5"/>
     </row>
     <row r="316" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A316" s="2">
         <v>317</v>
       </c>
       <c r="C316" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="317" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A317" s="2">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C317" s="1" t="s">
         <v>312</v>
@@ -7109,10 +7371,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A24CCD5-B140-49E1-9D6E-67F75307E332}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7125,58 +7387,128 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B1" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="C1" t="s">
+        <v>606</v>
+      </c>
+      <c r="D1" t="s">
         <v>607</v>
-      </c>
-      <c r="D1" t="s">
-        <v>608</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="38">
-        <v>45411</v>
+        <v>45412</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>583</v>
-      </c>
-      <c r="D2" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+        <v>663</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="38">
-        <v>45411</v>
+        <v>45412</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>609</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>610</v>
+        <v>663</v>
+      </c>
+      <c r="D3" t="s">
+        <v>664</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="38">
-        <v>45411</v>
+        <v>45412</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4" t="s">
+        <v>665</v>
+      </c>
+      <c r="D4" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="38">
+        <v>45412</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>669</v>
+      </c>
+      <c r="D5" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="38">
+        <v>45412</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>610</v>
+      </c>
+      <c r="D6" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="38">
+        <v>45411</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>582</v>
+      </c>
+      <c r="D7" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A8" s="38">
+        <v>45411</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>608</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="38">
+        <v>45411</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>610</v>
+      </c>
+      <c r="D9" t="s">
         <v>611</v>
-      </c>
-      <c r="D4" t="s">
-        <v>612</v>
       </c>
     </row>
   </sheetData>
@@ -7333,10 +7665,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD54439F-40DB-4068-9758-9F0A5DA03583}">
-  <dimension ref="A1:O18"/>
+  <dimension ref="A1:O44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView topLeftCell="E20" workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7369,34 +7701,34 @@
         <v>0</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F1" s="8" t="s">
+        <v>458</v>
+      </c>
+      <c r="G1" s="8" t="s">
         <v>459</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>460</v>
       </c>
       <c r="H1" s="8" t="s">
         <v>406</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="M1" s="8" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="N1" t="s">
         <v>400</v>
@@ -7411,10 +7743,10 @@
         <v>304</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="F2" t="s">
         <v>304</v>
@@ -7432,10 +7764,10 @@
         <v>410</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="M2" s="37" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="N2" t="s">
         <v>401</v>
@@ -7449,23 +7781,23 @@
       <c r="B3" s="39"/>
       <c r="C3" s="39"/>
       <c r="D3" s="40" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="E3" s="41"/>
       <c r="F3" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="I3">
         <v>2</v>
       </c>
       <c r="J3" t="s">
+        <v>476</v>
+      </c>
+      <c r="K3" s="6" t="s">
         <v>477</v>
       </c>
-      <c r="K3" s="6" t="s">
-        <v>478</v>
-      </c>
       <c r="M3" s="37" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="N3" t="s">
         <v>402</v>
@@ -7476,27 +7808,27 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="F4" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="I4">
         <v>3</v>
       </c>
       <c r="J4" t="s">
+        <v>478</v>
+      </c>
+      <c r="K4" s="6" t="s">
         <v>479</v>
       </c>
-      <c r="K4" s="6" t="s">
-        <v>480</v>
-      </c>
       <c r="M4" s="37" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="F5" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="G5" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="H5">
         <v>1</v>
@@ -7505,13 +7837,13 @@
         <v>4</v>
       </c>
       <c r="K5" s="6" t="s">
+        <v>480</v>
+      </c>
+      <c r="L5" t="s">
         <v>481</v>
       </c>
-      <c r="L5" t="s">
-        <v>482</v>
-      </c>
       <c r="M5" s="37" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="O5" t="s">
         <v>405</v>
@@ -7519,21 +7851,21 @@
     </row>
     <row r="6" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="F6" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="I6">
         <v>5</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="M6" s="37" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="F7" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="H7">
         <v>1</v>
@@ -7542,32 +7874,32 @@
         <v>6</v>
       </c>
       <c r="K7" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="L7" t="s">
         <v>483</v>
       </c>
-      <c r="L7" t="s">
-        <v>484</v>
-      </c>
       <c r="M7" s="37" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="F8" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="I8">
         <v>7</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="M8" s="37" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="F9" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -7576,29 +7908,29 @@
         <v>7.1</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="M9" s="37" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="F10" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="I10">
         <v>8</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="M10" s="37" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="F11" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="H11">
         <v>1</v>
@@ -7607,35 +7939,35 @@
         <v>8.1</v>
       </c>
       <c r="K11" s="6" t="s">
+        <v>486</v>
+      </c>
+      <c r="L11" t="s">
         <v>487</v>
       </c>
-      <c r="L11" t="s">
-        <v>488</v>
-      </c>
       <c r="M11" s="37" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="F12" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="I12">
         <v>9</v>
       </c>
       <c r="J12" t="s">
+        <v>488</v>
+      </c>
+      <c r="K12" s="6" t="s">
         <v>489</v>
       </c>
-      <c r="K12" s="6" t="s">
-        <v>490</v>
-      </c>
       <c r="L12" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="F13" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H13">
         <v>1</v>
@@ -7644,23 +7976,23 @@
         <v>9.1</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="F14" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="I14">
         <v>10</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="F15" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="H15">
         <v>1</v>
@@ -7669,23 +8001,23 @@
         <v>10.1</v>
       </c>
       <c r="K15" s="6" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="F16" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="I16">
         <v>11</v>
       </c>
       <c r="K16" s="6" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="17" spans="6:11" x14ac:dyDescent="0.25">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F17" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="G17">
         <v>7</v>
@@ -7697,18 +8029,378 @@
         <v>11.1</v>
       </c>
       <c r="K17" s="6" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="18" spans="6:11" ht="30" x14ac:dyDescent="0.25">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="F18" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="I18">
         <v>12</v>
       </c>
       <c r="K18" s="6" t="s">
-        <v>589</v>
+        <v>588</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>316</v>
+      </c>
+      <c r="B19" s="9"/>
+      <c r="C19" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>612</v>
+      </c>
+      <c r="E19"/>
+      <c r="F19" t="s">
+        <v>310</v>
+      </c>
+      <c r="G19">
+        <v>78</v>
+      </c>
+      <c r="H19">
+        <v>4</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="J19" t="s">
+        <v>613</v>
+      </c>
+      <c r="K19" s="6"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D20"/>
+      <c r="E20"/>
+      <c r="F20" t="s">
+        <v>463</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <v>2</v>
+      </c>
+      <c r="J20" t="s">
+        <v>410</v>
+      </c>
+      <c r="K20" s="6" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D21"/>
+      <c r="E21"/>
+      <c r="F21" t="s">
+        <v>462</v>
+      </c>
+      <c r="I21">
+        <v>3</v>
+      </c>
+      <c r="J21" t="s">
+        <v>614</v>
+      </c>
+      <c r="K21" s="6" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="D22"/>
+      <c r="E22"/>
+      <c r="F22" t="s">
+        <v>615</v>
+      </c>
+      <c r="G22" t="s">
+        <v>552</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>4</v>
+      </c>
+      <c r="J22" t="s">
+        <v>616</v>
+      </c>
+      <c r="K22" s="6" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D23"/>
+      <c r="E23"/>
+      <c r="F23" t="s">
+        <v>618</v>
+      </c>
+      <c r="G23" t="s">
+        <v>552</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <v>5</v>
+      </c>
+      <c r="K23" s="6" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="D24"/>
+      <c r="E24"/>
+      <c r="F24" t="s">
+        <v>620</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="I24">
+        <v>6</v>
+      </c>
+      <c r="K24" s="6" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="D25"/>
+      <c r="E25"/>
+      <c r="F25" t="s">
+        <v>622</v>
+      </c>
+      <c r="I25">
+        <v>7</v>
+      </c>
+      <c r="J25" t="s">
+        <v>458</v>
+      </c>
+      <c r="K25" s="6" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="D26"/>
+      <c r="E26"/>
+      <c r="F26" t="s">
+        <v>624</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="I26">
+        <v>8</v>
+      </c>
+      <c r="J26" t="s">
+        <v>625</v>
+      </c>
+      <c r="K26" s="6" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="D27"/>
+      <c r="E27"/>
+      <c r="F27" t="s">
+        <v>627</v>
+      </c>
+      <c r="I27">
+        <v>9</v>
+      </c>
+      <c r="K27" s="6" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D28"/>
+      <c r="E28"/>
+      <c r="F28" t="s">
+        <v>629</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="I28">
+        <v>10</v>
+      </c>
+      <c r="K28" s="6" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D29"/>
+      <c r="E29"/>
+      <c r="F29" t="s">
+        <v>471</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
+      <c r="I29">
+        <v>10.1</v>
+      </c>
+      <c r="K29" s="6" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D30"/>
+      <c r="E30"/>
+      <c r="F30" t="s">
+        <v>632</v>
+      </c>
+      <c r="I30">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="K30" s="6" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="D31"/>
+      <c r="E31"/>
+      <c r="F31" t="s">
+        <v>475</v>
+      </c>
+      <c r="H31">
+        <v>53</v>
+      </c>
+      <c r="I31">
+        <v>11</v>
+      </c>
+      <c r="K31" s="6" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D32"/>
+      <c r="E32"/>
+      <c r="F32" t="s">
+        <v>469</v>
+      </c>
+      <c r="K32" s="6" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="33" spans="4:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="D33"/>
+      <c r="E33"/>
+      <c r="F33" t="s">
+        <v>465</v>
+      </c>
+      <c r="K33" s="6" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="34" spans="4:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="D34"/>
+      <c r="E34"/>
+      <c r="F34" t="s">
+        <v>636</v>
+      </c>
+      <c r="K34" s="6" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="35" spans="4:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="D35"/>
+      <c r="E35"/>
+      <c r="F35" t="s">
+        <v>638</v>
+      </c>
+      <c r="K35" s="6" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="36" spans="4:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="D36"/>
+      <c r="E36"/>
+      <c r="F36" t="s">
+        <v>640</v>
+      </c>
+      <c r="K36" s="6" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="37" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D37"/>
+      <c r="E37"/>
+      <c r="F37" t="s">
+        <v>642</v>
+      </c>
+      <c r="K37" s="6" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="38" spans="4:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="D38"/>
+      <c r="E38"/>
+      <c r="F38" t="s">
+        <v>644</v>
+      </c>
+      <c r="K38" s="6" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="39" spans="4:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="D39"/>
+      <c r="E39"/>
+      <c r="F39" t="s">
+        <v>646</v>
+      </c>
+      <c r="K39" s="6" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="40" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D40"/>
+      <c r="E40"/>
+      <c r="F40" t="s">
+        <v>648</v>
+      </c>
+      <c r="K40" s="6" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="41" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D41"/>
+      <c r="E41"/>
+      <c r="F41" t="s">
+        <v>650</v>
+      </c>
+      <c r="K41" s="6" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="42" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D42"/>
+      <c r="E42"/>
+      <c r="F42" t="s">
+        <v>652</v>
+      </c>
+      <c r="K42" s="6" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="43" spans="4:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="D43"/>
+      <c r="E43"/>
+      <c r="F43" t="s">
+        <v>654</v>
+      </c>
+      <c r="K43" s="6" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="44" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D44"/>
+      <c r="E44"/>
+      <c r="F44" t="s">
+        <v>655</v>
+      </c>
+      <c r="K44" s="6" t="s">
+        <v>656</v>
       </c>
     </row>
   </sheetData>
@@ -7734,31 +8426,31 @@
   <sheetData>
     <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="45" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B1" s="46"/>
       <c r="C1" s="47"/>
     </row>
     <row r="2" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
+        <v>499</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>500</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="C2" s="12" t="s">
         <v>501</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>502</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
+        <v>502</v>
+      </c>
+      <c r="B3" s="14" t="s">
         <v>503</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="C3" s="15" t="s">
         <v>504</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>505</v>
       </c>
       <c r="D3" s="7">
         <v>192</v>
@@ -7771,13 +8463,13 @@
     </row>
     <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
+        <v>505</v>
+      </c>
+      <c r="B5" s="16" t="s">
         <v>506</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="C5" s="17" t="s">
         <v>507</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>508</v>
       </c>
       <c r="D5" s="7">
         <v>175</v>
@@ -7790,13 +8482,13 @@
     </row>
     <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
+        <v>508</v>
+      </c>
+      <c r="B7" s="14" t="s">
         <v>509</v>
       </c>
-      <c r="B7" s="14" t="s">
-        <v>510</v>
-      </c>
       <c r="C7" s="17" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="D7" s="7">
         <v>207</v>
@@ -7809,13 +8501,13 @@
     </row>
     <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B9" s="16" t="s">
+        <v>506</v>
+      </c>
+      <c r="C9" s="17" t="s">
         <v>507</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>508</v>
       </c>
       <c r="D9" s="7">
         <v>216</v>
@@ -7828,13 +8520,13 @@
     </row>
     <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D11" s="7">
         <v>177</v>
@@ -7847,13 +8539,13 @@
     </row>
     <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="13" t="s">
+        <v>512</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>506</v>
+      </c>
+      <c r="C13" s="15" t="s">
         <v>513</v>
-      </c>
-      <c r="B13" s="16" t="s">
-        <v>507</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>514</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7863,13 +8555,13 @@
     </row>
     <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="21" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -7879,13 +8571,13 @@
     </row>
     <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="13" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -7895,13 +8587,13 @@
     </row>
     <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="13" t="s">
+        <v>516</v>
+      </c>
+      <c r="B19" s="16" t="s">
         <v>517</v>
       </c>
-      <c r="B19" s="16" t="s">
-        <v>518</v>
-      </c>
       <c r="C19" s="15" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -7911,13 +8603,13 @@
     </row>
     <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="13" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -7927,13 +8619,13 @@
     </row>
     <row r="23" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="13" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B23" s="14" t="s">
+        <v>506</v>
+      </c>
+      <c r="C23" s="17" t="s">
         <v>507</v>
-      </c>
-      <c r="C23" s="17" t="s">
-        <v>508</v>
       </c>
     </row>
   </sheetData>
@@ -7970,38 +8662,38 @@
   <sheetData>
     <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="45" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B1" s="46"/>
       <c r="C1" s="47"/>
     </row>
     <row r="2" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
+        <v>521</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>522</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>523</v>
-      </c>
       <c r="C2" s="12" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="22" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B3" s="23"/>
       <c r="C3" s="23"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="55" t="s">
+        <v>524</v>
+      </c>
+      <c r="B4" s="24" t="s">
         <v>525</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="C4" s="57" t="s">
         <v>526</v>
-      </c>
-      <c r="C4" s="57" t="s">
-        <v>527</v>
       </c>
       <c r="D4" s="7">
         <v>314</v>
@@ -8010,99 +8702,99 @@
     <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="56"/>
       <c r="B5" s="25" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C5" s="58"/>
     </row>
     <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="26" t="s">
+        <v>528</v>
+      </c>
+      <c r="B6" s="27" t="s">
         <v>529</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="C6" s="28" t="s">
         <v>530</v>
-      </c>
-      <c r="C6" s="28" t="s">
-        <v>531</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="59" t="s">
+        <v>531</v>
+      </c>
+      <c r="B7" s="29" t="s">
         <v>532</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="C7" s="61" t="s">
         <v>533</v>
-      </c>
-      <c r="C7" s="61" t="s">
-        <v>534</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="60"/>
       <c r="B8" s="30" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C8" s="62"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="59" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B9" s="29" t="s">
+        <v>532</v>
+      </c>
+      <c r="C9" s="61" t="s">
         <v>533</v>
-      </c>
-      <c r="C9" s="61" t="s">
-        <v>534</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="60"/>
       <c r="B10" s="30" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C10" s="62"/>
     </row>
     <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="26" t="s">
+        <v>536</v>
+      </c>
+      <c r="B11" s="30" t="s">
         <v>537</v>
       </c>
-      <c r="B11" s="30" t="s">
-        <v>538</v>
-      </c>
       <c r="C11" s="31" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="26" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B12" s="30" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="26" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B13" s="30" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="22" t="s">
+        <v>540</v>
+      </c>
+      <c r="B14" s="14" t="s">
         <v>541</v>
       </c>
-      <c r="B14" s="14" t="s">
-        <v>542</v>
-      </c>
       <c r="C14" s="23" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8112,13 +8804,13 @@
     </row>
     <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="22" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8128,13 +8820,13 @@
     </row>
     <row r="18" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="22" t="s">
+        <v>543</v>
+      </c>
+      <c r="B18" s="14" t="s">
         <v>544</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="C18" s="34" t="s">
         <v>545</v>
-      </c>
-      <c r="C18" s="34" t="s">
-        <v>546</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8144,19 +8836,19 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="51" t="s">
+        <v>546</v>
+      </c>
+      <c r="B20" s="36" t="s">
         <v>547</v>
       </c>
-      <c r="B20" s="36" t="s">
-        <v>548</v>
-      </c>
       <c r="C20" s="53" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="52"/>
       <c r="B21" s="16" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="C21" s="54"/>
     </row>
@@ -8167,13 +8859,13 @@
     </row>
     <row r="23" spans="1:4" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="22" t="s">
+        <v>549</v>
+      </c>
+      <c r="B23" s="16" t="s">
         <v>550</v>
       </c>
-      <c r="B23" s="16" t="s">
-        <v>551</v>
-      </c>
       <c r="C23" s="23" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="D23" s="7">
         <v>308</v>

</xml_diff>

<commit_message>
Ajuste aplicación de consola envió de parámetros línea de comando  “server_reports.exe command23”
</commit_message>
<xml_diff>
--- a/00-Documentacion/Listado_Modulos2.xlsx
+++ b/00-Documentacion/Listado_Modulos2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\pc\raul\Net\migracion_spooler\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40BE315D-69C1-43B3-BA73-7EF50C3A5F90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B52AA915-23F3-4F10-9F7F-BB40894EB478}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="859" activeTab="1" xr2:uid="{9A494972-654C-41EC-A971-3BEDBD7DDBA9}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="903" uniqueCount="671">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="966" uniqueCount="714">
   <si>
     <t>Opción de Menú</t>
   </si>
@@ -2059,6 +2059,135 @@
   </si>
   <si>
     <t>reunion con lulu verificacion  de estrutura de objetos de Bd , se rediseño por el tamaño de los objeto, se envio el excel a lulu</t>
+  </si>
+  <si>
+    <t>proceso que estan en forma secuencial (corre, sql), veificar casos de generacion de pdf y timbrados , evaluar si crean proceso independientes</t>
+  </si>
+  <si>
+    <t>Ftp,sftp,timbrado,zip, genera pdf,xml, envio de correo</t>
+  </si>
+  <si>
+    <t>conecta los objetos a base de datos</t>
+  </si>
+  <si>
+    <t>genera un archivos excel de todsa la facturas pendientes en que se quedan en el dia, genera 150 hojas excel</t>
+  </si>
+  <si>
+    <t>UBoundCheck</t>
+  </si>
+  <si>
+    <t>SQL_1</t>
+  </si>
+  <si>
+    <t>IsInArray_Multi</t>
+  </si>
+  <si>
+    <t>save_datas</t>
+  </si>
+  <si>
+    <t>SQL_2</t>
+  </si>
+  <si>
+    <t>SQL_3</t>
+  </si>
+  <si>
+    <t>SQL_4</t>
+  </si>
+  <si>
+    <t>SQL_5</t>
+  </si>
+  <si>
+    <t>SQL_6</t>
+  </si>
+  <si>
+    <t>SQL_7</t>
+  </si>
+  <si>
+    <t>SQL_8</t>
+  </si>
+  <si>
+    <t>write_resumen_ejecutiva</t>
+  </si>
+  <si>
+    <t>Formato a la hoja de resumen</t>
+  </si>
+  <si>
+    <t>write_resumen_clientes</t>
+  </si>
+  <si>
+    <t>Formato a las hojas en generar</t>
+  </si>
+  <si>
+    <t>mes_sp</t>
+  </si>
+  <si>
+    <t>busca el nombre del mes en base la fecha</t>
+  </si>
+  <si>
+    <t>formato de excel , formato expecial</t>
+  </si>
+  <si>
+    <t>recolecta las documentacion de nui (numero unico de idetificador) (por cada carga es un nui) , pendientes de facturar</t>
+  </si>
+  <si>
+    <t>busca el tab del archivopara empezar a validar (dentro de arreglo)</t>
+  </si>
+  <si>
+    <t>graba los registros generados de acuerdo la consulta principal</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> recolecta las documentacion de nui (numero unico de idetificador) (por cada carga es un nui) , pendientes de facturar ,En Traslado desde el cedis de Origen no recibido en destino</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> recolecta las documentacion de nui (numero unico de idetificador) (por cada carga es un nui) , pendientes de facturar , En cedis de destino sin nota de Carga Directa validada</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> recolecta las documentacion de nui (numero unico de idetificador) (por cada carga es un nui) , pendientes de facturar </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> recolecta las documentacion de nui (numero unico de idetificador) (por cada carga es un nui) , pendientes de facturar  , Entregado a cliente final sin recepcion de evidencia en oficina Cedis Origen</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> recolecta las documentacion de nui (numero unico de idetificador) (por cada carga es un nui) , pendientes de facturar , Con recepcion evidencia sin entrega al cliente </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> recolecta las documentacion de nui (numero unico de idetificador) (por cada carga es un nui) , pendientes de facturar , RECHAZADOS SIN ENTRADA CEDIS ORIGEN O TLN</t>
+  </si>
+  <si>
+    <t>QuickSort_num</t>
+  </si>
+  <si>
+    <t>zip, correo</t>
+  </si>
+  <si>
+    <t>contemplar las funcion de zip, envio de correo y formateo de correo, asi como el excel que esta formateado</t>
+  </si>
+  <si>
+    <t>FTPSegAutomotive</t>
+  </si>
+  <si>
+    <t>ftp_digit_tupperware</t>
+  </si>
+  <si>
+    <t>pedim_pdf_antolin_his</t>
+  </si>
+  <si>
+    <t>- bosh  (ftp_digit_bosch) Definición de funciones contempladas en total 24  funciones , documentación de la funcionalidad,  se agregar sql generadas y relaciones</t>
+  </si>
+  <si>
+    <t>- Documentación  de spooler  (command vs función principal con numero de parámetros) , se llevan documentados 318</t>
+  </si>
+  <si>
+    <t>-reunion con Ricardo verificar proceso</t>
+  </si>
+  <si>
+    <t>-fact_pend_cedis_ori - Definición de funciones contempladas en total 15  funciones , documentación de la funcionalidad,  se agregar sql generadas y relaciones</t>
+  </si>
+  <si>
+    <t>Facturas pendientes cedis ori</t>
+  </si>
+  <si>
+    <t>Ajuste aplicación de consola envio de parámetros línea de comando  “server_reports.exe command23”</t>
   </si>
 </sst>
 </file>
@@ -2804,8 +2933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2793532-E55B-4B24-AE52-361B14773BDB}">
   <dimension ref="A1:I317"/>
   <sheetViews>
-    <sheetView topLeftCell="A292" workbookViewId="0">
-      <selection activeCell="D316" sqref="D316"/>
+    <sheetView topLeftCell="A300" workbookViewId="0">
+      <selection activeCell="D308" sqref="D308"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5812,18 +5941,20 @@
       </c>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A202" s="2">
+      <c r="A202" s="7">
         <v>203</v>
       </c>
-      <c r="C202" s="1" t="s">
+      <c r="B202" s="5"/>
+      <c r="C202" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="D202" s="1" t="s">
+      <c r="D202" s="5" t="s">
         <v>452</v>
       </c>
-      <c r="E202" s="1">
+      <c r="E202" s="5">
         <v>6</v>
       </c>
+      <c r="F202" s="5"/>
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A203" s="2">
@@ -7257,6 +7388,12 @@
       <c r="C305" s="1" t="s">
         <v>300</v>
       </c>
+      <c r="D305" s="1" t="s">
+        <v>705</v>
+      </c>
+      <c r="E305" s="1">
+        <v>6</v>
+      </c>
     </row>
     <row r="306" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A306" s="2">
@@ -7265,6 +7402,12 @@
       <c r="C306" s="1" t="s">
         <v>301</v>
       </c>
+      <c r="D306" s="1" t="s">
+        <v>706</v>
+      </c>
+      <c r="E306" s="1">
+        <v>3</v>
+      </c>
     </row>
     <row r="307" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A307" s="2">
@@ -7276,6 +7419,12 @@
       <c r="C307" s="1" t="s">
         <v>302</v>
       </c>
+      <c r="D307" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="E307" s="1">
+        <v>7</v>
+      </c>
     </row>
     <row r="308" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A308" s="2">
@@ -7284,6 +7433,12 @@
       <c r="C308" s="1" t="s">
         <v>303</v>
       </c>
+      <c r="D308" s="1" t="s">
+        <v>707</v>
+      </c>
+      <c r="E308" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="309" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A309" s="2">
@@ -7293,8 +7448,12 @@
       <c r="C309" s="5" t="s">
         <v>304</v>
       </c>
-      <c r="D309" s="5"/>
-      <c r="E309" s="5"/>
+      <c r="D309" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="E309" s="5">
+        <v>5</v>
+      </c>
     </row>
     <row r="310" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A310" s="2">
@@ -7302,6 +7461,12 @@
       </c>
       <c r="C310" s="1" t="s">
         <v>305</v>
+      </c>
+      <c r="D310" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="E310" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="311" spans="1:5" x14ac:dyDescent="0.25">
@@ -7371,17 +7536,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A24CCD5-B140-49E1-9D6E-67F75307E332}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="50.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -7401,7 +7566,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="38">
-        <v>45412</v>
+        <v>45414</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -7410,106 +7575,185 @@
         <v>663</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>662</v>
+        <v>708</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="38">
-        <v>45412</v>
+        <v>45414</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>663</v>
-      </c>
-      <c r="D3" t="s">
-        <v>664</v>
+        <v>665</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>709</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="38">
-        <v>45412</v>
+        <v>45414</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>665</v>
-      </c>
-      <c r="D4" t="s">
-        <v>667</v>
+        <v>669</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>713</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="38">
-        <v>45412</v>
+        <v>45414</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>669</v>
-      </c>
-      <c r="D5" t="s">
-        <v>668</v>
+        <v>665</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>710</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="38">
-        <v>45412</v>
+        <v>45414</v>
       </c>
       <c r="B6">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>610</v>
-      </c>
-      <c r="D6" t="s">
-        <v>670</v>
+        <v>712</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>711</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="38">
-        <v>45411</v>
+        <v>45412</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>582</v>
-      </c>
-      <c r="D7" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+        <v>663</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="38">
-        <v>45411</v>
+        <v>45412</v>
       </c>
       <c r="B8">
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>608</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>609</v>
+        <v>663</v>
+      </c>
+      <c r="D8" t="s">
+        <v>664</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="38">
-        <v>45411</v>
+        <v>45412</v>
       </c>
       <c r="B9">
         <v>3</v>
       </c>
       <c r="C9" t="s">
+        <v>665</v>
+      </c>
+      <c r="D9" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="38">
+        <v>45412</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10" t="s">
+        <v>669</v>
+      </c>
+      <c r="D10" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="38">
+        <v>45412</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
         <v>610</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D11" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="38">
+        <v>45411</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>582</v>
+      </c>
+      <c r="D12" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A13" s="38">
+        <v>45411</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>608</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="38">
+        <v>45411</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14" t="s">
+        <v>610</v>
+      </c>
+      <c r="D14" t="s">
         <v>611</v>
       </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7665,10 +7909,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD54439F-40DB-4068-9758-9F0A5DA03583}">
-  <dimension ref="A1:O44"/>
+  <dimension ref="A1:O61"/>
   <sheetViews>
-    <sheetView topLeftCell="E20" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="5" ySplit="1" topLeftCell="F49" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="topRight" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7678,14 +7925,14 @@
     <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="50.7109375" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="3.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="59.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="47.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="50.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="40" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" customWidth="1"/>
+    <col min="11" max="11" width="68.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" customWidth="1"/>
+    <col min="13" max="13" width="18.5703125" customWidth="1"/>
     <col min="14" max="14" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -7823,7 +8070,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="F5" t="s">
         <v>464</v>
       </c>
@@ -8043,8 +8290,8 @@
         <v>588</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
+    <row r="19" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A19" s="7">
         <v>316</v>
       </c>
       <c r="B19" s="9"/>
@@ -8054,7 +8301,9 @@
       <c r="D19" s="10" t="s">
         <v>612</v>
       </c>
-      <c r="E19"/>
+      <c r="E19" s="10" t="s">
+        <v>672</v>
+      </c>
       <c r="F19" t="s">
         <v>310</v>
       </c>
@@ -8072,9 +8321,14 @@
       </c>
       <c r="K19" s="6"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D20"/>
-      <c r="E20"/>
+    <row r="20" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="39"/>
+      <c r="B20" s="39"/>
+      <c r="C20" s="39"/>
+      <c r="D20" s="40" t="s">
+        <v>671</v>
+      </c>
+      <c r="E20" s="41"/>
       <c r="F20" t="s">
         <v>463</v>
       </c>
@@ -8148,7 +8402,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D24"/>
       <c r="E24"/>
       <c r="F24" t="s">
@@ -8199,7 +8453,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D27"/>
       <c r="E27"/>
       <c r="F27" t="s">
@@ -8279,128 +8533,483 @@
       <c r="F32" t="s">
         <v>469</v>
       </c>
+      <c r="H32">
+        <v>1</v>
+      </c>
+      <c r="I32">
+        <v>12</v>
+      </c>
       <c r="K32" s="6" t="s">
         <v>635</v>
       </c>
     </row>
-    <row r="33" spans="4:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="D33"/>
       <c r="E33"/>
       <c r="F33" t="s">
         <v>465</v>
       </c>
+      <c r="I33">
+        <v>13</v>
+      </c>
       <c r="K33" s="6" t="s">
         <v>586</v>
       </c>
     </row>
-    <row r="34" spans="4:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="D34"/>
       <c r="E34"/>
       <c r="F34" t="s">
         <v>636</v>
       </c>
+      <c r="H34">
+        <v>1</v>
+      </c>
+      <c r="I34">
+        <v>14</v>
+      </c>
       <c r="K34" s="6" t="s">
         <v>637</v>
       </c>
     </row>
-    <row r="35" spans="4:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="D35"/>
       <c r="E35"/>
       <c r="F35" t="s">
         <v>638</v>
       </c>
+      <c r="H35">
+        <v>1</v>
+      </c>
+      <c r="I35">
+        <v>15</v>
+      </c>
       <c r="K35" s="6" t="s">
         <v>639</v>
       </c>
     </row>
-    <row r="36" spans="4:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="D36"/>
       <c r="E36"/>
       <c r="F36" t="s">
         <v>640</v>
       </c>
+      <c r="H36">
+        <v>1</v>
+      </c>
+      <c r="I36">
+        <v>16</v>
+      </c>
       <c r="K36" s="6" t="s">
         <v>641</v>
       </c>
     </row>
-    <row r="37" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D37"/>
       <c r="E37"/>
       <c r="F37" t="s">
         <v>642</v>
       </c>
+      <c r="H37">
+        <v>1</v>
+      </c>
+      <c r="I37">
+        <v>17</v>
+      </c>
       <c r="K37" s="6" t="s">
         <v>643</v>
       </c>
     </row>
-    <row r="38" spans="4:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="D38"/>
       <c r="E38"/>
       <c r="F38" t="s">
         <v>644</v>
       </c>
+      <c r="I38">
+        <v>18</v>
+      </c>
       <c r="K38" s="6" t="s">
         <v>645</v>
       </c>
     </row>
-    <row r="39" spans="4:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="D39"/>
       <c r="E39"/>
       <c r="F39" t="s">
         <v>646</v>
       </c>
+      <c r="H39">
+        <v>2</v>
+      </c>
+      <c r="I39">
+        <v>19</v>
+      </c>
       <c r="K39" s="6" t="s">
         <v>647</v>
       </c>
     </row>
-    <row r="40" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D40"/>
       <c r="E40"/>
       <c r="F40" t="s">
         <v>648</v>
       </c>
+      <c r="I40">
+        <v>20</v>
+      </c>
       <c r="K40" s="6" t="s">
         <v>649</v>
       </c>
     </row>
-    <row r="41" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D41"/>
       <c r="E41"/>
       <c r="F41" t="s">
         <v>650</v>
       </c>
+      <c r="H41">
+        <v>1</v>
+      </c>
+      <c r="I41">
+        <v>21</v>
+      </c>
       <c r="K41" s="6" t="s">
         <v>651</v>
       </c>
     </row>
-    <row r="42" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D42"/>
       <c r="E42"/>
       <c r="F42" t="s">
         <v>652</v>
       </c>
+      <c r="H42">
+        <v>4</v>
+      </c>
+      <c r="I42">
+        <v>22</v>
+      </c>
       <c r="K42" s="6" t="s">
         <v>653</v>
       </c>
     </row>
-    <row r="43" spans="4:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="D43"/>
       <c r="E43"/>
       <c r="F43" t="s">
         <v>654</v>
       </c>
+      <c r="H43">
+        <v>2</v>
+      </c>
+      <c r="I43">
+        <v>23</v>
+      </c>
       <c r="K43" s="6" t="s">
         <v>647</v>
       </c>
     </row>
-    <row r="44" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D44"/>
       <c r="E44"/>
       <c r="F44" t="s">
         <v>655</v>
       </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+      <c r="I44">
+        <v>24</v>
+      </c>
       <c r="K44" s="6" t="s">
         <v>656</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A45" s="7">
+        <v>203</v>
+      </c>
+      <c r="B45" s="9"/>
+      <c r="C45" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="D45" s="10" t="s">
+        <v>674</v>
+      </c>
+      <c r="E45" s="10" t="s">
+        <v>703</v>
+      </c>
+      <c r="F45" t="s">
+        <v>452</v>
+      </c>
+      <c r="G45">
+        <v>28</v>
+      </c>
+      <c r="H45">
+        <v>4</v>
+      </c>
+      <c r="L45" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A46" s="39"/>
+      <c r="B46" s="39"/>
+      <c r="C46" s="39"/>
+      <c r="D46" s="40" t="s">
+        <v>704</v>
+      </c>
+      <c r="E46" s="41"/>
+      <c r="F46" t="s">
+        <v>462</v>
+      </c>
+      <c r="I46">
+        <v>1</v>
+      </c>
+      <c r="K46" s="6" t="s">
+        <v>673</v>
+      </c>
+      <c r="L46" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D47"/>
+      <c r="E47"/>
+      <c r="F47" t="s">
+        <v>463</v>
+      </c>
+      <c r="H47">
+        <v>1</v>
+      </c>
+      <c r="I47">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="D48"/>
+      <c r="E48"/>
+      <c r="F48" t="s">
+        <v>676</v>
+      </c>
+      <c r="G48" t="s">
+        <v>552</v>
+      </c>
+      <c r="H48">
+        <v>5</v>
+      </c>
+      <c r="I48">
+        <v>3</v>
+      </c>
+      <c r="K48" s="6" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="49" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D49"/>
+      <c r="E49"/>
+      <c r="F49" t="s">
+        <v>677</v>
+      </c>
+      <c r="I49">
+        <v>4</v>
+      </c>
+      <c r="K49" s="6" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="50" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D50"/>
+      <c r="E50"/>
+      <c r="F50" t="s">
+        <v>678</v>
+      </c>
+      <c r="H50">
+        <v>1</v>
+      </c>
+      <c r="I50">
+        <v>5</v>
+      </c>
+      <c r="K50" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="51" spans="4:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="D51"/>
+      <c r="E51"/>
+      <c r="F51" t="s">
+        <v>679</v>
+      </c>
+      <c r="G51" t="s">
+        <v>552</v>
+      </c>
+      <c r="H51">
+        <v>2</v>
+      </c>
+      <c r="I51">
+        <v>6</v>
+      </c>
+      <c r="K51" s="6" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="52" spans="4:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="D52"/>
+      <c r="E52"/>
+      <c r="F52" t="s">
+        <v>680</v>
+      </c>
+      <c r="G52" t="s">
+        <v>552</v>
+      </c>
+      <c r="H52">
+        <v>3</v>
+      </c>
+      <c r="I52">
+        <v>7</v>
+      </c>
+      <c r="K52" s="6" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="53" spans="4:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="D53"/>
+      <c r="E53"/>
+      <c r="F53" t="s">
+        <v>681</v>
+      </c>
+      <c r="G53" t="s">
+        <v>552</v>
+      </c>
+      <c r="H53">
+        <v>3</v>
+      </c>
+      <c r="I53">
+        <v>8</v>
+      </c>
+      <c r="K53" s="6" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="54" spans="4:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="D54"/>
+      <c r="E54"/>
+      <c r="F54" t="s">
+        <v>682</v>
+      </c>
+      <c r="G54" t="s">
+        <v>552</v>
+      </c>
+      <c r="H54">
+        <v>2</v>
+      </c>
+      <c r="I54">
+        <v>9</v>
+      </c>
+      <c r="K54" s="6" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="55" spans="4:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="D55"/>
+      <c r="E55"/>
+      <c r="F55" t="s">
+        <v>683</v>
+      </c>
+      <c r="G55" t="s">
+        <v>552</v>
+      </c>
+      <c r="H55">
+        <v>2</v>
+      </c>
+      <c r="I55">
+        <v>10</v>
+      </c>
+      <c r="K55" s="6" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="56" spans="4:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="D56"/>
+      <c r="E56"/>
+      <c r="F56" t="s">
+        <v>684</v>
+      </c>
+      <c r="G56" t="s">
+        <v>552</v>
+      </c>
+      <c r="H56">
+        <v>2</v>
+      </c>
+      <c r="I56">
+        <v>11</v>
+      </c>
+      <c r="K56" s="6" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="57" spans="4:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="D57"/>
+      <c r="E57"/>
+      <c r="F57" t="s">
+        <v>685</v>
+      </c>
+      <c r="G57" t="s">
+        <v>552</v>
+      </c>
+      <c r="H57">
+        <v>4</v>
+      </c>
+      <c r="I57">
+        <v>12</v>
+      </c>
+      <c r="K57" s="6" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="58" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D58"/>
+      <c r="E58"/>
+      <c r="F58" t="s">
+        <v>686</v>
+      </c>
+      <c r="I58">
+        <v>13</v>
+      </c>
+      <c r="K58" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="59" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D59"/>
+      <c r="E59"/>
+      <c r="F59" t="s">
+        <v>688</v>
+      </c>
+      <c r="I59">
+        <v>14</v>
+      </c>
+      <c r="K59" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="60" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D60"/>
+      <c r="E60"/>
+      <c r="F60" t="s">
+        <v>690</v>
+      </c>
+      <c r="I60">
+        <v>15</v>
+      </c>
+      <c r="K60" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="61" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="F61" t="s">
+        <v>702</v>
       </c>
     </row>
   </sheetData>
@@ -8649,8 +9258,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F5D2F2F-F5F5-4926-AEB8-E0B5FA412C4C}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
-	Solicito agregar dos parámetros a la aplicación y cambiar nombre  aplicación  “serverreports.exe 121212 0”
Se versiono
</commit_message>
<xml_diff>
--- a/00-Documentacion/Listado_Modulos2.xlsx
+++ b/00-Documentacion/Listado_Modulos2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\pc\raul\Net\migracion_spooler\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B52AA915-23F3-4F10-9F7F-BB40894EB478}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{591077B2-B933-498E-9D86-E6C796A0ABAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="859" activeTab="1" xr2:uid="{9A494972-654C-41EC-A971-3BEDBD7DDBA9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="859" xr2:uid="{9A494972-654C-41EC-A971-3BEDBD7DDBA9}"/>
   </bookViews>
   <sheets>
     <sheet name="Opción de Menú vs Funcion param" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="966" uniqueCount="714">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1005" uniqueCount="733">
   <si>
     <t>Opción de Menú</t>
   </si>
@@ -2188,6 +2188,63 @@
   </si>
   <si>
     <t>Ajuste aplicación de consola envio de parámetros línea de comando  “server_reports.exe command23”</t>
+  </si>
+  <si>
+    <t>anex24_GKN_det</t>
+  </si>
+  <si>
+    <t>PUT_ENCABEZADO</t>
+  </si>
+  <si>
+    <t>crea en cabezados, formatos</t>
+  </si>
+  <si>
+    <t>SQL_LTL</t>
+  </si>
+  <si>
+    <t>GET_FACT_NUM</t>
+  </si>
+  <si>
+    <t>PUT_ENCABEZADO2</t>
+  </si>
+  <si>
+    <t>GET_LTL_TIEMPO_PRECIO</t>
+  </si>
+  <si>
+    <t>SAVE_FACT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Análisis del main de spooler  </t>
+  </si>
+  <si>
+    <t>reunión con Ricardo verificar proceso</t>
+  </si>
+  <si>
+    <t>Solicito agregar dos parámetros a la aplicación y cambiar nombre  aplicación  “serverreports.exe 121212 0” Se versiono</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Documentación  de spooler  (command vs función principal con numero de parámetros) , se llevan documentados 318 , se subió avances a github (migracion_spooler/00-Documentacion/ Listado_Modulos2.xlsx)</t>
+  </si>
+  <si>
+    <t>trading_cd_pendientes- Definición de funciones contempladas en total 15  funciones , documentación de la funcionalidad,  se agregar sql generadas y relaciones se subio avances a github (migracion_spooler/00-Documentacion/ Listado_Modulos2</t>
+  </si>
+  <si>
+    <t>menu principal</t>
+  </si>
+  <si>
+    <t>consulta pendientes de cd (crossdock y picking) -facturas, y los guardo en archivo de txt . Modalidad de carga</t>
+  </si>
+  <si>
+    <t>traer informacion de la cargas que esta pendientes de (crossdock y picking)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">busca factura </t>
+  </si>
+  <si>
+    <t>busca  monto concepto de la factura de distribucion</t>
+  </si>
+  <si>
+    <t>guardar los registros y consultas para posteriormente usarlas en reporte de fusion</t>
   </si>
 </sst>
 </file>
@@ -2933,8 +2990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2793532-E55B-4B24-AE52-361B14773BDB}">
   <dimension ref="A1:I317"/>
   <sheetViews>
-    <sheetView topLeftCell="A300" workbookViewId="0">
-      <selection activeCell="D308" sqref="D308"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7476,6 +7533,12 @@
       <c r="C311" s="1" t="s">
         <v>306</v>
       </c>
+      <c r="D311" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="E311" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="312" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A312" s="2">
@@ -7484,6 +7547,12 @@
       <c r="C312" s="1" t="s">
         <v>307</v>
       </c>
+      <c r="D312" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="E312" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="313" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A313" s="2">
@@ -7492,6 +7561,12 @@
       <c r="C313" s="1" t="s">
         <v>308</v>
       </c>
+      <c r="D313" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="E313" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="314" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A314" s="2">
@@ -7500,6 +7575,12 @@
       <c r="C314" s="1" t="s">
         <v>309</v>
       </c>
+      <c r="D314" s="1" t="s">
+        <v>714</v>
+      </c>
+      <c r="E314" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="315" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A315" s="2">
@@ -7509,8 +7590,12 @@
       <c r="C315" s="5" t="s">
         <v>310</v>
       </c>
-      <c r="D315" s="5"/>
-      <c r="E315" s="5"/>
+      <c r="D315" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="E315" s="5">
+        <v>7</v>
+      </c>
     </row>
     <row r="316" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A316" s="2">
@@ -7519,6 +7604,12 @@
       <c r="C316" s="1" t="s">
         <v>311</v>
       </c>
+      <c r="D316" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="E316" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="317" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A317" s="2">
@@ -7526,6 +7617,12 @@
       </c>
       <c r="C317" s="1" t="s">
         <v>312</v>
+      </c>
+      <c r="D317" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="E317" s="1">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -7536,10 +7633,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A24CCD5-B140-49E1-9D6E-67F75307E332}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection sqref="A1:D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7566,77 +7663,77 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="38">
-        <v>45414</v>
+        <v>45415</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>663</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>708</v>
+        <v>727</v>
+      </c>
+      <c r="D2" t="s">
+        <v>722</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="38">
-        <v>45414</v>
+        <v>45415</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>665</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>709</v>
+        <v>669</v>
+      </c>
+      <c r="D3" t="s">
+        <v>724</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="38">
-        <v>45414</v>
+        <v>45415</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>669</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>713</v>
+        <v>665</v>
+      </c>
+      <c r="D4" t="s">
+        <v>725</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="38">
-        <v>45414</v>
+        <v>45415</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>665</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>710</v>
+        <v>178</v>
+      </c>
+      <c r="D5" t="s">
+        <v>726</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="38">
-        <v>45414</v>
+        <v>45415</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>712</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>711</v>
+        <v>665</v>
+      </c>
+      <c r="D6" t="s">
+        <v>723</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="38">
-        <v>45412</v>
+        <v>45414</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -7645,115 +7742,185 @@
         <v>663</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>662</v>
+        <v>708</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="38">
-        <v>45412</v>
+        <v>45414</v>
       </c>
       <c r="B8">
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>663</v>
-      </c>
-      <c r="D8" t="s">
-        <v>664</v>
+        <v>665</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>709</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="38">
-        <v>45412</v>
+        <v>45414</v>
       </c>
       <c r="B9">
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>665</v>
-      </c>
-      <c r="D9" t="s">
-        <v>667</v>
+        <v>669</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>713</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="38">
-        <v>45412</v>
+        <v>45414</v>
       </c>
       <c r="B10">
         <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>669</v>
-      </c>
-      <c r="D10" t="s">
-        <v>668</v>
+        <v>665</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>710</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="38">
-        <v>45412</v>
+        <v>45414</v>
       </c>
       <c r="B11">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>610</v>
-      </c>
-      <c r="D11" t="s">
-        <v>670</v>
+        <v>712</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>711</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="38">
-        <v>45411</v>
+        <v>45412</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>582</v>
-      </c>
-      <c r="D12" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+        <v>663</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="38">
-        <v>45411</v>
+        <v>45412</v>
       </c>
       <c r="B13">
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>608</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>609</v>
+        <v>663</v>
+      </c>
+      <c r="D13" t="s">
+        <v>664</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="38">
-        <v>45411</v>
+        <v>45412</v>
       </c>
       <c r="B14">
         <v>3</v>
       </c>
       <c r="C14" t="s">
+        <v>665</v>
+      </c>
+      <c r="D14" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="38">
+        <v>45412</v>
+      </c>
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15" t="s">
+        <v>669</v>
+      </c>
+      <c r="D15" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="38">
+        <v>45412</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
         <v>610</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D16" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="38">
+        <v>45411</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>582</v>
+      </c>
+      <c r="D17" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A18" s="38">
+        <v>45411</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>608</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="38">
+        <v>45411</v>
+      </c>
+      <c r="B19">
+        <v>3</v>
+      </c>
+      <c r="C19" t="s">
+        <v>610</v>
+      </c>
+      <c r="D19" t="s">
         <v>611</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7909,13 +8076,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD54439F-40DB-4068-9758-9F0A5DA03583}">
-  <dimension ref="A1:O61"/>
+  <dimension ref="A1:O70"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F49" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F59" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G46" sqref="G46"/>
+      <selection pane="bottomRight" activeCell="G71" sqref="G71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8806,7 +8973,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="49" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D49"/>
       <c r="E49"/>
       <c r="F49" t="s">
@@ -8819,7 +8986,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="50" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D50"/>
       <c r="E50"/>
       <c r="F50" t="s">
@@ -8835,7 +9002,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="51" spans="4:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="D51"/>
       <c r="E51"/>
       <c r="F51" t="s">
@@ -8854,7 +9021,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="52" spans="4:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="D52"/>
       <c r="E52"/>
       <c r="F52" t="s">
@@ -8873,7 +9040,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="53" spans="4:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="D53"/>
       <c r="E53"/>
       <c r="F53" t="s">
@@ -8892,7 +9059,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="54" spans="4:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="D54"/>
       <c r="E54"/>
       <c r="F54" t="s">
@@ -8911,7 +9078,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="55" spans="4:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="D55"/>
       <c r="E55"/>
       <c r="F55" t="s">
@@ -8930,7 +9097,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="56" spans="4:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="D56"/>
       <c r="E56"/>
       <c r="F56" t="s">
@@ -8949,7 +9116,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="57" spans="4:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="D57"/>
       <c r="E57"/>
       <c r="F57" t="s">
@@ -8968,7 +9135,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="58" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D58"/>
       <c r="E58"/>
       <c r="F58" t="s">
@@ -8981,7 +9148,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="59" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D59"/>
       <c r="E59"/>
       <c r="F59" t="s">
@@ -8994,7 +9161,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="60" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D60"/>
       <c r="E60"/>
       <c r="F60" t="s">
@@ -9007,9 +9174,160 @@
         <v>691</v>
       </c>
     </row>
-    <row r="61" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F61" t="s">
         <v>702</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A62" s="7">
+        <v>178</v>
+      </c>
+      <c r="B62" s="9"/>
+      <c r="C62" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="D62" s="10" t="s">
+        <v>728</v>
+      </c>
+      <c r="E62" s="10" t="s">
+        <v>703</v>
+      </c>
+      <c r="F62" t="s">
+        <v>178</v>
+      </c>
+      <c r="H62">
+        <v>16</v>
+      </c>
+      <c r="I62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A63" s="39"/>
+      <c r="B63" s="39"/>
+      <c r="C63" s="39"/>
+      <c r="D63" s="40" t="s">
+        <v>704</v>
+      </c>
+      <c r="E63" s="41"/>
+      <c r="F63" t="s">
+        <v>462</v>
+      </c>
+      <c r="I63">
+        <v>2</v>
+      </c>
+      <c r="K63" s="6" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D64"/>
+      <c r="E64"/>
+      <c r="F64" t="s">
+        <v>463</v>
+      </c>
+      <c r="H64">
+        <v>1</v>
+      </c>
+      <c r="I64">
+        <v>3</v>
+      </c>
+      <c r="K64" s="6" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="65" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D65"/>
+      <c r="E65"/>
+      <c r="F65" t="s">
+        <v>715</v>
+      </c>
+      <c r="I65">
+        <v>4</v>
+      </c>
+      <c r="K65" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="66" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D66"/>
+      <c r="E66"/>
+      <c r="F66" t="s">
+        <v>717</v>
+      </c>
+      <c r="G66" t="s">
+        <v>552</v>
+      </c>
+      <c r="H66">
+        <v>26</v>
+      </c>
+      <c r="I66">
+        <v>5</v>
+      </c>
+      <c r="K66" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="67" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D67"/>
+      <c r="E67"/>
+      <c r="F67" t="s">
+        <v>718</v>
+      </c>
+      <c r="H67">
+        <v>8</v>
+      </c>
+      <c r="I67">
+        <v>6</v>
+      </c>
+      <c r="K67" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="68" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D68"/>
+      <c r="E68"/>
+      <c r="F68" t="s">
+        <v>719</v>
+      </c>
+      <c r="I68">
+        <v>7</v>
+      </c>
+      <c r="K68" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="69" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D69"/>
+      <c r="E69"/>
+      <c r="F69" t="s">
+        <v>720</v>
+      </c>
+      <c r="H69">
+        <v>22</v>
+      </c>
+      <c r="I69">
+        <v>8</v>
+      </c>
+      <c r="K69" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="70" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D70"/>
+      <c r="E70"/>
+      <c r="F70" t="s">
+        <v>721</v>
+      </c>
+      <c r="H70">
+        <v>3</v>
+      </c>
+      <c r="I70">
+        <v>9</v>
+      </c>
+      <c r="K70" t="s">
+        <v>732</v>
       </c>
     </row>
   </sheetData>
@@ -9022,7 +9340,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1C6E86F-3642-4535-8BC6-DAA60E82AA2C}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
@@ -9258,7 +9576,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F5D2F2F-F5F5-4926-AEB8-E0B5FA412C4C}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
se actualizo las actividades
</commit_message>
<xml_diff>
--- a/00-Documentacion/Listado_Modulos2.xlsx
+++ b/00-Documentacion/Listado_Modulos2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\pc\raul\Net\migracion_spooler\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{591077B2-B933-498E-9D86-E6C796A0ABAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFCBB24C-30EE-40CD-A7CF-9757188125B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="859" xr2:uid="{9A494972-654C-41EC-A971-3BEDBD7DDBA9}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1005" uniqueCount="733">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1038" uniqueCount="746">
   <si>
     <t>Opción de Menú</t>
   </si>
@@ -2245,6 +2245,45 @@
   </si>
   <si>
     <t>guardar los registros y consultas para posteriormente usarlas en reporte de fusion</t>
+  </si>
+  <si>
+    <t>Análisis main spooler se desgloso sql</t>
+  </si>
+  <si>
+    <t>Implementación sql de spooler principal</t>
+  </si>
+  <si>
+    <t>Documentación tradiding_ltl_pendientes</t>
+  </si>
+  <si>
+    <t>Reunión con Enrique revisión de objetos table Oracle</t>
+  </si>
+  <si>
+    <t>Revisión de funciones que envió Ricardo , se ejecutaron en consola del developer ,  en aplicación solo se ejecutaron las simple la anterior el resultado era 'ORA-00911: carácter no válido'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se están realizando las clases de las conexión y objeto tabla </t>
+  </si>
+  <si>
+    <t>Se explico a lulu las conexión , y los objetos que se debe utilizar, así como la clase que se deberían crear</t>
+  </si>
+  <si>
+    <t>consulta pendientes de ltl (cargas) -facturas, y los guardo en archivo de txt . Modolidad de carga</t>
+  </si>
+  <si>
+    <t>guardar los datos para el resumen</t>
+  </si>
+  <si>
+    <t>TestAndConnect</t>
+  </si>
+  <si>
+    <t>se ecnuentra en archivo de varibles, prueba de conexión</t>
+  </si>
+  <si>
+    <t>titulos de los reporte excel</t>
+  </si>
+  <si>
+    <t>extrae informacion del numero de factura y fecha</t>
   </si>
 </sst>
 </file>
@@ -2990,8 +3029,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2793532-E55B-4B24-AE52-361B14773BDB}">
   <dimension ref="A1:I317"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A297" workbookViewId="0">
+      <selection activeCell="G312" sqref="G312"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7633,10 +7672,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A24CCD5-B140-49E1-9D6E-67F75307E332}">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection sqref="A1:D19"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection sqref="A1:D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7663,21 +7702,21 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="38">
-        <v>45415</v>
+        <v>45418</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>727</v>
+        <v>669</v>
       </c>
       <c r="D2" t="s">
-        <v>722</v>
+        <v>733</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="38">
-        <v>45415</v>
+        <v>45418</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -7686,12 +7725,12 @@
         <v>669</v>
       </c>
       <c r="D3" t="s">
-        <v>724</v>
+        <v>734</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="38">
-        <v>45415</v>
+        <v>45418</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -7700,227 +7739,325 @@
         <v>665</v>
       </c>
       <c r="D4" t="s">
-        <v>725</v>
+        <v>735</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="38">
-        <v>45415</v>
+        <v>45418</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>178</v>
+        <v>669</v>
       </c>
       <c r="D5" t="s">
-        <v>726</v>
+        <v>736</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="38">
-        <v>45415</v>
+        <v>45418</v>
       </c>
       <c r="B6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
         <v>665</v>
       </c>
       <c r="D6" t="s">
-        <v>723</v>
+        <v>737</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="38">
-        <v>45414</v>
+        <v>45418</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>663</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>708</v>
+        <v>665</v>
+      </c>
+      <c r="D7" t="s">
+        <v>738</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="38">
-        <v>45414</v>
+        <v>45415</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>665</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>709</v>
+        <v>727</v>
+      </c>
+      <c r="D8" t="s">
+        <v>739</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="38">
-        <v>45414</v>
+        <v>45415</v>
       </c>
       <c r="B9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>669</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>713</v>
+        <v>727</v>
+      </c>
+      <c r="D9" t="s">
+        <v>722</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="38">
-        <v>45414</v>
+        <v>45415</v>
       </c>
       <c r="B10">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>665</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>710</v>
+        <v>669</v>
+      </c>
+      <c r="D10" t="s">
+        <v>724</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="38">
-        <v>45414</v>
+        <v>45415</v>
       </c>
       <c r="B11">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>712</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>711</v>
+        <v>665</v>
+      </c>
+      <c r="D11" t="s">
+        <v>725</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="38">
-        <v>45412</v>
+        <v>45415</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>663</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>662</v>
+        <v>178</v>
+      </c>
+      <c r="D12" t="s">
+        <v>726</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="38">
-        <v>45412</v>
+        <v>45415</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>663</v>
+        <v>665</v>
       </c>
       <c r="D13" t="s">
-        <v>664</v>
+        <v>723</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="38">
-        <v>45412</v>
+        <v>45414</v>
       </c>
       <c r="B14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>665</v>
-      </c>
-      <c r="D14" t="s">
-        <v>667</v>
+        <v>663</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>708</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="38">
-        <v>45412</v>
+        <v>45414</v>
       </c>
       <c r="B15">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>669</v>
-      </c>
-      <c r="D15" t="s">
-        <v>668</v>
+        <v>665</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>709</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="38">
-        <v>45412</v>
+        <v>45414</v>
       </c>
       <c r="B16">
         <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>610</v>
-      </c>
-      <c r="D16" t="s">
-        <v>670</v>
+        <v>669</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>713</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="38">
-        <v>45411</v>
+        <v>45414</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C17" t="s">
-        <v>582</v>
-      </c>
-      <c r="D17" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+        <v>665</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="38">
-        <v>45411</v>
+        <v>45414</v>
       </c>
       <c r="B18">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C18" t="s">
-        <v>608</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>609</v>
+        <v>712</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>711</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="38">
+        <v>45412</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>663</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="38">
+        <v>45412</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20" t="s">
+        <v>663</v>
+      </c>
+      <c r="D20" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="38">
+        <v>45412</v>
+      </c>
+      <c r="B21">
+        <v>3</v>
+      </c>
+      <c r="C21" t="s">
+        <v>665</v>
+      </c>
+      <c r="D21" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="38">
+        <v>45412</v>
+      </c>
+      <c r="B22">
+        <v>4</v>
+      </c>
+      <c r="C22" t="s">
+        <v>669</v>
+      </c>
+      <c r="D22" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="38">
+        <v>45412</v>
+      </c>
+      <c r="B23">
+        <v>3</v>
+      </c>
+      <c r="C23" t="s">
+        <v>610</v>
+      </c>
+      <c r="D23" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="38">
         <v>45411</v>
       </c>
-      <c r="B19">
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
+        <v>582</v>
+      </c>
+      <c r="D24" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A25" s="38">
+        <v>45411</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25" t="s">
+        <v>608</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="38">
+        <v>45411</v>
+      </c>
+      <c r="B26">
         <v>3</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C26" t="s">
         <v>610</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D26" t="s">
         <v>611</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="1"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="1"/>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8076,13 +8213,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD54439F-40DB-4068-9758-9F0A5DA03583}">
-  <dimension ref="A1:O70"/>
+  <dimension ref="A1:O79"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F59" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F65" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G71" sqref="G71"/>
+      <selection pane="bottomRight" activeCell="K77" sqref="K77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9196,6 +9333,9 @@
       <c r="F62" t="s">
         <v>178</v>
       </c>
+      <c r="G62">
+        <v>76</v>
+      </c>
       <c r="H62">
         <v>16</v>
       </c>
@@ -9237,7 +9377,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="65" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D65"/>
       <c r="E65"/>
       <c r="F65" t="s">
@@ -9250,7 +9390,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="66" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D66"/>
       <c r="E66"/>
       <c r="F66" t="s">
@@ -9269,7 +9409,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="67" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D67"/>
       <c r="E67"/>
       <c r="F67" t="s">
@@ -9285,7 +9425,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="68" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D68"/>
       <c r="E68"/>
       <c r="F68" t="s">
@@ -9298,7 +9438,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="69" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D69"/>
       <c r="E69"/>
       <c r="F69" t="s">
@@ -9314,7 +9454,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="70" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D70"/>
       <c r="E70"/>
       <c r="F70" t="s">
@@ -9328,6 +9468,149 @@
       </c>
       <c r="K70" t="s">
         <v>732</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A71" s="7">
+        <v>176</v>
+      </c>
+      <c r="B71" s="9"/>
+      <c r="C71" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="D71" s="10" t="s">
+        <v>740</v>
+      </c>
+      <c r="E71" s="10" t="s">
+        <v>478</v>
+      </c>
+      <c r="F71" t="s">
+        <v>176</v>
+      </c>
+      <c r="G71">
+        <v>61</v>
+      </c>
+      <c r="H71">
+        <v>17</v>
+      </c>
+      <c r="I71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D72"/>
+      <c r="E72"/>
+      <c r="F72" t="s">
+        <v>462</v>
+      </c>
+      <c r="I72">
+        <v>2</v>
+      </c>
+      <c r="K72" s="6" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D73"/>
+      <c r="E73"/>
+      <c r="F73" t="s">
+        <v>463</v>
+      </c>
+      <c r="H73">
+        <v>1</v>
+      </c>
+      <c r="I73">
+        <v>3</v>
+      </c>
+      <c r="K73" s="6" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D74"/>
+      <c r="E74"/>
+      <c r="F74" t="s">
+        <v>715</v>
+      </c>
+      <c r="I74">
+        <v>4</v>
+      </c>
+      <c r="K74" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D75"/>
+      <c r="E75"/>
+      <c r="F75" t="s">
+        <v>717</v>
+      </c>
+      <c r="G75" t="s">
+        <v>552</v>
+      </c>
+      <c r="H75">
+        <v>16</v>
+      </c>
+      <c r="I75">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D76"/>
+      <c r="E76"/>
+      <c r="F76" t="s">
+        <v>718</v>
+      </c>
+      <c r="H76">
+        <v>2</v>
+      </c>
+      <c r="I76">
+        <v>6</v>
+      </c>
+      <c r="K76" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D77"/>
+      <c r="E77"/>
+      <c r="F77" t="s">
+        <v>720</v>
+      </c>
+      <c r="H77">
+        <v>22</v>
+      </c>
+      <c r="I77">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D78"/>
+      <c r="E78"/>
+      <c r="F78" t="s">
+        <v>721</v>
+      </c>
+      <c r="H78">
+        <v>3</v>
+      </c>
+      <c r="I78">
+        <v>8</v>
+      </c>
+      <c r="K78" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D79"/>
+      <c r="E79"/>
+      <c r="F79" t="s">
+        <v>742</v>
+      </c>
+      <c r="I79">
+        <v>9</v>
+      </c>
+      <c r="K79" t="s">
+        <v>743</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se aplicaron cambios de conexion de conecBD
</commit_message>
<xml_diff>
--- a/00-Documentacion/Listado_Modulos2.xlsx
+++ b/00-Documentacion/Listado_Modulos2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\pc\raul\Net\migracion_spooler\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFCBB24C-30EE-40CD-A7CF-9757188125B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FAF0224-3D64-434F-A303-2B8AE21D0EB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="859" xr2:uid="{9A494972-654C-41EC-A971-3BEDBD7DDBA9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="859" activeTab="3" xr2:uid="{9A494972-654C-41EC-A971-3BEDBD7DDBA9}"/>
   </bookViews>
   <sheets>
     <sheet name="Opción de Menú vs Funcion param" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1038" uniqueCount="746">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1066" uniqueCount="759">
   <si>
     <t>Opción de Menú</t>
   </si>
@@ -2284,6 +2284,45 @@
   </si>
   <si>
     <t>extrae informacion del numero de factura y fecha</t>
+  </si>
+  <si>
+    <t>Implementación de configuración de conexión BD por json, aplicación</t>
+  </si>
+  <si>
+    <t>Generación de función de conexión , aplicación</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Documentación tradiding_fusion_pendientes </t>
+  </si>
+  <si>
+    <t>Documentación sql principales en main</t>
+  </si>
+  <si>
+    <t>Generación de proceso de llamada de  SQL en clase</t>
+  </si>
+  <si>
+    <t>Se genero la publicación de proyecto , se reviso el json de conexión y esta en DLL</t>
+  </si>
+  <si>
+    <t>Probar funciones con parámetros de salida  los cuales regresa error size must be set</t>
+  </si>
+  <si>
+    <t>fusion de ltl pendientes y cd pendientes, archivo exe , que se conformo de dos proceso</t>
+  </si>
+  <si>
+    <t>REPORTE_FUSION_WEB</t>
+  </si>
+  <si>
+    <t>REPORTE_FUSION_WEB.ACTUALIZACION</t>
+  </si>
+  <si>
+    <t>store</t>
+  </si>
+  <si>
+    <t>SQL_DETALLE</t>
+  </si>
+  <si>
+    <t>write_resumen</t>
   </si>
 </sst>
 </file>
@@ -3029,8 +3068,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2793532-E55B-4B24-AE52-361B14773BDB}">
   <dimension ref="A1:I317"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A297" workbookViewId="0">
-      <selection activeCell="G312" sqref="G312"/>
+    <sheetView topLeftCell="A213" workbookViewId="0">
+      <selection activeCell="E223" sqref="A223:E223"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7672,10 +7711,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A24CCD5-B140-49E1-9D6E-67F75307E332}">
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection sqref="A1:D26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7702,7 +7741,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="38">
-        <v>45418</v>
+        <v>45419</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -7711,12 +7750,12 @@
         <v>669</v>
       </c>
       <c r="D2" t="s">
-        <v>733</v>
+        <v>746</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="38">
-        <v>45418</v>
+        <v>45419</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -7725,12 +7764,12 @@
         <v>669</v>
       </c>
       <c r="D3" t="s">
-        <v>734</v>
+        <v>747</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="38">
-        <v>45418</v>
+        <v>45419</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -7739,82 +7778,82 @@
         <v>665</v>
       </c>
       <c r="D4" t="s">
-        <v>735</v>
+        <v>748</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="38">
-        <v>45418</v>
+        <v>45419</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
       <c r="D5" t="s">
-        <v>736</v>
+        <v>749</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="38">
-        <v>45418</v>
+        <v>45419</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>665</v>
+        <v>669</v>
       </c>
       <c r="D6" t="s">
-        <v>737</v>
+        <v>750</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="38">
-        <v>45418</v>
+        <v>45419</v>
       </c>
       <c r="B7">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>665</v>
+        <v>669</v>
       </c>
       <c r="D7" t="s">
-        <v>738</v>
+        <v>751</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="38">
-        <v>45415</v>
+        <v>45419</v>
       </c>
       <c r="B8">
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>727</v>
+        <v>665</v>
       </c>
       <c r="D8" t="s">
-        <v>739</v>
+        <v>752</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="38">
-        <v>45415</v>
+        <v>45418</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>727</v>
+        <v>669</v>
       </c>
       <c r="D9" t="s">
-        <v>722</v>
+        <v>733</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="38">
-        <v>45415</v>
+        <v>45418</v>
       </c>
       <c r="B10">
         <v>2</v>
@@ -7823,12 +7862,12 @@
         <v>669</v>
       </c>
       <c r="D10" t="s">
-        <v>724</v>
+        <v>734</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="38">
-        <v>45415</v>
+        <v>45418</v>
       </c>
       <c r="B11">
         <v>3</v>
@@ -7837,227 +7876,325 @@
         <v>665</v>
       </c>
       <c r="D11" t="s">
-        <v>725</v>
+        <v>735</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="38">
-        <v>45415</v>
+        <v>45418</v>
       </c>
       <c r="B12">
         <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>178</v>
+        <v>669</v>
       </c>
       <c r="D12" t="s">
-        <v>726</v>
+        <v>736</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="38">
-        <v>45415</v>
+        <v>45418</v>
       </c>
       <c r="B13">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C13" t="s">
         <v>665</v>
       </c>
       <c r="D13" t="s">
-        <v>723</v>
+        <v>737</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="38">
-        <v>45414</v>
+        <v>45418</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>663</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>708</v>
+        <v>665</v>
+      </c>
+      <c r="D14" t="s">
+        <v>738</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="38">
-        <v>45414</v>
+        <v>45415</v>
       </c>
       <c r="B15">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C15" t="s">
-        <v>665</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>709</v>
+        <v>727</v>
+      </c>
+      <c r="D15" t="s">
+        <v>739</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="38">
-        <v>45414</v>
+        <v>45415</v>
       </c>
       <c r="B16">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>669</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>713</v>
+        <v>727</v>
+      </c>
+      <c r="D16" t="s">
+        <v>722</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="38">
-        <v>45414</v>
+        <v>45415</v>
       </c>
       <c r="B17">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>665</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>710</v>
+        <v>669</v>
+      </c>
+      <c r="D17" t="s">
+        <v>724</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="38">
-        <v>45414</v>
+        <v>45415</v>
       </c>
       <c r="B18">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C18" t="s">
-        <v>712</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>711</v>
+        <v>665</v>
+      </c>
+      <c r="D18" t="s">
+        <v>725</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="38">
-        <v>45412</v>
+        <v>45415</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>663</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>662</v>
+        <v>178</v>
+      </c>
+      <c r="D19" t="s">
+        <v>726</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="38">
-        <v>45412</v>
+        <v>45415</v>
       </c>
       <c r="B20">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>663</v>
+        <v>665</v>
       </c>
       <c r="D20" t="s">
-        <v>664</v>
+        <v>723</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="38">
-        <v>45412</v>
+        <v>45414</v>
       </c>
       <c r="B21">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>665</v>
-      </c>
-      <c r="D21" t="s">
-        <v>667</v>
+        <v>663</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>708</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="38">
-        <v>45412</v>
+        <v>45414</v>
       </c>
       <c r="B22">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>669</v>
-      </c>
-      <c r="D22" t="s">
-        <v>668</v>
+        <v>665</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>709</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="38">
-        <v>45412</v>
+        <v>45414</v>
       </c>
       <c r="B23">
         <v>3</v>
       </c>
       <c r="C23" t="s">
-        <v>610</v>
-      </c>
-      <c r="D23" t="s">
-        <v>670</v>
+        <v>669</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>713</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="38">
-        <v>45411</v>
+        <v>45414</v>
       </c>
       <c r="B24">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C24" t="s">
-        <v>582</v>
-      </c>
-      <c r="D24" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+        <v>665</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="38">
-        <v>45411</v>
+        <v>45414</v>
       </c>
       <c r="B25">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C25" t="s">
-        <v>608</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>609</v>
+        <v>712</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>711</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="38">
+        <v>45412</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>663</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="38">
+        <v>45412</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27" t="s">
+        <v>663</v>
+      </c>
+      <c r="D27" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="38">
+        <v>45412</v>
+      </c>
+      <c r="B28">
+        <v>3</v>
+      </c>
+      <c r="C28" t="s">
+        <v>665</v>
+      </c>
+      <c r="D28" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="38">
+        <v>45412</v>
+      </c>
+      <c r="B29">
+        <v>4</v>
+      </c>
+      <c r="C29" t="s">
+        <v>669</v>
+      </c>
+      <c r="D29" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="38">
+        <v>45412</v>
+      </c>
+      <c r="B30">
+        <v>3</v>
+      </c>
+      <c r="C30" t="s">
+        <v>610</v>
+      </c>
+      <c r="D30" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="38">
         <v>45411</v>
       </c>
-      <c r="B26">
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31" t="s">
+        <v>582</v>
+      </c>
+      <c r="D31" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A32" s="38">
+        <v>45411</v>
+      </c>
+      <c r="B32">
+        <v>2</v>
+      </c>
+      <c r="C32" t="s">
+        <v>608</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="38">
+        <v>45411</v>
+      </c>
+      <c r="B33">
         <v>3</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C33" t="s">
         <v>610</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D33" t="s">
         <v>611</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="1"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="1"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8213,13 +8350,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD54439F-40DB-4068-9758-9F0A5DA03583}">
-  <dimension ref="A1:O79"/>
+  <dimension ref="A1:O86"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F65" activePane="bottomRight" state="frozenSplit"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="5" ySplit="1" topLeftCell="F71" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K77" sqref="K77"/>
+      <selection pane="bottomRight" activeCell="F86" sqref="F86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9611,6 +9748,117 @@
       </c>
       <c r="K79" t="s">
         <v>743</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A80" s="7">
+        <v>212</v>
+      </c>
+      <c r="B80" s="9"/>
+      <c r="C80" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="D80" s="10" t="s">
+        <v>753</v>
+      </c>
+      <c r="E80" s="10" t="s">
+        <v>478</v>
+      </c>
+      <c r="F80" t="s">
+        <v>212</v>
+      </c>
+      <c r="G80">
+        <v>13</v>
+      </c>
+      <c r="H80">
+        <v>5</v>
+      </c>
+      <c r="I80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D81"/>
+      <c r="E81"/>
+      <c r="F81" t="s">
+        <v>462</v>
+      </c>
+      <c r="I81">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D82"/>
+      <c r="E82"/>
+      <c r="F82" t="s">
+        <v>463</v>
+      </c>
+      <c r="H82">
+        <v>1</v>
+      </c>
+      <c r="I82">
+        <v>3</v>
+      </c>
+      <c r="K82" s="6" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="83" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D83"/>
+      <c r="E83"/>
+      <c r="F83" t="s">
+        <v>754</v>
+      </c>
+      <c r="H83">
+        <v>1</v>
+      </c>
+      <c r="I83">
+        <v>4</v>
+      </c>
+      <c r="K83" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="84" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D84"/>
+      <c r="E84"/>
+      <c r="F84" t="s">
+        <v>755</v>
+      </c>
+      <c r="I84">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="K84" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="85" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D85"/>
+      <c r="E85"/>
+      <c r="F85" t="s">
+        <v>757</v>
+      </c>
+      <c r="G85" t="s">
+        <v>552</v>
+      </c>
+      <c r="H85">
+        <v>1</v>
+      </c>
+      <c r="I85">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="86" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D86"/>
+      <c r="E86"/>
+      <c r="F86" t="s">
+        <v>758</v>
+      </c>
+      <c r="H86">
+        <v>5</v>
+      </c>
+      <c r="I86">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Estructura de actividades RGG 20240509
 procedimiento almacenado se genero la aplicación y se versiono en la ruta de doucmentaciones carpeta (C:\pc\raul\Net\migracion_spooler\00-Documentacion\db\bdoracle)

Aplicación se modificó la aplicación se unieron los los 3 sql  , se modificó la función principal de sql,
agregan para metro opcional. Para el llenado del 3er sql.

Se investigo la ejecucion función los cuales , se ajustaron envia error al llenar la tabla “System.Exception: 'Size must be set.'”

Se continuo con al documentación de control_digit3
</commit_message>
<xml_diff>
--- a/00-Documentacion/Listado_Modulos2.xlsx
+++ b/00-Documentacion/Listado_Modulos2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\pc\raul\Net\migracion_spooler\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FAF0224-3D64-434F-A303-2B8AE21D0EB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36341786-A8BB-46DD-9564-C87DEEEEDA42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="859" activeTab="3" xr2:uid="{9A494972-654C-41EC-A971-3BEDBD7DDBA9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="859" activeTab="1" xr2:uid="{9A494972-654C-41EC-A971-3BEDBD7DDBA9}"/>
   </bookViews>
   <sheets>
     <sheet name="Opción de Menú vs Funcion param" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1066" uniqueCount="759">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1087" uniqueCount="772">
   <si>
     <t>Opción de Menú</t>
   </si>
@@ -2324,12 +2324,63 @@
   <si>
     <t>write_resumen</t>
   </si>
+  <si>
+    <t>General un excel - con inf. BD</t>
+  </si>
+  <si>
+    <t>ftp_sucursal_cargar</t>
+  </si>
+  <si>
+    <t>valida las sucursales que contenga dicho proceso  de pertenece a unidad  ftp_sucursal.bas</t>
+  </si>
+  <si>
+    <t>SQL_INSERT</t>
+  </si>
+  <si>
+    <t>validar_evidencia</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>SQL_DIGIT</t>
+  </si>
+  <si>
+    <t>correo,ftp,xml, excel</t>
+  </si>
+  <si>
+    <t>correo,excel</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> procedimiento almacenado se genero la aplicación y se versiono en la ruta de doucmentaciones carpeta (C:\pc\raul\Net\migracion_spooler\00-Documentacion\db\bdoracle)</t>
+  </si>
+  <si>
+    <t>Aplicación se modificó la aplicación se unieron los los 3 sql  , se modificó la función principal de sql, agregan para metro opcional. Para el llenado del 3er sql.</t>
+  </si>
+  <si>
+    <t>Se investigo la ejecucion función los cuales , se ajustaron envia error al llenar la tabla “System.Exception: 'Size must be set.'”</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Se continuo con al documentación de </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>control_digit3</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2415,6 +2466,13 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -7711,10 +7769,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A24CCD5-B140-49E1-9D6E-67F75307E332}">
-  <dimension ref="A1:D46"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7741,7 +7799,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="38">
-        <v>45419</v>
+        <v>45421</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -7749,13 +7807,13 @@
       <c r="C2" t="s">
         <v>669</v>
       </c>
-      <c r="D2" t="s">
-        <v>746</v>
+      <c r="D2" s="1" t="s">
+        <v>768</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="38">
-        <v>45419</v>
+        <v>45421</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -7763,27 +7821,27 @@
       <c r="C3" t="s">
         <v>669</v>
       </c>
-      <c r="D3" t="s">
-        <v>747</v>
+      <c r="D3" s="1" t="s">
+        <v>769</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="38">
-        <v>45419</v>
+        <v>45421</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>665</v>
-      </c>
-      <c r="D4" t="s">
-        <v>748</v>
+        <v>669</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>770</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="38">
-        <v>45419</v>
+        <v>45421</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -7791,8 +7849,8 @@
       <c r="C5" t="s">
         <v>665</v>
       </c>
-      <c r="D5" t="s">
-        <v>749</v>
+      <c r="D5" s="1" t="s">
+        <v>771</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -7800,13 +7858,13 @@
         <v>45419</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C6" t="s">
         <v>669</v>
       </c>
       <c r="D6" t="s">
-        <v>750</v>
+        <v>746</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -7814,13 +7872,13 @@
         <v>45419</v>
       </c>
       <c r="B7">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C7" t="s">
         <v>669</v>
       </c>
       <c r="D7" t="s">
-        <v>751</v>
+        <v>747</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -7828,69 +7886,69 @@
         <v>45419</v>
       </c>
       <c r="B8">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C8" t="s">
         <v>665</v>
       </c>
       <c r="D8" t="s">
-        <v>752</v>
+        <v>748</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="38">
-        <v>45418</v>
+        <v>45419</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
       <c r="D9" t="s">
-        <v>733</v>
+        <v>749</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="38">
-        <v>45418</v>
+        <v>45419</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C10" t="s">
         <v>669</v>
       </c>
       <c r="D10" t="s">
-        <v>734</v>
+        <v>750</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="38">
-        <v>45418</v>
+        <v>45419</v>
       </c>
       <c r="B11">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>665</v>
+        <v>669</v>
       </c>
       <c r="D11" t="s">
-        <v>735</v>
+        <v>751</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="38">
-        <v>45418</v>
+        <v>45419</v>
       </c>
       <c r="B12">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
       <c r="D12" t="s">
-        <v>736</v>
+        <v>752</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -7898,13 +7956,13 @@
         <v>45418</v>
       </c>
       <c r="B13">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>665</v>
+        <v>669</v>
       </c>
       <c r="D13" t="s">
-        <v>737</v>
+        <v>733</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -7912,69 +7970,69 @@
         <v>45418</v>
       </c>
       <c r="B14">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>665</v>
+        <v>669</v>
       </c>
       <c r="D14" t="s">
-        <v>738</v>
+        <v>734</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="38">
-        <v>45415</v>
+        <v>45418</v>
       </c>
       <c r="B15">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>727</v>
+        <v>665</v>
       </c>
       <c r="D15" t="s">
-        <v>739</v>
+        <v>735</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="38">
-        <v>45415</v>
+        <v>45418</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>727</v>
+        <v>669</v>
       </c>
       <c r="D16" t="s">
-        <v>722</v>
+        <v>736</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="38">
-        <v>45415</v>
+        <v>45418</v>
       </c>
       <c r="B17">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
       <c r="D17" t="s">
-        <v>724</v>
+        <v>737</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="38">
-        <v>45415</v>
+        <v>45418</v>
       </c>
       <c r="B18">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C18" t="s">
         <v>665</v>
       </c>
       <c r="D18" t="s">
-        <v>725</v>
+        <v>738</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -7982,13 +8040,13 @@
         <v>45415</v>
       </c>
       <c r="B19">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C19" t="s">
-        <v>178</v>
+        <v>727</v>
       </c>
       <c r="D19" t="s">
-        <v>726</v>
+        <v>739</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -7996,69 +8054,69 @@
         <v>45415</v>
       </c>
       <c r="B20">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>665</v>
+        <v>727</v>
       </c>
       <c r="D20" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="38">
-        <v>45414</v>
+        <v>45415</v>
       </c>
       <c r="B21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>663</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>708</v>
+        <v>669</v>
+      </c>
+      <c r="D21" t="s">
+        <v>724</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="38">
-        <v>45414</v>
+        <v>45415</v>
       </c>
       <c r="B22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C22" t="s">
         <v>665</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>709</v>
+      <c r="D22" t="s">
+        <v>725</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="38">
-        <v>45414</v>
+        <v>45415</v>
       </c>
       <c r="B23">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C23" t="s">
-        <v>669</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>713</v>
+        <v>178</v>
+      </c>
+      <c r="D23" t="s">
+        <v>726</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="38">
-        <v>45414</v>
+        <v>45415</v>
       </c>
       <c r="B24">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C24" t="s">
         <v>665</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>710</v>
+      <c r="D24" t="s">
+        <v>723</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -8066,69 +8124,69 @@
         <v>45414</v>
       </c>
       <c r="B25">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>712</v>
+        <v>663</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>711</v>
+        <v>708</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="38">
-        <v>45412</v>
+        <v>45414</v>
       </c>
       <c r="B26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C26" t="s">
-        <v>663</v>
+        <v>665</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>662</v>
+        <v>709</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="38">
-        <v>45412</v>
+        <v>45414</v>
       </c>
       <c r="B27">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C27" t="s">
-        <v>663</v>
-      </c>
-      <c r="D27" t="s">
-        <v>664</v>
+        <v>669</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>713</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="38">
-        <v>45412</v>
+        <v>45414</v>
       </c>
       <c r="B28">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C28" t="s">
         <v>665</v>
       </c>
-      <c r="D28" t="s">
-        <v>667</v>
+      <c r="D28" s="1" t="s">
+        <v>710</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="38">
-        <v>45412</v>
+        <v>45414</v>
       </c>
       <c r="B29">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C29" t="s">
-        <v>669</v>
-      </c>
-      <c r="D29" t="s">
-        <v>668</v>
+        <v>712</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>711</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -8136,65 +8194,121 @@
         <v>45412</v>
       </c>
       <c r="B30">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>610</v>
-      </c>
-      <c r="D30" t="s">
-        <v>670</v>
+        <v>663</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>662</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="38">
-        <v>45411</v>
+        <v>45412</v>
       </c>
       <c r="B31">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C31" t="s">
-        <v>582</v>
+        <v>663</v>
       </c>
       <c r="D31" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="38">
-        <v>45411</v>
+        <v>45412</v>
       </c>
       <c r="B32">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C32" t="s">
-        <v>608</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>609</v>
+        <v>665</v>
+      </c>
+      <c r="D32" t="s">
+        <v>667</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="38">
+        <v>45412</v>
+      </c>
+      <c r="B33">
+        <v>4</v>
+      </c>
+      <c r="C33" t="s">
+        <v>669</v>
+      </c>
+      <c r="D33" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="38">
+        <v>45412</v>
+      </c>
+      <c r="B34">
+        <v>3</v>
+      </c>
+      <c r="C34" t="s">
+        <v>610</v>
+      </c>
+      <c r="D34" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="38">
         <v>45411</v>
       </c>
-      <c r="B33">
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35" t="s">
+        <v>582</v>
+      </c>
+      <c r="D35" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A36" s="38">
+        <v>45411</v>
+      </c>
+      <c r="B36">
+        <v>2</v>
+      </c>
+      <c r="C36" t="s">
+        <v>608</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="38">
+        <v>45411</v>
+      </c>
+      <c r="B37">
         <v>3</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C37" t="s">
         <v>610</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D37" t="s">
         <v>611</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="1"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="1"/>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8350,13 +8464,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD54439F-40DB-4068-9758-9F0A5DA03583}">
-  <dimension ref="A1:O86"/>
+  <dimension ref="A1:O93"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F71" activePane="bottomRight" state="frozenSplit"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="5" ySplit="1" topLeftCell="F77" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F86" sqref="F86"/>
+      <selection pane="bottomRight" activeCell="G87" sqref="G87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9619,7 +9733,7 @@
         <v>740</v>
       </c>
       <c r="E71" s="10" t="s">
-        <v>478</v>
+        <v>767</v>
       </c>
       <c r="F71" t="s">
         <v>176</v>
@@ -9636,7 +9750,6 @@
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D72"/>
-      <c r="E72"/>
       <c r="F72" t="s">
         <v>462</v>
       </c>
@@ -9762,7 +9875,7 @@
         <v>753</v>
       </c>
       <c r="E80" s="10" t="s">
-        <v>478</v>
+        <v>767</v>
       </c>
       <c r="F80" t="s">
         <v>212</v>
@@ -9777,7 +9890,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D81"/>
       <c r="E81"/>
       <c r="F81" t="s">
@@ -9787,7 +9900,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="82" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D82"/>
       <c r="E82"/>
       <c r="F82" t="s">
@@ -9803,7 +9916,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="83" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D83"/>
       <c r="E83"/>
       <c r="F83" t="s">
@@ -9819,7 +9932,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="84" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D84"/>
       <c r="E84"/>
       <c r="F84" t="s">
@@ -9832,7 +9945,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="85" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D85"/>
       <c r="E85"/>
       <c r="F85" t="s">
@@ -9848,7 +9961,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="86" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D86"/>
       <c r="E86"/>
       <c r="F86" t="s">
@@ -9859,6 +9972,114 @@
       </c>
       <c r="I86">
         <v>6</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A87" s="7">
+        <v>188</v>
+      </c>
+      <c r="B87" s="9"/>
+      <c r="C87" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="D87" s="10" t="s">
+        <v>759</v>
+      </c>
+      <c r="E87" s="10" t="s">
+        <v>766</v>
+      </c>
+      <c r="F87" t="s">
+        <v>188</v>
+      </c>
+      <c r="G87">
+        <v>12</v>
+      </c>
+      <c r="H87">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D88"/>
+      <c r="E88"/>
+      <c r="F88" t="s">
+        <v>462</v>
+      </c>
+      <c r="I88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D89"/>
+      <c r="E89"/>
+      <c r="F89" t="s">
+        <v>760</v>
+      </c>
+      <c r="H89">
+        <v>1</v>
+      </c>
+      <c r="I89">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K89" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D90"/>
+      <c r="E90"/>
+      <c r="F90" t="s">
+        <v>762</v>
+      </c>
+      <c r="H90">
+        <v>4</v>
+      </c>
+      <c r="I90">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D91"/>
+      <c r="E91"/>
+      <c r="F91" t="s">
+        <v>463</v>
+      </c>
+      <c r="H91">
+        <v>1</v>
+      </c>
+      <c r="I91">
+        <v>3</v>
+      </c>
+      <c r="K91" s="6" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D92"/>
+      <c r="E92"/>
+      <c r="F92" t="s">
+        <v>763</v>
+      </c>
+      <c r="H92">
+        <v>0</v>
+      </c>
+      <c r="I92">
+        <v>4</v>
+      </c>
+      <c r="K92" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D93"/>
+      <c r="E93"/>
+      <c r="F93" t="s">
+        <v>765</v>
+      </c>
+      <c r="H93">
+        <v>2</v>
+      </c>
+      <c r="I93">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1.	Sql de main – adaptar los joins en la consulta (pruebas con el sql original)(num_of_param)
i.	tomar con esta la consulta de datos del reportes, generar el recorrido por el numero de parámetros (pruebas con el sql original) ()
2.	Aplicación Spooler Agrega la opciones en menú principal , generar algoritmo de que reciba parámetros adicionales num_of_param y armar el sql de datos del reporte
3.	Documentación de los proceso : trading_lista_citas, porteos_tln, pedidos_tracking, gsk_pedimientos, ind_cal_bosch
4.	Se investigo la ejecucion función seguimos con el mismo  “System.Exception: 'Size must be set.'”
</commit_message>
<xml_diff>
--- a/00-Documentacion/Listado_Modulos2.xlsx
+++ b/00-Documentacion/Listado_Modulos2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\pc\raul\Net\migracion_spooler\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36341786-A8BB-46DD-9564-C87DEEEEDA42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AD458CD-8F6B-46E9-B15E-5F0CFCAE6F96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="859" activeTab="1" xr2:uid="{9A494972-654C-41EC-A971-3BEDBD7DDBA9}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1087" uniqueCount="772">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1133" uniqueCount="783">
   <si>
     <t>Opción de Menú</t>
   </si>
@@ -2374,6 +2374,71 @@
       </rPr>
       <t>control_digit3</t>
     </r>
+  </si>
+  <si>
+    <t>Sql de main – adaptar los joins en la consulta (pruebas con el sql original)(num_of_param)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                          tomar con esta la consulta de datos del reportes, generar el recorrido por el numero de parámetros (pruebas con el sql original) ()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aplicación Spooler Agrega la opciones en menú principal , generar algoritmo de que reciba parámetros adicionales num_of_param y armar el sql de datos del reporte                                                           </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Documentación de los proceso : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>trading_lista_citas, porteos_tln, pedidos_tracking,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>gsk_pedimientos, ind_cal_bosch</t>
+    </r>
+  </si>
+  <si>
+    <t>WS,correo, ftp</t>
+  </si>
+  <si>
+    <t>inicializa onjetos de sql y titulos de reportes</t>
+  </si>
+  <si>
+    <t>recuperacion de los TDCD con TN_cliente y con TN_interno</t>
+  </si>
+  <si>
+    <t>conecta los objetos a base de datos, y gnera itulos</t>
+  </si>
+  <si>
+    <t>genera la lista de contactos</t>
+  </si>
+  <si>
+    <t>fill_tab</t>
+  </si>
+  <si>
+    <t>genera formao en excel</t>
   </si>
 </sst>
 </file>
@@ -7769,10 +7834,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A24CCD5-B140-49E1-9D6E-67F75307E332}">
-  <dimension ref="A1:D50"/>
+  <dimension ref="A1:D54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7799,7 +7864,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="38">
-        <v>45421</v>
+        <v>45422</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -7808,12 +7873,12 @@
         <v>669</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>768</v>
+        <v>772</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="38">
-        <v>45421</v>
+        <v>45422</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -7822,12 +7887,12 @@
         <v>669</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>769</v>
+        <v>773</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="38">
-        <v>45421</v>
+        <v>45422</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -7836,12 +7901,12 @@
         <v>669</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>770</v>
+        <v>774</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="38">
-        <v>45421</v>
+        <v>45422</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -7850,12 +7915,12 @@
         <v>665</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>771</v>
+        <v>775</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="38">
-        <v>45419</v>
+        <v>45421</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -7863,13 +7928,13 @@
       <c r="C6" t="s">
         <v>669</v>
       </c>
-      <c r="D6" t="s">
-        <v>746</v>
+      <c r="D6" s="1" t="s">
+        <v>768</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="38">
-        <v>45419</v>
+        <v>45421</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -7877,27 +7942,27 @@
       <c r="C7" t="s">
         <v>669</v>
       </c>
-      <c r="D7" t="s">
-        <v>747</v>
+      <c r="D7" s="1" t="s">
+        <v>769</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="38">
-        <v>45419</v>
+        <v>45421</v>
       </c>
       <c r="B8">
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>665</v>
-      </c>
-      <c r="D8" t="s">
-        <v>748</v>
+        <v>669</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>770</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="38">
-        <v>45419</v>
+        <v>45421</v>
       </c>
       <c r="B9">
         <v>4</v>
@@ -7905,8 +7970,8 @@
       <c r="C9" t="s">
         <v>665</v>
       </c>
-      <c r="D9" t="s">
-        <v>749</v>
+      <c r="D9" s="1" t="s">
+        <v>771</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -7914,13 +7979,13 @@
         <v>45419</v>
       </c>
       <c r="B10">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C10" t="s">
         <v>669</v>
       </c>
       <c r="D10" t="s">
-        <v>750</v>
+        <v>746</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -7928,13 +7993,13 @@
         <v>45419</v>
       </c>
       <c r="B11">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C11" t="s">
         <v>669</v>
       </c>
       <c r="D11" t="s">
-        <v>751</v>
+        <v>747</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -7942,69 +8007,69 @@
         <v>45419</v>
       </c>
       <c r="B12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C12" t="s">
         <v>665</v>
       </c>
       <c r="D12" t="s">
-        <v>752</v>
+        <v>748</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="38">
-        <v>45418</v>
+        <v>45419</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C13" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
       <c r="D13" t="s">
-        <v>733</v>
+        <v>749</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="38">
-        <v>45418</v>
+        <v>45419</v>
       </c>
       <c r="B14">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C14" t="s">
         <v>669</v>
       </c>
       <c r="D14" t="s">
-        <v>734</v>
+        <v>750</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="38">
-        <v>45418</v>
+        <v>45419</v>
       </c>
       <c r="B15">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>665</v>
+        <v>669</v>
       </c>
       <c r="D15" t="s">
-        <v>735</v>
+        <v>751</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="38">
-        <v>45418</v>
+        <v>45419</v>
       </c>
       <c r="B16">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C16" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
       <c r="D16" t="s">
-        <v>736</v>
+        <v>752</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -8012,13 +8077,13 @@
         <v>45418</v>
       </c>
       <c r="B17">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>665</v>
+        <v>669</v>
       </c>
       <c r="D17" t="s">
-        <v>737</v>
+        <v>733</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -8026,69 +8091,69 @@
         <v>45418</v>
       </c>
       <c r="B18">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>665</v>
+        <v>669</v>
       </c>
       <c r="D18" t="s">
-        <v>738</v>
+        <v>734</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="38">
-        <v>45415</v>
+        <v>45418</v>
       </c>
       <c r="B19">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C19" t="s">
-        <v>727</v>
+        <v>665</v>
       </c>
       <c r="D19" t="s">
-        <v>739</v>
+        <v>735</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="38">
-        <v>45415</v>
+        <v>45418</v>
       </c>
       <c r="B20">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C20" t="s">
-        <v>727</v>
+        <v>669</v>
       </c>
       <c r="D20" t="s">
-        <v>722</v>
+        <v>736</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="38">
-        <v>45415</v>
+        <v>45418</v>
       </c>
       <c r="B21">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
       <c r="D21" t="s">
-        <v>724</v>
+        <v>737</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="38">
-        <v>45415</v>
+        <v>45418</v>
       </c>
       <c r="B22">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C22" t="s">
         <v>665</v>
       </c>
       <c r="D22" t="s">
-        <v>725</v>
+        <v>738</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -8096,13 +8161,13 @@
         <v>45415</v>
       </c>
       <c r="B23">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C23" t="s">
-        <v>178</v>
+        <v>727</v>
       </c>
       <c r="D23" t="s">
-        <v>726</v>
+        <v>739</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -8110,69 +8175,69 @@
         <v>45415</v>
       </c>
       <c r="B24">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>665</v>
+        <v>727</v>
       </c>
       <c r="D24" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="38">
-        <v>45414</v>
+        <v>45415</v>
       </c>
       <c r="B25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C25" t="s">
-        <v>663</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>708</v>
+        <v>669</v>
+      </c>
+      <c r="D25" t="s">
+        <v>724</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="38">
-        <v>45414</v>
+        <v>45415</v>
       </c>
       <c r="B26">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C26" t="s">
         <v>665</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>709</v>
+      <c r="D26" t="s">
+        <v>725</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="38">
-        <v>45414</v>
+        <v>45415</v>
       </c>
       <c r="B27">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C27" t="s">
-        <v>669</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>713</v>
+        <v>178</v>
+      </c>
+      <c r="D27" t="s">
+        <v>726</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="38">
-        <v>45414</v>
+        <v>45415</v>
       </c>
       <c r="B28">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C28" t="s">
         <v>665</v>
       </c>
-      <c r="D28" s="1" t="s">
-        <v>710</v>
+      <c r="D28" t="s">
+        <v>723</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -8180,69 +8245,69 @@
         <v>45414</v>
       </c>
       <c r="B29">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>712</v>
+        <v>663</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>711</v>
+        <v>708</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="38">
-        <v>45412</v>
+        <v>45414</v>
       </c>
       <c r="B30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C30" t="s">
-        <v>663</v>
+        <v>665</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>662</v>
+        <v>709</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="38">
-        <v>45412</v>
+        <v>45414</v>
       </c>
       <c r="B31">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C31" t="s">
-        <v>663</v>
-      </c>
-      <c r="D31" t="s">
-        <v>664</v>
+        <v>669</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>713</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="38">
-        <v>45412</v>
+        <v>45414</v>
       </c>
       <c r="B32">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C32" t="s">
         <v>665</v>
       </c>
-      <c r="D32" t="s">
-        <v>667</v>
+      <c r="D32" s="1" t="s">
+        <v>710</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="38">
-        <v>45412</v>
+        <v>45414</v>
       </c>
       <c r="B33">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C33" t="s">
-        <v>669</v>
-      </c>
-      <c r="D33" t="s">
-        <v>668</v>
+        <v>712</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>711</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -8250,65 +8315,121 @@
         <v>45412</v>
       </c>
       <c r="B34">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>610</v>
-      </c>
-      <c r="D34" t="s">
-        <v>670</v>
+        <v>663</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>662</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="38">
-        <v>45411</v>
+        <v>45412</v>
       </c>
       <c r="B35">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C35" t="s">
-        <v>582</v>
+        <v>663</v>
       </c>
       <c r="D35" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="38">
-        <v>45411</v>
+        <v>45412</v>
       </c>
       <c r="B36">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C36" t="s">
-        <v>608</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>609</v>
+        <v>665</v>
+      </c>
+      <c r="D36" t="s">
+        <v>667</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="38">
+        <v>45412</v>
+      </c>
+      <c r="B37">
+        <v>4</v>
+      </c>
+      <c r="C37" t="s">
+        <v>669</v>
+      </c>
+      <c r="D37" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="38">
+        <v>45412</v>
+      </c>
+      <c r="B38">
+        <v>3</v>
+      </c>
+      <c r="C38" t="s">
+        <v>610</v>
+      </c>
+      <c r="D38" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="38">
         <v>45411</v>
       </c>
-      <c r="B37">
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39" t="s">
+        <v>582</v>
+      </c>
+      <c r="D39" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A40" s="38">
+        <v>45411</v>
+      </c>
+      <c r="B40">
+        <v>2</v>
+      </c>
+      <c r="C40" t="s">
+        <v>608</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="38">
+        <v>45411</v>
+      </c>
+      <c r="B41">
         <v>3</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C41" t="s">
         <v>610</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D41" t="s">
         <v>611</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="1"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="1"/>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="1"/>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8464,13 +8585,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD54439F-40DB-4068-9758-9F0A5DA03583}">
-  <dimension ref="A1:O93"/>
+  <dimension ref="A1:O109"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F77" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F92" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G87" sqref="G87"/>
+      <selection pane="bottomRight" activeCell="D108" sqref="D108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10082,6 +10203,238 @@
         <v>5</v>
       </c>
     </row>
+    <row r="94" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A94" s="7">
+        <v>95</v>
+      </c>
+      <c r="B94" s="5"/>
+      <c r="C94" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D94" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="E94" s="10" t="s">
+        <v>776</v>
+      </c>
+      <c r="F94" t="s">
+        <v>94</v>
+      </c>
+      <c r="G94">
+        <v>5</v>
+      </c>
+      <c r="I94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D95"/>
+      <c r="E95"/>
+      <c r="F95" t="s">
+        <v>462</v>
+      </c>
+      <c r="I95">
+        <v>2</v>
+      </c>
+      <c r="K95" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D96"/>
+      <c r="E96"/>
+      <c r="F96" t="s">
+        <v>757</v>
+      </c>
+      <c r="G96" t="s">
+        <v>552</v>
+      </c>
+      <c r="H96">
+        <v>5</v>
+      </c>
+      <c r="I96">
+        <v>3</v>
+      </c>
+      <c r="K96" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A97" s="7">
+        <v>265</v>
+      </c>
+      <c r="B97" s="5"/>
+      <c r="C97" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="D97" s="5"/>
+      <c r="E97" s="10" t="s">
+        <v>767</v>
+      </c>
+      <c r="F97" t="s">
+        <v>594</v>
+      </c>
+      <c r="G97">
+        <v>1</v>
+      </c>
+      <c r="H97">
+        <v>1</v>
+      </c>
+      <c r="I97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D98"/>
+      <c r="E98"/>
+      <c r="F98" t="s">
+        <v>462</v>
+      </c>
+      <c r="I98">
+        <v>2</v>
+      </c>
+      <c r="K98" s="6" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A99" s="7">
+        <v>105</v>
+      </c>
+      <c r="B99" s="5"/>
+      <c r="C99" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D99" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="E99" s="10" t="s">
+        <v>767</v>
+      </c>
+      <c r="F99" t="s">
+        <v>104</v>
+      </c>
+      <c r="G99">
+        <v>4</v>
+      </c>
+      <c r="H99">
+        <v>3</v>
+      </c>
+      <c r="I99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D100"/>
+      <c r="E100"/>
+      <c r="F100" t="s">
+        <v>462</v>
+      </c>
+      <c r="I100">
+        <v>2</v>
+      </c>
+      <c r="K100" s="6" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D101"/>
+      <c r="E101"/>
+      <c r="F101" t="s">
+        <v>620</v>
+      </c>
+      <c r="H101">
+        <v>1</v>
+      </c>
+      <c r="I101">
+        <v>3</v>
+      </c>
+      <c r="K101" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A102" s="7">
+        <v>264</v>
+      </c>
+      <c r="B102" s="5"/>
+      <c r="C102" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="D102" s="5" t="s">
+        <v>593</v>
+      </c>
+      <c r="E102" s="10" t="s">
+        <v>767</v>
+      </c>
+      <c r="F102" t="s">
+        <v>593</v>
+      </c>
+      <c r="H102">
+        <v>2</v>
+      </c>
+      <c r="I102">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D103"/>
+      <c r="E103"/>
+      <c r="F103" t="s">
+        <v>462</v>
+      </c>
+      <c r="I103">
+        <v>3</v>
+      </c>
+      <c r="K103" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A104" s="7">
+        <v>138</v>
+      </c>
+      <c r="B104" s="5"/>
+      <c r="C104" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="D104" s="5" t="s">
+        <v>389</v>
+      </c>
+      <c r="E104" s="10" t="s">
+        <v>767</v>
+      </c>
+      <c r="F104" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F107" t="s">
+        <v>462</v>
+      </c>
+      <c r="K107" s="6" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F108" t="s">
+        <v>679</v>
+      </c>
+      <c r="G108" t="s">
+        <v>552</v>
+      </c>
+      <c r="H108">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F109" t="s">
+        <v>781</v>
+      </c>
+      <c r="K109" t="s">
+        <v>782</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -10329,7 +10682,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
se actulizo el reporte, con los solicitos Listado de reportes activos
</commit_message>
<xml_diff>
--- a/00-Documentacion/Listado_Modulos2.xlsx
+++ b/00-Documentacion/Listado_Modulos2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\pc\raul\Net\migracion_spooler\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E271144-8005-4C59-8F0E-A277B2B94AAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{319C9CE1-D0C4-4DF4-8488-E25972A8879D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="859" activeTab="1" xr2:uid="{9A494972-654C-41EC-A971-3BEDBD7DDBA9}"/>
+    <workbookView xWindow="2235" yWindow="840" windowWidth="12450" windowHeight="9270" tabRatio="859" activeTab="3" xr2:uid="{9A494972-654C-41EC-A971-3BEDBD7DDBA9}"/>
   </bookViews>
   <sheets>
     <sheet name="Opción de Menú vs Funcion param" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1165" uniqueCount="792">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1240" uniqueCount="820">
   <si>
     <t>Opción de Menú</t>
   </si>
@@ -2508,6 +2508,90 @@
   </si>
   <si>
     <t>4 Reunión con Ricardo explicación de función de Get_IP();,    4.1Reunión con Ricardo explicación de función de filter_file_name</t>
+  </si>
+  <si>
+    <t>excel. Correo</t>
+  </si>
+  <si>
+    <t>excel. Correo, ftp</t>
+  </si>
+  <si>
+    <t>conecta los objetos a base de datos, titulos y rutas</t>
+  </si>
+  <si>
+    <t>ObtienePrecioXnui</t>
+  </si>
+  <si>
+    <t>Se obtiene el monto por NUI y se calcula el monto inicial de la Factura</t>
+  </si>
+  <si>
+    <t>MakeTxtFile</t>
+  </si>
+  <si>
+    <t>genera txt</t>
+  </si>
+  <si>
+    <t>Excel_simple3</t>
+  </si>
+  <si>
+    <t>genera formto de excel</t>
+  </si>
+  <si>
+    <t>excel,correo</t>
+  </si>
+  <si>
+    <t>excel</t>
+  </si>
+  <si>
+    <t>generea el formato de excel</t>
+  </si>
+  <si>
+    <t>sc_reportes_step_folios_egr_ing_pend</t>
+  </si>
+  <si>
+    <t>consumo store</t>
+  </si>
+  <si>
+    <t>genera una conexión ala base de datso</t>
+  </si>
+  <si>
+    <t>SQL</t>
+  </si>
+  <si>
+    <t>sc_reportes_gen_rep_clave</t>
+  </si>
+  <si>
+    <t>consume store</t>
+  </si>
+  <si>
+    <t>sc_reportes_fondo_fijo</t>
+  </si>
+  <si>
+    <t>backlog2</t>
+  </si>
+  <si>
+    <t>put_ctnr</t>
+  </si>
+  <si>
+    <t>agregar los numeros de CTNR</t>
+  </si>
+  <si>
+    <t>full_tab</t>
+  </si>
+  <si>
+    <t>para llenar la tabla, los tabl en excel</t>
+  </si>
+  <si>
+    <t>put_factura</t>
+  </si>
+  <si>
+    <t>agregar los numeros de factura, de PO y los nombres de provedores</t>
+  </si>
+  <si>
+    <t>QuickSort</t>
+  </si>
+  <si>
+    <t>funcion de ordenamiento recursivo</t>
   </si>
 </sst>
 </file>
@@ -2881,6 +2965,9 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="5"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2943,9 +3030,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="5"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7908,7 +7992,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A24CCD5-B140-49E1-9D6E-67F75307E332}">
   <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -7944,7 +8028,7 @@
       <c r="C2" t="s">
         <v>669</v>
       </c>
-      <c r="D2" s="63" t="s">
+      <c r="D2" s="42" t="s">
         <v>787</v>
       </c>
     </row>
@@ -7958,7 +8042,7 @@
       <c r="C3" t="s">
         <v>669</v>
       </c>
-      <c r="D3" s="63" t="s">
+      <c r="D3" s="42" t="s">
         <v>788</v>
       </c>
     </row>
@@ -7972,7 +8056,7 @@
       <c r="C4" t="s">
         <v>669</v>
       </c>
-      <c r="D4" s="63" t="s">
+      <c r="D4" s="42" t="s">
         <v>790</v>
       </c>
     </row>
@@ -7986,7 +8070,7 @@
       <c r="C5" t="s">
         <v>669</v>
       </c>
-      <c r="D5" s="63" t="s">
+      <c r="D5" s="42" t="s">
         <v>791</v>
       </c>
     </row>
@@ -8000,7 +8084,7 @@
       <c r="C6" t="s">
         <v>665</v>
       </c>
-      <c r="D6" s="63" t="s">
+      <c r="D6" s="42" t="s">
         <v>789</v>
       </c>
     </row>
@@ -8727,13 +8811,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD54439F-40DB-4068-9758-9F0A5DA03583}">
-  <dimension ref="A1:O117"/>
+  <dimension ref="A1:O150"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F101" activePane="bottomRight" state="frozenSplit"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="5" ySplit="1" topLeftCell="F143" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D118" sqref="D118"/>
+      <selection pane="bottomRight" activeCell="E153" sqref="E153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10711,6 +10795,428 @@
         <v>673</v>
       </c>
     </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A118" s="7">
+        <v>146</v>
+      </c>
+      <c r="B118" s="5"/>
+      <c r="C118" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="D118" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="E118" s="5" t="s">
+        <v>792</v>
+      </c>
+      <c r="F118" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D119"/>
+      <c r="E119"/>
+      <c r="F119" t="s">
+        <v>462</v>
+      </c>
+      <c r="K119" s="6" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D120"/>
+      <c r="E120"/>
+      <c r="F120" t="s">
+        <v>676</v>
+      </c>
+      <c r="H120">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A121" s="7">
+        <v>223</v>
+      </c>
+      <c r="B121" s="5"/>
+      <c r="C121" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="D121" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="E121" s="5" t="s">
+        <v>793</v>
+      </c>
+      <c r="F121" t="s">
+        <v>222</v>
+      </c>
+      <c r="H121">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D122"/>
+      <c r="E122"/>
+      <c r="F122" t="s">
+        <v>462</v>
+      </c>
+      <c r="K122" s="6" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D123"/>
+      <c r="E123"/>
+      <c r="F123" t="s">
+        <v>795</v>
+      </c>
+      <c r="H123">
+        <v>1</v>
+      </c>
+      <c r="K123" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D124"/>
+      <c r="E124"/>
+      <c r="F124" t="s">
+        <v>260</v>
+      </c>
+      <c r="H124">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D125"/>
+      <c r="E125"/>
+      <c r="F125" t="s">
+        <v>797</v>
+      </c>
+      <c r="H125">
+        <v>1</v>
+      </c>
+      <c r="K125" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D126"/>
+      <c r="E126"/>
+      <c r="F126" t="s">
+        <v>463</v>
+      </c>
+      <c r="H126">
+        <v>1</v>
+      </c>
+      <c r="K126" s="6" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D127"/>
+      <c r="E127"/>
+      <c r="F127" t="s">
+        <v>799</v>
+      </c>
+      <c r="K127" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A128" s="7">
+        <v>224</v>
+      </c>
+      <c r="B128" s="5"/>
+      <c r="C128" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="D128" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="E128" s="5" t="s">
+        <v>801</v>
+      </c>
+      <c r="F128" t="s">
+        <v>223</v>
+      </c>
+      <c r="H128">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D129"/>
+      <c r="E129"/>
+      <c r="F129" t="s">
+        <v>462</v>
+      </c>
+      <c r="K129" s="6" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D130"/>
+      <c r="E130"/>
+      <c r="F130" t="s">
+        <v>795</v>
+      </c>
+      <c r="H130">
+        <v>1</v>
+      </c>
+      <c r="K130" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D131"/>
+      <c r="E131"/>
+      <c r="F131" t="s">
+        <v>463</v>
+      </c>
+      <c r="H131">
+        <v>1</v>
+      </c>
+      <c r="K131" s="6" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A132" s="7">
+        <v>138</v>
+      </c>
+      <c r="B132" s="5"/>
+      <c r="C132" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="D132" s="5" t="s">
+        <v>389</v>
+      </c>
+      <c r="E132" s="5" t="s">
+        <v>802</v>
+      </c>
+      <c r="F132" s="1" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D133"/>
+      <c r="E133"/>
+      <c r="F133" t="s">
+        <v>462</v>
+      </c>
+      <c r="K133" s="6" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D134"/>
+      <c r="E134"/>
+      <c r="F134" t="s">
+        <v>679</v>
+      </c>
+      <c r="G134" t="s">
+        <v>552</v>
+      </c>
+      <c r="H134">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D135"/>
+      <c r="E135"/>
+      <c r="F135" t="s">
+        <v>781</v>
+      </c>
+      <c r="K135" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A136" s="7">
+        <v>298</v>
+      </c>
+      <c r="B136" s="5"/>
+      <c r="C136" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="D136" s="5" t="s">
+        <v>659</v>
+      </c>
+      <c r="E136" s="5" t="s">
+        <v>801</v>
+      </c>
+      <c r="F136" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D137"/>
+      <c r="E137"/>
+      <c r="F137" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D138"/>
+      <c r="E138"/>
+      <c r="F138" t="s">
+        <v>804</v>
+      </c>
+      <c r="H138">
+        <v>1</v>
+      </c>
+      <c r="K138" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D139"/>
+      <c r="E139"/>
+      <c r="F139" t="s">
+        <v>742</v>
+      </c>
+      <c r="K139" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D140"/>
+      <c r="E140"/>
+      <c r="F140" t="s">
+        <v>807</v>
+      </c>
+      <c r="H140">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A141" s="7">
+        <v>299</v>
+      </c>
+      <c r="B141" s="5"/>
+      <c r="C141" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="D141" s="5" t="s">
+        <v>660</v>
+      </c>
+      <c r="E141" s="5" t="s">
+        <v>478</v>
+      </c>
+      <c r="F141" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D142"/>
+      <c r="E142"/>
+      <c r="F142" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D143"/>
+      <c r="E143"/>
+      <c r="F143" t="s">
+        <v>808</v>
+      </c>
+      <c r="H143">
+        <v>1</v>
+      </c>
+      <c r="K143" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D144"/>
+      <c r="E144"/>
+      <c r="F144" t="s">
+        <v>810</v>
+      </c>
+      <c r="H144">
+        <v>1</v>
+      </c>
+      <c r="K144" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A145" s="7">
+        <v>6</v>
+      </c>
+      <c r="B145" s="5"/>
+      <c r="C145" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D145" s="5" t="s">
+        <v>811</v>
+      </c>
+      <c r="E145" s="5" t="s">
+        <v>801</v>
+      </c>
+      <c r="F145" t="s">
+        <v>811</v>
+      </c>
+      <c r="H145">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D146"/>
+      <c r="E146"/>
+      <c r="F146" t="s">
+        <v>462</v>
+      </c>
+      <c r="K146" s="6" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D147"/>
+      <c r="E147"/>
+      <c r="F147" t="s">
+        <v>812</v>
+      </c>
+      <c r="H147">
+        <v>1</v>
+      </c>
+      <c r="K147" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D148"/>
+      <c r="E148"/>
+      <c r="F148" t="s">
+        <v>814</v>
+      </c>
+      <c r="K148" t="s">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D149"/>
+      <c r="E149"/>
+      <c r="F149" t="s">
+        <v>816</v>
+      </c>
+      <c r="H149">
+        <v>2</v>
+      </c>
+      <c r="K149" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D150"/>
+      <c r="E150"/>
+      <c r="F150" t="s">
+        <v>818</v>
+      </c>
+      <c r="K150" t="s">
+        <v>819</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -10733,11 +11239,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="46" t="s">
         <v>498</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="47"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="48"/>
     </row>
     <row r="2" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
@@ -10765,9 +11271,9 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="48"/>
-      <c r="B4" s="49"/>
-      <c r="C4" s="50"/>
+      <c r="A4" s="49"/>
+      <c r="B4" s="50"/>
+      <c r="C4" s="51"/>
     </row>
     <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
@@ -10803,9 +11309,9 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="48"/>
-      <c r="B8" s="49"/>
-      <c r="C8" s="50"/>
+      <c r="A8" s="49"/>
+      <c r="B8" s="50"/>
+      <c r="C8" s="51"/>
     </row>
     <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
@@ -10822,9 +11328,9 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="48"/>
-      <c r="B10" s="49"/>
-      <c r="C10" s="50"/>
+      <c r="A10" s="49"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="51"/>
     </row>
     <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
@@ -10841,9 +11347,9 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="48"/>
-      <c r="B12" s="49"/>
-      <c r="C12" s="50"/>
+      <c r="A12" s="49"/>
+      <c r="B12" s="50"/>
+      <c r="C12" s="51"/>
     </row>
     <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="13" t="s">
@@ -10857,9 +11363,9 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="48"/>
-      <c r="B14" s="49"/>
-      <c r="C14" s="50"/>
+      <c r="A14" s="49"/>
+      <c r="B14" s="50"/>
+      <c r="C14" s="51"/>
     </row>
     <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="21" t="s">
@@ -10873,9 +11379,9 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="42"/>
-      <c r="B16" s="43"/>
-      <c r="C16" s="44"/>
+      <c r="A16" s="43"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="45"/>
     </row>
     <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="13" t="s">
@@ -10889,9 +11395,9 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="42"/>
-      <c r="B18" s="43"/>
-      <c r="C18" s="44"/>
+      <c r="A18" s="43"/>
+      <c r="B18" s="44"/>
+      <c r="C18" s="45"/>
     </row>
     <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="13" t="s">
@@ -10905,9 +11411,9 @@
       </c>
     </row>
     <row r="20" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="42"/>
-      <c r="B20" s="43"/>
-      <c r="C20" s="44"/>
+      <c r="A20" s="43"/>
+      <c r="B20" s="44"/>
+      <c r="C20" s="45"/>
     </row>
     <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="13" t="s">
@@ -10921,9 +11427,9 @@
       </c>
     </row>
     <row r="22" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="42"/>
-      <c r="B22" s="43"/>
-      <c r="C22" s="44"/>
+      <c r="A22" s="43"/>
+      <c r="B22" s="44"/>
+      <c r="C22" s="45"/>
     </row>
     <row r="23" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="13" t="s">
@@ -10969,11 +11475,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="46" t="s">
         <v>520</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="47"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="48"/>
     </row>
     <row r="2" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
@@ -10994,13 +11500,13 @@
       <c r="C3" s="23"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="55" t="s">
+      <c r="A4" s="56" t="s">
         <v>524</v>
       </c>
       <c r="B4" s="24" t="s">
         <v>525</v>
       </c>
-      <c r="C4" s="57" t="s">
+      <c r="C4" s="58" t="s">
         <v>526</v>
       </c>
       <c r="D4" s="7">
@@ -11008,11 +11514,11 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="56"/>
+      <c r="A5" s="57"/>
       <c r="B5" s="25" t="s">
         <v>527</v>
       </c>
-      <c r="C5" s="58"/>
+      <c r="C5" s="59"/>
     </row>
     <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="26" t="s">
@@ -11026,40 +11532,40 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="59" t="s">
+      <c r="A7" s="60" t="s">
         <v>531</v>
       </c>
       <c r="B7" s="29" t="s">
         <v>532</v>
       </c>
-      <c r="C7" s="61" t="s">
+      <c r="C7" s="62" t="s">
         <v>533</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="60"/>
+      <c r="A8" s="61"/>
       <c r="B8" s="30" t="s">
         <v>534</v>
       </c>
-      <c r="C8" s="62"/>
+      <c r="C8" s="63"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="59" t="s">
+      <c r="A9" s="60" t="s">
         <v>535</v>
       </c>
       <c r="B9" s="29" t="s">
         <v>532</v>
       </c>
-      <c r="C9" s="61" t="s">
+      <c r="C9" s="62" t="s">
         <v>533</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="60"/>
+      <c r="A10" s="61"/>
       <c r="B10" s="30" t="s">
         <v>534</v>
       </c>
-      <c r="C10" s="62"/>
+      <c r="C10" s="63"/>
     </row>
     <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="26" t="s">
@@ -11143,22 +11649,22 @@
       <c r="C19" s="35"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="51" t="s">
+      <c r="A20" s="52" t="s">
         <v>546</v>
       </c>
       <c r="B20" s="36" t="s">
         <v>547</v>
       </c>
-      <c r="C20" s="53" t="s">
+      <c r="C20" s="54" t="s">
         <v>533</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="52"/>
+      <c r="A21" s="53"/>
       <c r="B21" s="16" t="s">
         <v>548</v>
       </c>
-      <c r="C21" s="54"/>
+      <c r="C21" s="55"/>
     </row>
     <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="32"/>

</xml_diff>

<commit_message>
actualizacion de sql de menu principal con las decripcion y el numero de parametros  ruta sql spooler/main/sql main_act.txt
</commit_message>
<xml_diff>
--- a/00-Documentacion/Listado_Modulos2.xlsx
+++ b/00-Documentacion/Listado_Modulos2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\pc\raul\Net\migracion_spooler\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{319C9CE1-D0C4-4DF4-8488-E25972A8879D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA59FDCB-39F7-4BA9-B5B6-63D272C03118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2235" yWindow="840" windowWidth="12450" windowHeight="9270" tabRatio="859" activeTab="3" xr2:uid="{9A494972-654C-41EC-A971-3BEDBD7DDBA9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="859" activeTab="3" xr2:uid="{9A494972-654C-41EC-A971-3BEDBD7DDBA9}"/>
   </bookViews>
   <sheets>
     <sheet name="Opción de Menú vs Funcion param" sheetId="1" r:id="rId1"/>
@@ -8817,7 +8817,7 @@
       <pane xSplit="5" ySplit="1" topLeftCell="F143" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E153" sqref="E153"/>
+      <selection pane="bottomRight" activeCell="D148" sqref="D148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Se actualizaron las siguientes columnas (correo,liga,ftp,ws,txt,excel)
</commit_message>
<xml_diff>
--- a/00-Documentacion/Listado_Modulos2.xlsx
+++ b/00-Documentacion/Listado_Modulos2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\pc\raul\Net\migracion_spooler\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6877C66-B377-4D11-8540-ACCC52FD9540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFF22A87-2DC6-469B-AA4B-892B0CE84632}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="859" activeTab="3" xr2:uid="{9A494972-654C-41EC-A971-3BEDBD7DDBA9}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1557" uniqueCount="981">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1617" uniqueCount="989">
   <si>
     <t>Opción de Menú</t>
   </si>
@@ -3100,6 +3100,30 @@
   </si>
   <si>
     <t>ObtieneStatusTalon_txt</t>
+  </si>
+  <si>
+    <t>IsInArray</t>
+  </si>
+  <si>
+    <t>ws,ftp,pdf,correo,excel,zip</t>
+  </si>
+  <si>
+    <t>BuscarCliente</t>
+  </si>
+  <si>
+    <t>iniciliza conexión bd</t>
+  </si>
+  <si>
+    <t>listado de direccion de ftp</t>
+  </si>
+  <si>
+    <t>explore_folder</t>
+  </si>
+  <si>
+    <t>write_ftp_bat</t>
+  </si>
+  <si>
+    <t>IsInArray_Single</t>
   </si>
 </sst>
 </file>
@@ -3501,6 +3525,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3563,12 +3593,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -9547,13 +9571,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD54439F-40DB-4068-9758-9F0A5DA03583}">
-  <dimension ref="A1:O328"/>
+  <dimension ref="A1:O365"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F183" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F315" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G199" sqref="G199"/>
+      <selection pane="bottomRight" activeCell="F325" sqref="F325"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13734,7 +13758,7 @@
     <row r="263" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D263"/>
       <c r="E263"/>
-      <c r="F263" s="65" t="s">
+      <c r="F263" s="44" t="s">
         <v>948</v>
       </c>
       <c r="H263">
@@ -14313,7 +14337,7 @@
         <v>2</v>
       </c>
       <c r="B307" s="9"/>
-      <c r="C307" s="66" t="s">
+      <c r="C307" s="45" t="s">
         <v>144</v>
       </c>
       <c r="D307" s="9" t="s">
@@ -14623,6 +14647,383 @@
       </c>
       <c r="I328">
         <v>3</v>
+      </c>
+    </row>
+    <row r="329" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A329" s="9">
+        <v>15</v>
+      </c>
+      <c r="B329" s="9"/>
+      <c r="C329" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D329" s="9"/>
+      <c r="E329" s="9" t="s">
+        <v>898</v>
+      </c>
+      <c r="F329" t="s">
+        <v>5</v>
+      </c>
+      <c r="H329">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="330" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D330"/>
+      <c r="E330"/>
+      <c r="F330" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="331" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D331"/>
+      <c r="E331"/>
+      <c r="F331" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="332" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D332"/>
+      <c r="E332"/>
+      <c r="F332" t="s">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="333" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A333" s="9">
+        <v>173</v>
+      </c>
+      <c r="B333" s="9"/>
+      <c r="C333" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D333" s="9"/>
+      <c r="E333" s="9" t="s">
+        <v>982</v>
+      </c>
+      <c r="F333" t="s">
+        <v>69</v>
+      </c>
+      <c r="H333">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="334" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D334"/>
+      <c r="E334"/>
+      <c r="F334" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="335" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D335"/>
+      <c r="E335"/>
+      <c r="F335" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="336" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D336"/>
+      <c r="E336"/>
+      <c r="F336" t="s">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="337" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D337"/>
+      <c r="E337"/>
+      <c r="F337" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="338" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D338"/>
+      <c r="E338"/>
+      <c r="F338" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="339" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A339" s="9">
+        <v>328</v>
+      </c>
+      <c r="B339" s="9"/>
+      <c r="C339" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="D339" s="9"/>
+      <c r="E339" s="9" t="s">
+        <v>760</v>
+      </c>
+      <c r="F339" t="s">
+        <v>653</v>
+      </c>
+      <c r="H339">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="340" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D340"/>
+      <c r="E340"/>
+      <c r="F340" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="341" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D341"/>
+      <c r="E341"/>
+      <c r="F341" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="342" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A342" s="9">
+        <v>5</v>
+      </c>
+      <c r="B342" s="9"/>
+      <c r="C342" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="D342" s="9" t="s">
+        <v>378</v>
+      </c>
+      <c r="E342" s="9" t="s">
+        <v>760</v>
+      </c>
+      <c r="F342" t="s">
+        <v>378</v>
+      </c>
+      <c r="H342">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="343" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D343"/>
+      <c r="E343"/>
+      <c r="F343" t="s">
+        <v>459</v>
+      </c>
+      <c r="K343" t="s">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="344" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A344" s="9">
+        <v>248</v>
+      </c>
+      <c r="B344" s="9"/>
+      <c r="C344" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="D344" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="E344" s="9" t="s">
+        <v>906</v>
+      </c>
+      <c r="F344" t="s">
+        <v>120</v>
+      </c>
+      <c r="H344">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="345" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D345"/>
+      <c r="E345"/>
+      <c r="F345" t="s">
+        <v>753</v>
+      </c>
+      <c r="H345">
+        <v>1</v>
+      </c>
+      <c r="K345" t="s">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="346" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D346"/>
+      <c r="E346"/>
+      <c r="F346" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="347" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D347"/>
+      <c r="E347"/>
+      <c r="F347" t="s">
+        <v>986</v>
+      </c>
+    </row>
+    <row r="348" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D348"/>
+      <c r="E348"/>
+      <c r="F348" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="349" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D349"/>
+      <c r="E349"/>
+      <c r="F349" t="s">
+        <v>986</v>
+      </c>
+    </row>
+    <row r="350" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D350"/>
+      <c r="E350"/>
+      <c r="F350" t="s">
+        <v>987</v>
+      </c>
+    </row>
+    <row r="351" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D351"/>
+      <c r="E351"/>
+      <c r="F351" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="352" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A352" s="9">
+        <v>20</v>
+      </c>
+      <c r="B352" s="9"/>
+      <c r="C352" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D352" s="9"/>
+      <c r="E352" s="9" t="s">
+        <v>898</v>
+      </c>
+      <c r="F352" t="s">
+        <v>317</v>
+      </c>
+      <c r="H352">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="353" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D353"/>
+      <c r="E353"/>
+      <c r="F353" t="s">
+        <v>459</v>
+      </c>
+      <c r="K353" t="s">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="354" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D354"/>
+      <c r="E354"/>
+      <c r="F354" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="355" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D355"/>
+      <c r="E355"/>
+      <c r="F355" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="356" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D356"/>
+      <c r="E356"/>
+      <c r="F356" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="357" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D357"/>
+      <c r="E357"/>
+      <c r="F357" t="s">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="358" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A358" s="9">
+        <v>22</v>
+      </c>
+      <c r="B358" s="9"/>
+      <c r="C358" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D358" s="9"/>
+      <c r="E358" s="9" t="s">
+        <v>898</v>
+      </c>
+      <c r="F358" t="s">
+        <v>317</v>
+      </c>
+      <c r="H358">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="359" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D359"/>
+      <c r="E359"/>
+      <c r="F359" t="s">
+        <v>459</v>
+      </c>
+      <c r="K359" t="s">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="360" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D360"/>
+      <c r="E360"/>
+      <c r="F360" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="361" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D361"/>
+      <c r="E361"/>
+      <c r="F361" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="362" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D362"/>
+      <c r="E362"/>
+      <c r="F362" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="363" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D363"/>
+      <c r="E363"/>
+      <c r="F363" t="s">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="364" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A364" s="9">
+        <v>128</v>
+      </c>
+      <c r="B364" s="9"/>
+      <c r="C364" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="D364" s="9"/>
+      <c r="E364" s="9" t="s">
+        <v>898</v>
+      </c>
+      <c r="F364" t="s">
+        <v>395</v>
+      </c>
+      <c r="H364">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="365" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D365"/>
+      <c r="E365"/>
+      <c r="F365" t="s">
+        <v>459</v>
+      </c>
+      <c r="K365" t="s">
+        <v>984</v>
       </c>
     </row>
   </sheetData>
@@ -14647,11 +15048,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="49" t="s">
         <v>495</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="49"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="51"/>
     </row>
     <row r="2" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
@@ -14679,9 +15080,9 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="50"/>
-      <c r="B4" s="51"/>
-      <c r="C4" s="52"/>
+      <c r="A4" s="52"/>
+      <c r="B4" s="53"/>
+      <c r="C4" s="54"/>
     </row>
     <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
@@ -14717,9 +15118,9 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="50"/>
-      <c r="B8" s="51"/>
-      <c r="C8" s="52"/>
+      <c r="A8" s="52"/>
+      <c r="B8" s="53"/>
+      <c r="C8" s="54"/>
     </row>
     <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
@@ -14736,9 +15137,9 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="50"/>
-      <c r="B10" s="51"/>
-      <c r="C10" s="52"/>
+      <c r="A10" s="52"/>
+      <c r="B10" s="53"/>
+      <c r="C10" s="54"/>
     </row>
     <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
@@ -14755,9 +15156,9 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="50"/>
-      <c r="B12" s="51"/>
-      <c r="C12" s="52"/>
+      <c r="A12" s="52"/>
+      <c r="B12" s="53"/>
+      <c r="C12" s="54"/>
     </row>
     <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="13" t="s">
@@ -14771,9 +15172,9 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="50"/>
-      <c r="B14" s="51"/>
-      <c r="C14" s="52"/>
+      <c r="A14" s="52"/>
+      <c r="B14" s="53"/>
+      <c r="C14" s="54"/>
     </row>
     <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="21" t="s">
@@ -14787,9 +15188,9 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="44"/>
-      <c r="B16" s="45"/>
-      <c r="C16" s="46"/>
+      <c r="A16" s="46"/>
+      <c r="B16" s="47"/>
+      <c r="C16" s="48"/>
     </row>
     <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="13" t="s">
@@ -14803,9 +15204,9 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="44"/>
-      <c r="B18" s="45"/>
-      <c r="C18" s="46"/>
+      <c r="A18" s="46"/>
+      <c r="B18" s="47"/>
+      <c r="C18" s="48"/>
     </row>
     <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="13" t="s">
@@ -14819,9 +15220,9 @@
       </c>
     </row>
     <row r="20" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="44"/>
-      <c r="B20" s="45"/>
-      <c r="C20" s="46"/>
+      <c r="A20" s="46"/>
+      <c r="B20" s="47"/>
+      <c r="C20" s="48"/>
     </row>
     <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="13" t="s">
@@ -14835,9 +15236,9 @@
       </c>
     </row>
     <row r="22" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="44"/>
-      <c r="B22" s="45"/>
-      <c r="C22" s="46"/>
+      <c r="A22" s="46"/>
+      <c r="B22" s="47"/>
+      <c r="C22" s="48"/>
     </row>
     <row r="23" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="13" t="s">
@@ -14883,11 +15284,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="49" t="s">
         <v>517</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="49"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="51"/>
     </row>
     <row r="2" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
@@ -14908,13 +15309,13 @@
       <c r="C3" s="23"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="57" t="s">
+      <c r="A4" s="59" t="s">
         <v>521</v>
       </c>
       <c r="B4" s="24" t="s">
         <v>522</v>
       </c>
-      <c r="C4" s="59" t="s">
+      <c r="C4" s="61" t="s">
         <v>523</v>
       </c>
       <c r="D4" s="7">
@@ -14922,11 +15323,11 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="58"/>
+      <c r="A5" s="60"/>
       <c r="B5" s="25" t="s">
         <v>524</v>
       </c>
-      <c r="C5" s="60"/>
+      <c r="C5" s="62"/>
     </row>
     <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="26" t="s">
@@ -14940,40 +15341,40 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="61" t="s">
+      <c r="A7" s="63" t="s">
         <v>528</v>
       </c>
       <c r="B7" s="29" t="s">
         <v>529</v>
       </c>
-      <c r="C7" s="63" t="s">
+      <c r="C7" s="65" t="s">
         <v>530</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="62"/>
+      <c r="A8" s="64"/>
       <c r="B8" s="30" t="s">
         <v>531</v>
       </c>
-      <c r="C8" s="64"/>
+      <c r="C8" s="66"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="61" t="s">
+      <c r="A9" s="63" t="s">
         <v>532</v>
       </c>
       <c r="B9" s="29" t="s">
         <v>529</v>
       </c>
-      <c r="C9" s="63" t="s">
+      <c r="C9" s="65" t="s">
         <v>530</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="62"/>
+      <c r="A10" s="64"/>
       <c r="B10" s="30" t="s">
         <v>531</v>
       </c>
-      <c r="C10" s="64"/>
+      <c r="C10" s="66"/>
     </row>
     <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="26" t="s">
@@ -15057,22 +15458,22 @@
       <c r="C19" s="35"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="53" t="s">
+      <c r="A20" s="55" t="s">
         <v>543</v>
       </c>
       <c r="B20" s="36" t="s">
         <v>544</v>
       </c>
-      <c r="C20" s="55" t="s">
+      <c r="C20" s="57" t="s">
         <v>530</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="54"/>
+      <c r="A21" s="56"/>
       <c r="B21" s="16" t="s">
         <v>545</v>
       </c>
-      <c r="C21" s="56"/>
+      <c r="C21" s="58"/>
     </row>
     <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="32"/>

</xml_diff>

<commit_message>
Estructura de actividades RGG 20240522
1. se documentaron:
cd_ltl_email
rent_exp_cedis
imp_exp_bosch
facturas_conceptos_magnetti
ftp_clientesruta \00-Documentacion\Listado_Modulos2.xlsx "descriptivo- detalle a migrar f"

2 Se actualizaron las columnas txt, ws, pdf, zip  de los proceso que estan mapeados
3 Se actualizaron los command agreados, localizando los tipos de comunicion
4 Se actualizaron de matriz de los command agreados : (correo,liga,ftp,ws,txt,excel,xml,pdf,zip,otros)
5 se realizo diagrama Documentacion\diagrama\ Diagrama de flujo Spooler 1er parte - solicitud de datos.pdf
</commit_message>
<xml_diff>
--- a/00-Documentacion/Listado_Modulos2.xlsx
+++ b/00-Documentacion/Listado_Modulos2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\pc\raul\Net\migracion_spooler\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFF22A87-2DC6-469B-AA4B-892B0CE84632}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B3FD020-EC8D-4537-AB4F-1B6E48FC4CD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="859" activeTab="3" xr2:uid="{9A494972-654C-41EC-A971-3BEDBD7DDBA9}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1617" uniqueCount="989">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1674" uniqueCount="1002">
   <si>
     <t>Opción de Menú</t>
   </si>
@@ -3124,6 +3124,45 @@
   </si>
   <si>
     <t>IsInArray_Single</t>
+  </si>
+  <si>
+    <t>listado de contacto envio correo</t>
+  </si>
+  <si>
+    <t>ValidEmail</t>
+  </si>
+  <si>
+    <t>valida estruxtura de correo</t>
+  </si>
+  <si>
+    <t>TIPO_OPERACION</t>
+  </si>
+  <si>
+    <t>FORMAS_PAGO</t>
+  </si>
+  <si>
+    <t>SQL_CONCEPTOS</t>
+  </si>
+  <si>
+    <t>SQL_E</t>
+  </si>
+  <si>
+    <t>SQL_Facturas</t>
+  </si>
+  <si>
+    <t>GET_MONTO_CONCEPTO</t>
+  </si>
+  <si>
+    <t>SQL_F_A</t>
+  </si>
+  <si>
+    <t>zip, pdf, excel, correo,ftp</t>
+  </si>
+  <si>
+    <t>save_files_his</t>
+  </si>
+  <si>
+    <t>ESTE PROCEDIMIENTO TRANSFIERE LOS ARCHIVOS QUE ESTAN EN EL ARRAY real_files_to_transfer</t>
   </si>
 </sst>
 </file>
@@ -9571,13 +9610,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD54439F-40DB-4068-9758-9F0A5DA03583}">
-  <dimension ref="A1:O365"/>
+  <dimension ref="A1:O402"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F315" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F387" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F325" sqref="F325"/>
+      <selection pane="bottomRight" activeCell="C366" sqref="C366:C385"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15024,6 +15063,420 @@
       </c>
       <c r="K365" t="s">
         <v>984</v>
+      </c>
+    </row>
+    <row r="366" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A366" s="9">
+        <v>242</v>
+      </c>
+      <c r="B366" s="9"/>
+      <c r="C366" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="D366" s="9" t="s">
+        <v>568</v>
+      </c>
+      <c r="E366" s="9" t="s">
+        <v>898</v>
+      </c>
+      <c r="F366" t="s">
+        <v>568</v>
+      </c>
+      <c r="H366">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="367" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D367"/>
+      <c r="E367"/>
+      <c r="F367" t="s">
+        <v>459</v>
+      </c>
+      <c r="K367" t="s">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="368" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D368"/>
+      <c r="E368"/>
+      <c r="F368" t="s">
+        <v>615</v>
+      </c>
+      <c r="H368">
+        <v>1</v>
+      </c>
+      <c r="K368" t="s">
+        <v>989</v>
+      </c>
+    </row>
+    <row r="369" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D369"/>
+      <c r="E369"/>
+      <c r="F369" t="s">
+        <v>990</v>
+      </c>
+      <c r="K369" t="s">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="370" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A370" s="9">
+        <v>98</v>
+      </c>
+      <c r="B370" s="9"/>
+      <c r="C370" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D370" s="9" t="s">
+        <v>362</v>
+      </c>
+      <c r="E370" s="9" t="s">
+        <v>898</v>
+      </c>
+      <c r="F370" t="s">
+        <v>362</v>
+      </c>
+      <c r="H370">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="371" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D371"/>
+      <c r="E371"/>
+      <c r="F371" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="372" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D372"/>
+      <c r="E372"/>
+      <c r="F372" t="s">
+        <v>992</v>
+      </c>
+    </row>
+    <row r="373" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A373" s="9">
+        <v>322</v>
+      </c>
+      <c r="B373" s="9"/>
+      <c r="C373" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="D373" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="E373" s="9" t="s">
+        <v>898</v>
+      </c>
+      <c r="F373" t="s">
+        <v>145</v>
+      </c>
+      <c r="H373">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="374" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D374"/>
+      <c r="E374"/>
+      <c r="F374" t="s">
+        <v>459</v>
+      </c>
+      <c r="K374" t="s">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="375" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D375"/>
+      <c r="E375"/>
+      <c r="F375" t="s">
+        <v>993</v>
+      </c>
+      <c r="H375">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="376" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D376"/>
+      <c r="E376"/>
+      <c r="F376" t="s">
+        <v>671</v>
+      </c>
+      <c r="H376">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="377" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A377" s="9">
+        <v>220</v>
+      </c>
+      <c r="B377" s="9"/>
+      <c r="C377" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="D377" s="9"/>
+      <c r="E377" s="9" t="s">
+        <v>898</v>
+      </c>
+      <c r="F377" t="s">
+        <v>405</v>
+      </c>
+      <c r="I377">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="378" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D378"/>
+      <c r="E378"/>
+      <c r="F378" t="s">
+        <v>459</v>
+      </c>
+      <c r="I378">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="379" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D379"/>
+      <c r="E379"/>
+      <c r="F379" t="s">
+        <v>755</v>
+      </c>
+      <c r="H379">
+        <v>2</v>
+      </c>
+      <c r="I379">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="380" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D380"/>
+      <c r="E380"/>
+      <c r="F380" t="s">
+        <v>994</v>
+      </c>
+      <c r="G380" t="s">
+        <v>549</v>
+      </c>
+      <c r="H380">
+        <v>1</v>
+      </c>
+      <c r="I380">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="381" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D381"/>
+      <c r="E381"/>
+      <c r="F381" t="s">
+        <v>995</v>
+      </c>
+      <c r="H381">
+        <v>4</v>
+      </c>
+      <c r="I381">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="382" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D382"/>
+      <c r="E382"/>
+      <c r="F382" t="s">
+        <v>996</v>
+      </c>
+      <c r="H382">
+        <v>2</v>
+      </c>
+      <c r="I382">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="383" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D383"/>
+      <c r="E383"/>
+      <c r="F383" t="s">
+        <v>997</v>
+      </c>
+      <c r="I383">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="384" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D384"/>
+      <c r="E384"/>
+      <c r="F384" t="s">
+        <v>998</v>
+      </c>
+      <c r="H384">
+        <v>1</v>
+      </c>
+      <c r="I384">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="385" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A385" s="9">
+        <v>269</v>
+      </c>
+      <c r="B385" s="9"/>
+      <c r="C385" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="D385" s="9" t="s">
+        <v>375</v>
+      </c>
+      <c r="E385" s="9" t="s">
+        <v>999</v>
+      </c>
+      <c r="F385" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="386" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D386"/>
+      <c r="E386"/>
+      <c r="F386" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="387" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D387"/>
+      <c r="E387"/>
+      <c r="F387" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="388" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D388"/>
+      <c r="E388"/>
+      <c r="F388" t="s">
+        <v>610</v>
+      </c>
+      <c r="H388">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="389" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D389"/>
+      <c r="E389"/>
+      <c r="F389" t="s">
+        <v>613</v>
+      </c>
+      <c r="H389">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="390" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D390"/>
+      <c r="E390"/>
+      <c r="F390" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="391" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D391"/>
+      <c r="E391"/>
+      <c r="F391" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="392" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D392"/>
+      <c r="E392"/>
+      <c r="F392" t="s">
+        <v>631</v>
+      </c>
+      <c r="H392">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="393" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D393"/>
+      <c r="E393"/>
+      <c r="F393" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="394" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D394"/>
+      <c r="E394"/>
+      <c r="F394" t="s">
+        <v>1000</v>
+      </c>
+      <c r="H394">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="395" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D395"/>
+      <c r="E395"/>
+      <c r="F395" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="396" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D396"/>
+      <c r="E396"/>
+      <c r="F396" t="s">
+        <v>647</v>
+      </c>
+      <c r="H396">
+        <v>2</v>
+      </c>
+      <c r="K396" t="s">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="397" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D397"/>
+      <c r="E397"/>
+      <c r="F397" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="398" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D398"/>
+      <c r="E398"/>
+      <c r="F398" t="s">
+        <v>649</v>
+      </c>
+      <c r="H398">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="399" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D399"/>
+      <c r="E399"/>
+      <c r="F399" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="400" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D400"/>
+      <c r="E400"/>
+      <c r="F400" t="s">
+        <v>468</v>
+      </c>
+      <c r="H400">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="401" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D401"/>
+      <c r="E401"/>
+      <c r="F401" t="s">
+        <v>472</v>
+      </c>
+      <c r="H401">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="402" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D402"/>
+      <c r="E402"/>
+      <c r="F402" t="s">
+        <v>624</v>
+      </c>
+      <c r="H402">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Estructura de actividades RGG 20240523
1. se documentaron:
 versiono \00-Documentacion\Listado_Modulos2.xlsx "descriptivo- detalle a migrar f"
ftp_clientes
trans_bosch
aviso_pago_pedim
back_cliente_mot_vin
carga_ltl_helvex
cove_consulta
lista_edc
pedimentos_cove
pedim_pdf_doda
back_resumen_aduana
carga_ltl_austromex
update_BTM
codigos_pedimentos
control_digit_entrada
trading_cp_pendientes_fact
cp_periodo
factura_de_pedimento
ftp_cfd_con_excel
2. Se actualizaron de matriz de los command deacuredo a lo doucuemnatos- se aplicaron cambios
                     (correo,liga,ftp,ws,txt,excel,xml,pdf,zip,otros)
     versionador \00-Documentacion\Listado de reportes totales.xlsx
3. Se realizaron ajuste al diagrama de flujo de la primera parte de solicitud de reporte.
     versionador \00-Documentacion\diagrama\ Diagrama de flujo Spooler 1er parte - solicitud de datos.pdf
</commit_message>
<xml_diff>
--- a/00-Documentacion/Listado_Modulos2.xlsx
+++ b/00-Documentacion/Listado_Modulos2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\pc\raul\Net\migracion_spooler\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B3FD020-EC8D-4537-AB4F-1B6E48FC4CD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6514952-085C-4847-8B27-0E9316177F85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="859" activeTab="3" xr2:uid="{9A494972-654C-41EC-A971-3BEDBD7DDBA9}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1674" uniqueCount="1002">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1825" uniqueCount="1040">
   <si>
     <t>Opción de Menú</t>
   </si>
@@ -3093,9 +3093,6 @@
     <t>Excel_Gen</t>
   </si>
   <si>
-    <t>correo,excel,zip,ftp</t>
-  </si>
-  <si>
     <t>pdf,zip,correo,excel,xml</t>
   </si>
   <si>
@@ -3163,6 +3160,123 @@
   </si>
   <si>
     <t>ESTE PROCEDIMIENTO TRANSFIERE LOS ARCHIVOS QUE ESTAN EN EL ARRAY real_files_to_transfer</t>
+  </si>
+  <si>
+    <t>correo, excel, Link</t>
+  </si>
+  <si>
+    <t>correo.excel</t>
+  </si>
+  <si>
+    <t>resumen_aduana</t>
+  </si>
+  <si>
+    <t>SQL_Det</t>
+  </si>
+  <si>
+    <t>inicaliza columnas</t>
+  </si>
+  <si>
+    <t>LIMPIA_TEB</t>
+  </si>
+  <si>
+    <t>excel,correo,ws,pdf</t>
+  </si>
+  <si>
+    <t>xml_envio_archivo</t>
+  </si>
+  <si>
+    <t>3.2.1</t>
+  </si>
+  <si>
+    <t>Init_PGP_Data</t>
+  </si>
+  <si>
+    <t>3.2.2</t>
+  </si>
+  <si>
+    <t>get_certificado_datos</t>
+  </si>
+  <si>
+    <t>3.2.3</t>
+  </si>
+  <si>
+    <t>GetSelloDigital</t>
+  </si>
+  <si>
+    <t>3.2.4</t>
+  </si>
+  <si>
+    <t>xml_respuesta</t>
+  </si>
+  <si>
+    <t>cove_web_service</t>
+  </si>
+  <si>
+    <t>pdf,correo,excel</t>
+  </si>
+  <si>
+    <t>SQL_PEDTOS_ANTOLIN</t>
+  </si>
+  <si>
+    <t>SQL_DODA</t>
+  </si>
+  <si>
+    <t>SQL_CLAVE_PEDTOS</t>
+  </si>
+  <si>
+    <t>tab_resumen_export</t>
+  </si>
+  <si>
+    <t>ws,correo,pdf,excel,xml,ftp</t>
+  </si>
+  <si>
+    <t>update_BTM</t>
+  </si>
+  <si>
+    <t>update_BTM_VALID</t>
+  </si>
+  <si>
+    <t>ftp, correo , excel</t>
+  </si>
+  <si>
+    <t>ws,correo,excel</t>
+  </si>
+  <si>
+    <t>xml_consulta_tipos</t>
+  </si>
+  <si>
+    <t>SQL_CAJAS</t>
+  </si>
+  <si>
+    <t>correo,excel,txt</t>
+  </si>
+  <si>
+    <t>SQL_F</t>
+  </si>
+  <si>
+    <t>imprimir_resumen_ori_dest_CP_Vacio</t>
+  </si>
+  <si>
+    <t>fill_tabs_CP_Vacio</t>
+  </si>
+  <si>
+    <t>fill_tabs_Cedis_CP_Vacio</t>
+  </si>
+  <si>
+    <t>imprimir_resumen_ori_dest_Cedis_CP_Vacio</t>
+  </si>
+  <si>
+    <t>correo,excel,zip,ftp,txt</t>
+  </si>
+  <si>
+    <t>SQL_Rep</t>
+  </si>
+  <si>
+    <t>ftp,correo,pdf,excel,zip</t>
+  </si>
+  <si>
+    <t>ftp_cfd_logis</t>
   </si>
 </sst>
 </file>
@@ -3439,7 +3553,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -3569,6 +3683,9 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -9610,13 +9727,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD54439F-40DB-4068-9758-9F0A5DA03583}">
-  <dimension ref="A1:O402"/>
+  <dimension ref="A1:O510"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F387" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F496" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C366" sqref="C366:C385"/>
+      <selection pane="bottomRight" activeCell="F511" sqref="F511"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14616,7 +14733,7 @@
         <v>246</v>
       </c>
       <c r="E324" s="9" t="s">
-        <v>978</v>
+        <v>1036</v>
       </c>
       <c r="F324" t="s">
         <v>246</v>
@@ -14653,7 +14770,7 @@
         <v>44</v>
       </c>
       <c r="E326" s="9" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="F326" t="s">
         <v>44</v>
@@ -14682,7 +14799,7 @@
       <c r="D328"/>
       <c r="E328"/>
       <c r="F328" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="I328">
         <v>3</v>
@@ -14703,8 +14820,14 @@
       <c r="F329" t="s">
         <v>5</v>
       </c>
+      <c r="G329">
+        <v>2</v>
+      </c>
       <c r="H329">
         <v>2</v>
+      </c>
+      <c r="I329">
+        <v>1</v>
       </c>
     </row>
     <row r="330" spans="1:9" x14ac:dyDescent="0.25">
@@ -14713,6 +14836,9 @@
       <c r="F330" t="s">
         <v>459</v>
       </c>
+      <c r="I330">
+        <v>2</v>
+      </c>
     </row>
     <row r="331" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D331"/>
@@ -14720,12 +14846,18 @@
       <c r="F331" t="s">
         <v>460</v>
       </c>
+      <c r="I331">
+        <v>3</v>
+      </c>
     </row>
     <row r="332" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D332"/>
       <c r="E332"/>
       <c r="F332" t="s">
-        <v>981</v>
+        <v>980</v>
+      </c>
+      <c r="I332">
+        <v>4</v>
       </c>
     </row>
     <row r="333" spans="1:9" x14ac:dyDescent="0.25">
@@ -14738,13 +14870,19 @@
       </c>
       <c r="D333" s="9"/>
       <c r="E333" s="9" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="F333" t="s">
         <v>69</v>
       </c>
+      <c r="G333">
+        <v>7</v>
+      </c>
       <c r="H333">
         <v>7</v>
+      </c>
+      <c r="I333">
+        <v>1</v>
       </c>
     </row>
     <row r="334" spans="1:9" x14ac:dyDescent="0.25">
@@ -14753,6 +14891,9 @@
       <c r="F334" t="s">
         <v>459</v>
       </c>
+      <c r="I334">
+        <v>2</v>
+      </c>
     </row>
     <row r="335" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D335"/>
@@ -14760,12 +14901,18 @@
       <c r="F335" t="s">
         <v>466</v>
       </c>
+      <c r="I335">
+        <v>3</v>
+      </c>
     </row>
     <row r="336" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D336"/>
       <c r="E336"/>
       <c r="F336" t="s">
-        <v>983</v>
+        <v>982</v>
+      </c>
+      <c r="I336">
+        <v>4</v>
       </c>
     </row>
     <row r="337" spans="1:11" x14ac:dyDescent="0.25">
@@ -14774,6 +14921,9 @@
       <c r="F337" t="s">
         <v>836</v>
       </c>
+      <c r="I337">
+        <v>5</v>
+      </c>
     </row>
     <row r="338" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D338"/>
@@ -14781,6 +14931,9 @@
       <c r="F338" t="s">
         <v>838</v>
       </c>
+      <c r="I338">
+        <v>6</v>
+      </c>
     </row>
     <row r="339" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A339" s="9">
@@ -14797,8 +14950,14 @@
       <c r="F339" t="s">
         <v>653</v>
       </c>
+      <c r="G339">
+        <v>12</v>
+      </c>
       <c r="H339">
         <v>12</v>
+      </c>
+      <c r="I339">
+        <v>1</v>
       </c>
     </row>
     <row r="340" spans="1:11" x14ac:dyDescent="0.25">
@@ -14807,6 +14966,9 @@
       <c r="F340" t="s">
         <v>459</v>
       </c>
+      <c r="I340">
+        <v>2</v>
+      </c>
     </row>
     <row r="341" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D341"/>
@@ -14814,6 +14976,9 @@
       <c r="F341" t="s">
         <v>672</v>
       </c>
+      <c r="I341">
+        <v>3</v>
+      </c>
     </row>
     <row r="342" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A342" s="9">
@@ -14832,8 +14997,14 @@
       <c r="F342" t="s">
         <v>378</v>
       </c>
+      <c r="G342">
+        <v>16</v>
+      </c>
       <c r="H342">
         <v>16</v>
+      </c>
+      <c r="I342">
+        <v>1</v>
       </c>
     </row>
     <row r="343" spans="1:11" x14ac:dyDescent="0.25">
@@ -14842,8 +15013,11 @@
       <c r="F343" t="s">
         <v>459</v>
       </c>
+      <c r="I343">
+        <v>2</v>
+      </c>
       <c r="K343" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
     <row r="344" spans="1:11" x14ac:dyDescent="0.25">
@@ -14863,8 +15037,14 @@
       <c r="F344" t="s">
         <v>120</v>
       </c>
+      <c r="G344">
+        <v>5</v>
+      </c>
       <c r="H344">
         <v>4</v>
+      </c>
+      <c r="I344">
+        <v>1</v>
       </c>
     </row>
     <row r="345" spans="1:11" x14ac:dyDescent="0.25">
@@ -14876,8 +15056,11 @@
       <c r="H345">
         <v>1</v>
       </c>
+      <c r="I345">
+        <v>2</v>
+      </c>
       <c r="K345" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
     </row>
     <row r="346" spans="1:11" x14ac:dyDescent="0.25">
@@ -14886,12 +15069,18 @@
       <c r="F346" t="s">
         <v>622</v>
       </c>
+      <c r="I346">
+        <v>3</v>
+      </c>
     </row>
     <row r="347" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D347"/>
       <c r="E347"/>
       <c r="F347" t="s">
-        <v>986</v>
+        <v>985</v>
+      </c>
+      <c r="I347">
+        <v>4</v>
       </c>
     </row>
     <row r="348" spans="1:11" x14ac:dyDescent="0.25">
@@ -14900,19 +15089,28 @@
       <c r="F348" t="s">
         <v>460</v>
       </c>
+      <c r="I348">
+        <v>5</v>
+      </c>
     </row>
     <row r="349" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D349"/>
       <c r="E349"/>
       <c r="F349" t="s">
-        <v>986</v>
+        <v>985</v>
+      </c>
+      <c r="I349">
+        <v>6</v>
       </c>
     </row>
     <row r="350" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D350"/>
       <c r="E350"/>
       <c r="F350" t="s">
-        <v>987</v>
+        <v>986</v>
+      </c>
+      <c r="I350">
+        <v>7</v>
       </c>
     </row>
     <row r="351" spans="1:11" x14ac:dyDescent="0.25">
@@ -14921,6 +15119,9 @@
       <c r="F351" t="s">
         <v>459</v>
       </c>
+      <c r="I351">
+        <v>8</v>
+      </c>
     </row>
     <row r="352" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A352" s="9">
@@ -14937,8 +15138,14 @@
       <c r="F352" t="s">
         <v>317</v>
       </c>
+      <c r="G352">
+        <v>3</v>
+      </c>
       <c r="H352">
         <v>3</v>
+      </c>
+      <c r="I352">
+        <v>1</v>
       </c>
     </row>
     <row r="353" spans="1:11" x14ac:dyDescent="0.25">
@@ -14947,8 +15154,11 @@
       <c r="F353" t="s">
         <v>459</v>
       </c>
+      <c r="I353">
+        <v>2</v>
+      </c>
       <c r="K353" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
     <row r="354" spans="1:11" x14ac:dyDescent="0.25">
@@ -14957,6 +15167,9 @@
       <c r="F354" t="s">
         <v>806</v>
       </c>
+      <c r="I354">
+        <v>3</v>
+      </c>
     </row>
     <row r="355" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D355"/>
@@ -14964,6 +15177,9 @@
       <c r="F355" t="s">
         <v>810</v>
       </c>
+      <c r="I355">
+        <v>4</v>
+      </c>
     </row>
     <row r="356" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D356"/>
@@ -14971,12 +15187,18 @@
       <c r="F356" t="s">
         <v>672</v>
       </c>
+      <c r="I356">
+        <v>5</v>
+      </c>
     </row>
     <row r="357" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D357"/>
       <c r="E357"/>
       <c r="F357" t="s">
-        <v>988</v>
+        <v>987</v>
+      </c>
+      <c r="I357">
+        <v>6</v>
       </c>
     </row>
     <row r="358" spans="1:11" x14ac:dyDescent="0.25">
@@ -14994,8 +15216,14 @@
       <c r="F358" t="s">
         <v>317</v>
       </c>
+      <c r="G358">
+        <v>3</v>
+      </c>
       <c r="H358">
         <v>3</v>
+      </c>
+      <c r="I358">
+        <v>1</v>
       </c>
     </row>
     <row r="359" spans="1:11" x14ac:dyDescent="0.25">
@@ -15004,8 +15232,11 @@
       <c r="F359" t="s">
         <v>459</v>
       </c>
+      <c r="I359">
+        <v>2</v>
+      </c>
       <c r="K359" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
     <row r="360" spans="1:11" x14ac:dyDescent="0.25">
@@ -15014,6 +15245,9 @@
       <c r="F360" t="s">
         <v>806</v>
       </c>
+      <c r="I360">
+        <v>3</v>
+      </c>
     </row>
     <row r="361" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D361"/>
@@ -15021,6 +15255,9 @@
       <c r="F361" t="s">
         <v>810</v>
       </c>
+      <c r="I361">
+        <v>4</v>
+      </c>
     </row>
     <row r="362" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D362"/>
@@ -15028,12 +15265,18 @@
       <c r="F362" t="s">
         <v>672</v>
       </c>
+      <c r="I362">
+        <v>5</v>
+      </c>
     </row>
     <row r="363" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D363"/>
       <c r="E363"/>
       <c r="F363" t="s">
-        <v>988</v>
+        <v>987</v>
+      </c>
+      <c r="I363">
+        <v>6</v>
       </c>
     </row>
     <row r="364" spans="1:11" x14ac:dyDescent="0.25">
@@ -15051,8 +15294,14 @@
       <c r="F364" t="s">
         <v>395</v>
       </c>
+      <c r="G364">
+        <v>6</v>
+      </c>
       <c r="H364">
         <v>6</v>
+      </c>
+      <c r="I364">
+        <v>1</v>
       </c>
     </row>
     <row r="365" spans="1:11" x14ac:dyDescent="0.25">
@@ -15061,8 +15310,11 @@
       <c r="F365" t="s">
         <v>459</v>
       </c>
+      <c r="I365">
+        <v>2</v>
+      </c>
       <c r="K365" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
     <row r="366" spans="1:11" x14ac:dyDescent="0.25">
@@ -15077,13 +15329,19 @@
         <v>568</v>
       </c>
       <c r="E366" s="9" t="s">
-        <v>898</v>
+        <v>1001</v>
       </c>
       <c r="F366" t="s">
         <v>568</v>
       </c>
+      <c r="G366">
+        <v>5</v>
+      </c>
       <c r="H366">
         <v>4</v>
+      </c>
+      <c r="I366">
+        <v>1</v>
       </c>
     </row>
     <row r="367" spans="1:11" x14ac:dyDescent="0.25">
@@ -15092,8 +15350,11 @@
       <c r="F367" t="s">
         <v>459</v>
       </c>
+      <c r="I367">
+        <v>2</v>
+      </c>
       <c r="K367" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
     <row r="368" spans="1:11" x14ac:dyDescent="0.25">
@@ -15105,18 +15366,24 @@
       <c r="H368">
         <v>1</v>
       </c>
+      <c r="I368">
+        <v>3</v>
+      </c>
       <c r="K368" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
     </row>
     <row r="369" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D369"/>
       <c r="E369"/>
       <c r="F369" t="s">
+        <v>989</v>
+      </c>
+      <c r="I369">
+        <v>4</v>
+      </c>
+      <c r="K369" t="s">
         <v>990</v>
-      </c>
-      <c r="K369" t="s">
-        <v>991</v>
       </c>
     </row>
     <row r="370" spans="1:11" x14ac:dyDescent="0.25">
@@ -15136,8 +15403,14 @@
       <c r="F370" t="s">
         <v>362</v>
       </c>
+      <c r="G370">
+        <v>8</v>
+      </c>
       <c r="H370">
         <v>8</v>
+      </c>
+      <c r="I370">
+        <v>1</v>
       </c>
     </row>
     <row r="371" spans="1:11" x14ac:dyDescent="0.25">
@@ -15146,12 +15419,18 @@
       <c r="F371" t="s">
         <v>459</v>
       </c>
+      <c r="I371">
+        <v>2</v>
+      </c>
     </row>
     <row r="372" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D372"/>
       <c r="E372"/>
       <c r="F372" t="s">
-        <v>992</v>
+        <v>991</v>
+      </c>
+      <c r="I372">
+        <v>3</v>
       </c>
     </row>
     <row r="373" spans="1:11" x14ac:dyDescent="0.25">
@@ -15171,8 +15450,14 @@
       <c r="F373" t="s">
         <v>145</v>
       </c>
+      <c r="G373">
+        <v>15</v>
+      </c>
       <c r="H373">
         <v>13</v>
+      </c>
+      <c r="I373">
+        <v>1</v>
       </c>
     </row>
     <row r="374" spans="1:11" x14ac:dyDescent="0.25">
@@ -15181,18 +15466,24 @@
       <c r="F374" t="s">
         <v>459</v>
       </c>
+      <c r="I374">
+        <v>2</v>
+      </c>
       <c r="K374" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
     <row r="375" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D375"/>
       <c r="E375"/>
       <c r="F375" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="H375">
         <v>1</v>
+      </c>
+      <c r="I375">
+        <v>3</v>
       </c>
     </row>
     <row r="376" spans="1:11" x14ac:dyDescent="0.25">
@@ -15204,6 +15495,9 @@
       <c r="H376">
         <v>1</v>
       </c>
+      <c r="I376">
+        <v>4</v>
+      </c>
     </row>
     <row r="377" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A377" s="9">
@@ -15219,6 +15513,9 @@
       </c>
       <c r="F377" t="s">
         <v>405</v>
+      </c>
+      <c r="G377">
+        <v>10</v>
       </c>
       <c r="I377">
         <v>1</v>
@@ -15251,7 +15548,7 @@
       <c r="D380"/>
       <c r="E380"/>
       <c r="F380" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="G380" t="s">
         <v>549</v>
@@ -15267,7 +15564,7 @@
       <c r="D381"/>
       <c r="E381"/>
       <c r="F381" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="H381">
         <v>4</v>
@@ -15280,7 +15577,7 @@
       <c r="D382"/>
       <c r="E382"/>
       <c r="F382" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="H382">
         <v>2</v>
@@ -15293,7 +15590,7 @@
       <c r="D383"/>
       <c r="E383"/>
       <c r="F383" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="I383">
         <v>6</v>
@@ -15303,7 +15600,7 @@
       <c r="D384"/>
       <c r="E384"/>
       <c r="F384" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="H384">
         <v>1</v>
@@ -15324,10 +15621,16 @@
         <v>375</v>
       </c>
       <c r="E385" s="9" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="F385" t="s">
         <v>375</v>
+      </c>
+      <c r="G385">
+        <v>11</v>
+      </c>
+      <c r="I385">
+        <v>1</v>
       </c>
     </row>
     <row r="386" spans="1:11" x14ac:dyDescent="0.25">
@@ -15336,6 +15639,9 @@
       <c r="F386" t="s">
         <v>460</v>
       </c>
+      <c r="I386">
+        <v>2</v>
+      </c>
     </row>
     <row r="387" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D387"/>
@@ -15343,6 +15649,9 @@
       <c r="F387" t="s">
         <v>459</v>
       </c>
+      <c r="I387">
+        <v>3</v>
+      </c>
     </row>
     <row r="388" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D388"/>
@@ -15353,6 +15662,9 @@
       <c r="H388">
         <v>1</v>
       </c>
+      <c r="I388">
+        <v>4</v>
+      </c>
     </row>
     <row r="389" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D389"/>
@@ -15363,6 +15675,9 @@
       <c r="H389">
         <v>1</v>
       </c>
+      <c r="I389">
+        <v>5</v>
+      </c>
     </row>
     <row r="390" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D390"/>
@@ -15370,6 +15685,9 @@
       <c r="F390" t="s">
         <v>619</v>
       </c>
+      <c r="I390">
+        <v>6</v>
+      </c>
     </row>
     <row r="391" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D391"/>
@@ -15377,6 +15695,9 @@
       <c r="F391" t="s">
         <v>622</v>
       </c>
+      <c r="I391">
+        <v>7</v>
+      </c>
     </row>
     <row r="392" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D392"/>
@@ -15387,6 +15708,9 @@
       <c r="H392">
         <v>1</v>
       </c>
+      <c r="I392">
+        <v>8</v>
+      </c>
     </row>
     <row r="393" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D393"/>
@@ -15394,15 +15718,21 @@
       <c r="F393" t="s">
         <v>627</v>
       </c>
+      <c r="I393">
+        <v>9</v>
+      </c>
     </row>
     <row r="394" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D394"/>
       <c r="E394"/>
       <c r="F394" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="H394">
         <v>1</v>
+      </c>
+      <c r="I394">
+        <v>10</v>
       </c>
     </row>
     <row r="395" spans="1:11" x14ac:dyDescent="0.25">
@@ -15411,6 +15741,9 @@
       <c r="F395" t="s">
         <v>643</v>
       </c>
+      <c r="I395">
+        <v>11</v>
+      </c>
     </row>
     <row r="396" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D396"/>
@@ -15421,8 +15754,11 @@
       <c r="H396">
         <v>2</v>
       </c>
+      <c r="I396">
+        <v>12</v>
+      </c>
       <c r="K396" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="397" spans="1:11" x14ac:dyDescent="0.25">
@@ -15431,6 +15767,9 @@
       <c r="F397" t="s">
         <v>650</v>
       </c>
+      <c r="I397">
+        <v>13</v>
+      </c>
     </row>
     <row r="398" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D398"/>
@@ -15441,6 +15780,9 @@
       <c r="H398">
         <v>1</v>
       </c>
+      <c r="I398">
+        <v>14</v>
+      </c>
     </row>
     <row r="399" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D399"/>
@@ -15448,6 +15790,9 @@
       <c r="F399" t="s">
         <v>639</v>
       </c>
+      <c r="I399">
+        <v>15</v>
+      </c>
     </row>
     <row r="400" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D400"/>
@@ -15458,8 +15803,11 @@
       <c r="H400">
         <v>1</v>
       </c>
-    </row>
-    <row r="401" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="I400">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="401" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D401"/>
       <c r="E401"/>
       <c r="F401" t="s">
@@ -15468,14 +15816,1429 @@
       <c r="H401">
         <v>2</v>
       </c>
-    </row>
-    <row r="402" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="I401">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="402" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D402"/>
       <c r="E402"/>
       <c r="F402" t="s">
         <v>624</v>
       </c>
       <c r="H402">
+        <v>1</v>
+      </c>
+      <c r="I402">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="403" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A403" s="9">
+        <v>9</v>
+      </c>
+      <c r="B403" s="9"/>
+      <c r="C403" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="D403" s="9" t="s">
+        <v>390</v>
+      </c>
+      <c r="E403" s="9"/>
+      <c r="F403" t="s">
+        <v>390</v>
+      </c>
+      <c r="G403">
+        <v>7</v>
+      </c>
+      <c r="H403">
+        <v>7</v>
+      </c>
+      <c r="I403">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="404" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D404"/>
+      <c r="E404"/>
+      <c r="F404" t="s">
+        <v>459</v>
+      </c>
+      <c r="I404">
+        <v>2</v>
+      </c>
+      <c r="K404" t="s">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="405" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A405" s="9">
+        <v>143</v>
+      </c>
+      <c r="B405" s="9"/>
+      <c r="C405" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="D405" s="9"/>
+      <c r="E405" s="9" t="s">
+        <v>1002</v>
+      </c>
+      <c r="F405" t="s">
+        <v>180</v>
+      </c>
+      <c r="G405">
+        <v>1</v>
+      </c>
+      <c r="H405">
+        <v>1</v>
+      </c>
+      <c r="I405">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="406" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D406"/>
+      <c r="E406"/>
+      <c r="F406" t="s">
+        <v>459</v>
+      </c>
+      <c r="I406">
+        <v>2</v>
+      </c>
+      <c r="K406" t="s">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="407" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A407" s="9">
+        <v>300</v>
+      </c>
+      <c r="B407" s="9"/>
+      <c r="C407" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D407" s="9"/>
+      <c r="E407" s="9"/>
+      <c r="F407" t="s">
+        <v>316</v>
+      </c>
+      <c r="G407">
+        <v>18</v>
+      </c>
+      <c r="H407">
+        <v>15</v>
+      </c>
+      <c r="I407">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="408" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D408"/>
+      <c r="E408"/>
+      <c r="F408" t="s">
+        <v>459</v>
+      </c>
+      <c r="I408">
+        <v>2</v>
+      </c>
+      <c r="K408" t="s">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="409" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D409"/>
+      <c r="E409"/>
+      <c r="F409" t="s">
+        <v>804</v>
+      </c>
+      <c r="H409">
+        <v>1</v>
+      </c>
+      <c r="I409">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="410" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D410"/>
+      <c r="E410"/>
+      <c r="F410" t="s">
+        <v>806</v>
+      </c>
+      <c r="I410">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="411" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D411"/>
+      <c r="E411"/>
+      <c r="F411" t="s">
+        <v>808</v>
+      </c>
+      <c r="H411">
+        <v>2</v>
+      </c>
+      <c r="I411">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="412" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D412"/>
+      <c r="E412"/>
+      <c r="F412" t="s">
+        <v>810</v>
+      </c>
+      <c r="I412">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="413" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D413"/>
+      <c r="E413"/>
+      <c r="F413" t="s">
+        <v>1003</v>
+      </c>
+      <c r="I413">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="414" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D414"/>
+      <c r="E414"/>
+      <c r="F414" t="s">
+        <v>672</v>
+      </c>
+      <c r="I414">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="415" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D415"/>
+      <c r="E415"/>
+      <c r="F415" t="s">
+        <v>987</v>
+      </c>
+      <c r="I415">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="416" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D416"/>
+      <c r="E416"/>
+      <c r="F416" t="s">
+        <v>1004</v>
+      </c>
+      <c r="I416">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="417" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A417" s="9">
+        <v>186</v>
+      </c>
+      <c r="B417" s="9"/>
+      <c r="C417" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="D417" s="9"/>
+      <c r="E417" s="9"/>
+      <c r="F417" t="s">
+        <v>101</v>
+      </c>
+      <c r="G417">
+        <v>35</v>
+      </c>
+      <c r="H417">
+        <v>2</v>
+      </c>
+      <c r="I417">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="418" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D418"/>
+      <c r="E418"/>
+      <c r="F418" t="s">
+        <v>459</v>
+      </c>
+      <c r="I418">
+        <v>2</v>
+      </c>
+      <c r="K418" t="s">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="419" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D419"/>
+      <c r="E419"/>
+      <c r="F419" t="s">
+        <v>908</v>
+      </c>
+      <c r="I419">
+        <v>3</v>
+      </c>
+      <c r="K419" t="s">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="420" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D420"/>
+      <c r="E420"/>
+      <c r="F420" t="s">
+        <v>913</v>
+      </c>
+      <c r="H420">
+        <v>4</v>
+      </c>
+      <c r="I420">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="421" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D421"/>
+      <c r="E421"/>
+      <c r="F421" t="s">
+        <v>915</v>
+      </c>
+      <c r="H421">
+        <v>8</v>
+      </c>
+      <c r="I421">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="422" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D422"/>
+      <c r="E422"/>
+      <c r="F422" s="46" t="s">
+        <v>974</v>
+      </c>
+      <c r="H422">
+        <v>1</v>
+      </c>
+      <c r="I422">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="423" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D423"/>
+      <c r="E423"/>
+      <c r="F423" s="46" t="s">
+        <v>973</v>
+      </c>
+      <c r="H423">
+        <v>5</v>
+      </c>
+      <c r="I423">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="424" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D424"/>
+      <c r="E424"/>
+      <c r="F424" s="46" t="s">
+        <v>1006</v>
+      </c>
+      <c r="H424">
+        <v>1</v>
+      </c>
+      <c r="I424">
+        <v>5.3</v>
+      </c>
+    </row>
+    <row r="425" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D425"/>
+      <c r="E425"/>
+      <c r="F425" s="46" t="s">
+        <v>917</v>
+      </c>
+      <c r="H425">
+        <v>2</v>
+      </c>
+      <c r="I425">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="426" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D426"/>
+      <c r="E426"/>
+      <c r="F426" s="46" t="s">
+        <v>918</v>
+      </c>
+      <c r="H426">
+        <v>1</v>
+      </c>
+      <c r="I426">
+        <v>6.1</v>
+      </c>
+    </row>
+    <row r="427" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D427"/>
+      <c r="E427"/>
+      <c r="F427" s="46" t="s">
+        <v>970</v>
+      </c>
+      <c r="H427">
+        <v>11</v>
+      </c>
+      <c r="I427">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="428" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D428"/>
+      <c r="E428"/>
+      <c r="F428" s="46" t="s">
+        <v>672</v>
+      </c>
+      <c r="I428">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="429" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A429" s="9">
+        <v>211</v>
+      </c>
+      <c r="B429" s="9"/>
+      <c r="C429" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="D429" s="9"/>
+      <c r="E429" s="9" t="s">
+        <v>1007</v>
+      </c>
+      <c r="F429" t="s">
+        <v>111</v>
+      </c>
+      <c r="G429">
+        <v>15</v>
+      </c>
+      <c r="H429">
+        <v>2</v>
+      </c>
+      <c r="I429">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="430" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D430"/>
+      <c r="E430"/>
+      <c r="F430" t="s">
+        <v>459</v>
+      </c>
+      <c r="I430">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="431" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D431"/>
+      <c r="E431"/>
+      <c r="F431" t="s">
+        <v>371</v>
+      </c>
+      <c r="I431">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="432" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D432"/>
+      <c r="E432"/>
+      <c r="F432" s="46" t="s">
+        <v>459</v>
+      </c>
+      <c r="I432">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="433" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D433"/>
+      <c r="E433"/>
+      <c r="F433" s="46" t="s">
+        <v>1008</v>
+      </c>
+      <c r="H433">
+        <v>2</v>
+      </c>
+      <c r="I433">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="434" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D434"/>
+      <c r="E434"/>
+      <c r="F434" s="46" t="s">
+        <v>372</v>
+      </c>
+      <c r="I434" s="43" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="435" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D435"/>
+      <c r="E435"/>
+      <c r="F435" s="46" t="s">
+        <v>1010</v>
+      </c>
+      <c r="H435">
+        <v>1</v>
+      </c>
+      <c r="I435" s="43" t="s">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="436" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D436"/>
+      <c r="E436"/>
+      <c r="F436" s="46" t="s">
+        <v>1012</v>
+      </c>
+      <c r="H436">
+        <v>2</v>
+      </c>
+      <c r="I436" s="43" t="s">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="437" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D437"/>
+      <c r="E437"/>
+      <c r="F437" s="46" t="s">
+        <v>1014</v>
+      </c>
+      <c r="H437">
+        <v>1</v>
+      </c>
+      <c r="I437" s="43" t="s">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="438" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D438"/>
+      <c r="E438"/>
+      <c r="F438" s="46" t="s">
+        <v>1016</v>
+      </c>
+      <c r="I438">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="439" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D439"/>
+      <c r="E439"/>
+      <c r="F439" s="46" t="s">
+        <v>643</v>
+      </c>
+      <c r="I439">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="440" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D440"/>
+      <c r="E440"/>
+      <c r="F440" s="46" t="s">
+        <v>1017</v>
+      </c>
+      <c r="H440">
+        <v>7</v>
+      </c>
+      <c r="I440">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="441" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D441"/>
+      <c r="E441"/>
+      <c r="F441" s="46" t="s">
+        <v>460</v>
+      </c>
+      <c r="I441">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="442" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D442"/>
+      <c r="E442"/>
+      <c r="F442" s="46" t="s">
+        <v>459</v>
+      </c>
+      <c r="I442">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="443" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A443" s="9">
+        <v>41</v>
+      </c>
+      <c r="B443" s="9"/>
+      <c r="C443" s="9" t="s">
+        <v>296</v>
+      </c>
+      <c r="D443" s="9"/>
+      <c r="E443" s="9" t="s">
+        <v>1018</v>
+      </c>
+      <c r="F443" s="43"/>
+      <c r="I443">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="444" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A444" s="9">
+        <v>216</v>
+      </c>
+      <c r="B444" s="9"/>
+      <c r="C444" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="D444" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="E444" s="9" t="s">
+        <v>760</v>
+      </c>
+      <c r="F444" t="s">
+        <v>228</v>
+      </c>
+      <c r="I444">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="445" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D445"/>
+      <c r="E445"/>
+      <c r="F445" t="s">
+        <v>459</v>
+      </c>
+      <c r="I445">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="446" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A446" s="9">
+        <v>326</v>
+      </c>
+      <c r="B446" s="9"/>
+      <c r="C446" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="D446" s="9"/>
+      <c r="E446" s="9" t="s">
+        <v>1018</v>
+      </c>
+      <c r="F446" t="s">
+        <v>290</v>
+      </c>
+      <c r="G446">
+        <v>9</v>
+      </c>
+      <c r="H446">
+        <v>5</v>
+      </c>
+      <c r="I446">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="447" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D447"/>
+      <c r="E447"/>
+      <c r="F447" t="s">
+        <v>459</v>
+      </c>
+      <c r="I447">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="448" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D448"/>
+      <c r="E448"/>
+      <c r="F448" t="s">
+        <v>615</v>
+      </c>
+      <c r="H448">
+        <v>1</v>
+      </c>
+      <c r="I448">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="449" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D449"/>
+      <c r="E449"/>
+      <c r="F449" t="s">
+        <v>1019</v>
+      </c>
+      <c r="H449">
+        <v>2</v>
+      </c>
+      <c r="I449">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="450" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D450"/>
+      <c r="E450"/>
+      <c r="F450" t="s">
+        <v>1020</v>
+      </c>
+      <c r="H450">
+        <v>1</v>
+      </c>
+      <c r="I450">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="451" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D451"/>
+      <c r="E451"/>
+      <c r="F451" t="s">
+        <v>1021</v>
+      </c>
+      <c r="I451">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="452" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A452" s="9">
+        <v>18</v>
+      </c>
+      <c r="B452" s="9"/>
+      <c r="C452" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D452" s="9"/>
+      <c r="E452" s="9" t="s">
+        <v>898</v>
+      </c>
+      <c r="F452" t="s">
+        <v>318</v>
+      </c>
+      <c r="G452">
+        <v>14</v>
+      </c>
+      <c r="H452">
+        <v>14</v>
+      </c>
+      <c r="I452">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="453" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D453"/>
+      <c r="E453"/>
+      <c r="F453" t="s">
+        <v>459</v>
+      </c>
+      <c r="I453">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="454" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D454"/>
+      <c r="E454"/>
+      <c r="F454" t="s">
+        <v>806</v>
+      </c>
+      <c r="I454">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="455" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D455"/>
+      <c r="E455"/>
+      <c r="F455" t="s">
+        <v>810</v>
+      </c>
+      <c r="I455">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="456" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D456"/>
+      <c r="E456"/>
+      <c r="F456" t="s">
+        <v>1022</v>
+      </c>
+      <c r="I456">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="457" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D457"/>
+      <c r="E457"/>
+      <c r="F457" t="s">
+        <v>672</v>
+      </c>
+      <c r="I457">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="458" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A458" s="9">
+        <v>282</v>
+      </c>
+      <c r="B458" s="9"/>
+      <c r="C458" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="D458" s="9"/>
+      <c r="E458" s="9" t="s">
+        <v>1023</v>
+      </c>
+      <c r="F458" t="s">
+        <v>103</v>
+      </c>
+      <c r="G458">
+        <v>19</v>
+      </c>
+      <c r="I458">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="459" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D459"/>
+      <c r="E459"/>
+      <c r="F459" t="s">
+        <v>459</v>
+      </c>
+      <c r="I459">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="460" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D460"/>
+      <c r="E460"/>
+      <c r="F460" t="s">
+        <v>908</v>
+      </c>
+      <c r="I460">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="461" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D461"/>
+      <c r="E461"/>
+      <c r="F461" t="s">
+        <v>913</v>
+      </c>
+      <c r="H461">
+        <v>1</v>
+      </c>
+      <c r="I461">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="462" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D462"/>
+      <c r="E462"/>
+      <c r="F462" t="s">
+        <v>915</v>
+      </c>
+      <c r="H462">
+        <v>3</v>
+      </c>
+      <c r="I462">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="463" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D463"/>
+      <c r="E463"/>
+      <c r="F463" t="s">
+        <v>917</v>
+      </c>
+      <c r="H463">
+        <v>1</v>
+      </c>
+      <c r="I463">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="464" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D464"/>
+      <c r="E464"/>
+      <c r="F464" s="46" t="s">
+        <v>44</v>
+      </c>
+      <c r="H464">
+        <v>6</v>
+      </c>
+      <c r="I464">
+        <v>6.1</v>
+      </c>
+    </row>
+    <row r="465" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D465"/>
+      <c r="E465"/>
+      <c r="F465" s="46" t="s">
+        <v>792</v>
+      </c>
+      <c r="I465">
+        <v>6.1</v>
+      </c>
+    </row>
+    <row r="466" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D466"/>
+      <c r="E466"/>
+      <c r="F466" s="46" t="s">
+        <v>918</v>
+      </c>
+      <c r="H466">
+        <v>1</v>
+      </c>
+      <c r="I466">
+        <v>6.1</v>
+      </c>
+    </row>
+    <row r="467" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D467"/>
+      <c r="E467"/>
+      <c r="F467" t="s">
+        <v>672</v>
+      </c>
+      <c r="I467">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="468" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D468"/>
+      <c r="E468"/>
+      <c r="F468" t="s">
+        <v>973</v>
+      </c>
+      <c r="H468">
+        <v>2</v>
+      </c>
+      <c r="I468">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="469" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D469"/>
+      <c r="E469"/>
+      <c r="F469" t="s">
+        <v>974</v>
+      </c>
+      <c r="H469">
+        <v>1</v>
+      </c>
+      <c r="I469">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="470" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D470"/>
+      <c r="E470"/>
+      <c r="F470" t="s">
+        <v>972</v>
+      </c>
+      <c r="H470">
+        <v>4</v>
+      </c>
+      <c r="I470">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="471" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A471" s="9">
+        <v>39</v>
+      </c>
+      <c r="B471" s="9"/>
+      <c r="C471" s="9" t="s">
+        <v>1024</v>
+      </c>
+      <c r="D471" s="9"/>
+      <c r="E471" s="9" t="s">
+        <v>760</v>
+      </c>
+      <c r="F471" t="s">
+        <v>1025</v>
+      </c>
+      <c r="G471">
+        <v>3</v>
+      </c>
+      <c r="H471">
+        <v>3</v>
+      </c>
+      <c r="I471">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="472" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D472"/>
+      <c r="E472"/>
+      <c r="F472" t="s">
+        <v>459</v>
+      </c>
+      <c r="I472">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="473" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A473" s="9">
+        <v>156</v>
+      </c>
+      <c r="B473" s="9"/>
+      <c r="C473" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="D473" s="9"/>
+      <c r="E473" s="9" t="s">
+        <v>1026</v>
+      </c>
+      <c r="F473" t="s">
+        <v>95</v>
+      </c>
+      <c r="I473">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="474" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A474" s="9">
+        <v>176</v>
+      </c>
+      <c r="B474" s="9"/>
+      <c r="C474" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="D474" s="9"/>
+      <c r="E474" s="9" t="s">
+        <v>760</v>
+      </c>
+      <c r="F474" t="s">
+        <v>189</v>
+      </c>
+      <c r="H474">
+        <v>1</v>
+      </c>
+      <c r="I474">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="475" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D475"/>
+      <c r="E475"/>
+      <c r="F475" t="s">
+        <v>459</v>
+      </c>
+      <c r="I475">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="476" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A476" s="9">
+        <v>246</v>
+      </c>
+      <c r="B476" s="9"/>
+      <c r="C476" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="D476" s="9"/>
+      <c r="E476" s="9" t="s">
+        <v>1027</v>
+      </c>
+      <c r="F476" t="s">
+        <v>373</v>
+      </c>
+      <c r="H476">
+        <v>3</v>
+      </c>
+      <c r="I476">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="477" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D477"/>
+      <c r="E477"/>
+      <c r="F477" t="s">
+        <v>459</v>
+      </c>
+      <c r="I477">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="478" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D478"/>
+      <c r="E478"/>
+      <c r="F478" t="s">
+        <v>1028</v>
+      </c>
+      <c r="I478">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="479" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D479"/>
+      <c r="E479"/>
+      <c r="F479" s="46" t="s">
+        <v>372</v>
+      </c>
+      <c r="I479">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="480" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D480"/>
+      <c r="E480"/>
+      <c r="F480" s="46" t="s">
+        <v>1010</v>
+      </c>
+      <c r="H480">
+        <v>1</v>
+      </c>
+      <c r="I480">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="481" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D481"/>
+      <c r="E481"/>
+      <c r="F481" s="46" t="s">
+        <v>1012</v>
+      </c>
+      <c r="H481">
+        <v>2</v>
+      </c>
+      <c r="I481">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="482" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D482"/>
+      <c r="E482"/>
+      <c r="F482" s="46" t="s">
+        <v>1014</v>
+      </c>
+      <c r="H482">
+        <v>1</v>
+      </c>
+      <c r="I482">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="483" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A483" s="9">
+        <v>236</v>
+      </c>
+      <c r="B483" s="9"/>
+      <c r="C483" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="D483" s="9"/>
+      <c r="E483" s="9" t="s">
+        <v>760</v>
+      </c>
+      <c r="F483" t="s">
+        <v>239</v>
+      </c>
+      <c r="H483">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="484" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D484"/>
+      <c r="E484"/>
+      <c r="F484" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="485" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D485"/>
+      <c r="E485"/>
+      <c r="F485" t="s">
+        <v>1029</v>
+      </c>
+      <c r="H485">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="486" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A486" s="9">
+        <v>249</v>
+      </c>
+      <c r="B486" s="9"/>
+      <c r="C486" s="9" t="s">
+        <v>250</v>
+      </c>
+      <c r="D486" s="9"/>
+      <c r="E486" s="9" t="s">
+        <v>1030</v>
+      </c>
+      <c r="F486" t="s">
+        <v>577</v>
+      </c>
+      <c r="H486">
+        <v>2</v>
+      </c>
+      <c r="I486">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="487" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D487"/>
+      <c r="E487"/>
+      <c r="F487" t="s">
+        <v>459</v>
+      </c>
+      <c r="I487">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="488" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D488"/>
+      <c r="E488"/>
+      <c r="F488" t="s">
+        <v>1031</v>
+      </c>
+      <c r="H488">
+        <v>2</v>
+      </c>
+      <c r="I488">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="489" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D489"/>
+      <c r="E489"/>
+      <c r="F489" t="s">
+        <v>888</v>
+      </c>
+      <c r="I489">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="490" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D490"/>
+      <c r="E490"/>
+      <c r="F490" t="s">
+        <v>1032</v>
+      </c>
+      <c r="I490">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="491" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D491"/>
+      <c r="E491"/>
+      <c r="F491" t="s">
+        <v>1033</v>
+      </c>
+      <c r="H491">
+        <v>2</v>
+      </c>
+      <c r="I491">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="492" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D492"/>
+      <c r="E492"/>
+      <c r="F492" t="s">
+        <v>1034</v>
+      </c>
+      <c r="H492">
+        <v>2</v>
+      </c>
+      <c r="I492">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="493" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D493"/>
+      <c r="E493"/>
+      <c r="F493" t="s">
+        <v>1035</v>
+      </c>
+      <c r="I493">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="494" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D494"/>
+      <c r="E494"/>
+      <c r="F494" t="s">
+        <v>572</v>
+      </c>
+      <c r="H494">
+        <v>3</v>
+      </c>
+      <c r="I494">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="495" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D495"/>
+      <c r="E495"/>
+      <c r="F495" t="s">
+        <v>459</v>
+      </c>
+      <c r="I495">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="496" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D496"/>
+      <c r="E496"/>
+      <c r="F496" t="s">
+        <v>1031</v>
+      </c>
+      <c r="H496">
+        <v>2</v>
+      </c>
+      <c r="I496">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="497" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D497"/>
+      <c r="E497"/>
+      <c r="F497" t="s">
+        <v>888</v>
+      </c>
+      <c r="I497">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="498" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D498"/>
+      <c r="E498"/>
+      <c r="F498" t="s">
+        <v>1032</v>
+      </c>
+      <c r="I498">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="499" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D499"/>
+      <c r="E499"/>
+      <c r="F499" t="s">
+        <v>1033</v>
+      </c>
+      <c r="H499">
+        <v>2</v>
+      </c>
+      <c r="I499">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="500" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D500"/>
+      <c r="E500"/>
+      <c r="F500" t="s">
+        <v>1034</v>
+      </c>
+      <c r="H500">
+        <v>2</v>
+      </c>
+      <c r="I500">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="501" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D501"/>
+      <c r="E501"/>
+      <c r="F501" t="s">
+        <v>1035</v>
+      </c>
+      <c r="I501">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="502" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D502"/>
+      <c r="E502"/>
+      <c r="F502" t="s">
+        <v>987</v>
+      </c>
+      <c r="I502">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="503" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D503"/>
+      <c r="E503"/>
+      <c r="F503" t="s">
+        <v>573</v>
+      </c>
+      <c r="I503">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="504" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A504" s="9">
+        <v>284</v>
+      </c>
+      <c r="B504" s="9"/>
+      <c r="C504" s="9" t="s">
+        <v>284</v>
+      </c>
+      <c r="D504" s="9"/>
+      <c r="E504" s="9" t="s">
+        <v>794</v>
+      </c>
+      <c r="F504" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="505" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D505"/>
+      <c r="E505"/>
+      <c r="F505" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="506" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D506"/>
+      <c r="E506"/>
+      <c r="F506" t="s">
+        <v>1037</v>
+      </c>
+      <c r="H506">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="507" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D507"/>
+      <c r="E507"/>
+      <c r="F507" t="s">
+        <v>1004</v>
+      </c>
+      <c r="H507">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="508" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A508" s="9">
+        <v>290</v>
+      </c>
+      <c r="B508" s="9"/>
+      <c r="C508" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="D508" s="9"/>
+      <c r="E508" s="9" t="s">
+        <v>1038</v>
+      </c>
+      <c r="F508" t="s">
+        <v>93</v>
+      </c>
+      <c r="H508">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="509" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D509"/>
+      <c r="E509"/>
+      <c r="F509" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="510" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D510"/>
+      <c r="E510"/>
+      <c r="F510" t="s">
+        <v>1039</v>
+      </c>
+      <c r="H510">
         <v>1</v>
       </c>
     </row>
@@ -15501,11 +17264,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="50" t="s">
         <v>495</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="51"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="52"/>
     </row>
     <row r="2" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
@@ -15533,9 +17296,9 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="52"/>
-      <c r="B4" s="53"/>
-      <c r="C4" s="54"/>
+      <c r="A4" s="53"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="55"/>
     </row>
     <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
@@ -15571,9 +17334,9 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="52"/>
-      <c r="B8" s="53"/>
-      <c r="C8" s="54"/>
+      <c r="A8" s="53"/>
+      <c r="B8" s="54"/>
+      <c r="C8" s="55"/>
     </row>
     <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
@@ -15590,9 +17353,9 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="52"/>
-      <c r="B10" s="53"/>
-      <c r="C10" s="54"/>
+      <c r="A10" s="53"/>
+      <c r="B10" s="54"/>
+      <c r="C10" s="55"/>
     </row>
     <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
@@ -15609,9 +17372,9 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="52"/>
-      <c r="B12" s="53"/>
-      <c r="C12" s="54"/>
+      <c r="A12" s="53"/>
+      <c r="B12" s="54"/>
+      <c r="C12" s="55"/>
     </row>
     <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="13" t="s">
@@ -15625,9 +17388,9 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="52"/>
-      <c r="B14" s="53"/>
-      <c r="C14" s="54"/>
+      <c r="A14" s="53"/>
+      <c r="B14" s="54"/>
+      <c r="C14" s="55"/>
     </row>
     <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="21" t="s">
@@ -15641,9 +17404,9 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="46"/>
-      <c r="B16" s="47"/>
-      <c r="C16" s="48"/>
+      <c r="A16" s="47"/>
+      <c r="B16" s="48"/>
+      <c r="C16" s="49"/>
     </row>
     <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="13" t="s">
@@ -15657,9 +17420,9 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="46"/>
-      <c r="B18" s="47"/>
-      <c r="C18" s="48"/>
+      <c r="A18" s="47"/>
+      <c r="B18" s="48"/>
+      <c r="C18" s="49"/>
     </row>
     <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="13" t="s">
@@ -15673,9 +17436,9 @@
       </c>
     </row>
     <row r="20" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="46"/>
-      <c r="B20" s="47"/>
-      <c r="C20" s="48"/>
+      <c r="A20" s="47"/>
+      <c r="B20" s="48"/>
+      <c r="C20" s="49"/>
     </row>
     <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="13" t="s">
@@ -15689,9 +17452,9 @@
       </c>
     </row>
     <row r="22" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="46"/>
-      <c r="B22" s="47"/>
-      <c r="C22" s="48"/>
+      <c r="A22" s="47"/>
+      <c r="B22" s="48"/>
+      <c r="C22" s="49"/>
     </row>
     <row r="23" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="13" t="s">
@@ -15737,11 +17500,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="50" t="s">
         <v>517</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="51"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="52"/>
     </row>
     <row r="2" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
@@ -15762,13 +17525,13 @@
       <c r="C3" s="23"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="59" t="s">
+      <c r="A4" s="60" t="s">
         <v>521</v>
       </c>
       <c r="B4" s="24" t="s">
         <v>522</v>
       </c>
-      <c r="C4" s="61" t="s">
+      <c r="C4" s="62" t="s">
         <v>523</v>
       </c>
       <c r="D4" s="7">
@@ -15776,11 +17539,11 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="60"/>
+      <c r="A5" s="61"/>
       <c r="B5" s="25" t="s">
         <v>524</v>
       </c>
-      <c r="C5" s="62"/>
+      <c r="C5" s="63"/>
     </row>
     <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="26" t="s">
@@ -15794,40 +17557,40 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="63" t="s">
+      <c r="A7" s="64" t="s">
         <v>528</v>
       </c>
       <c r="B7" s="29" t="s">
         <v>529</v>
       </c>
-      <c r="C7" s="65" t="s">
+      <c r="C7" s="66" t="s">
         <v>530</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="64"/>
+      <c r="A8" s="65"/>
       <c r="B8" s="30" t="s">
         <v>531</v>
       </c>
-      <c r="C8" s="66"/>
+      <c r="C8" s="67"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="63" t="s">
+      <c r="A9" s="64" t="s">
         <v>532</v>
       </c>
       <c r="B9" s="29" t="s">
         <v>529</v>
       </c>
-      <c r="C9" s="65" t="s">
+      <c r="C9" s="66" t="s">
         <v>530</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="64"/>
+      <c r="A10" s="65"/>
       <c r="B10" s="30" t="s">
         <v>531</v>
       </c>
-      <c r="C10" s="66"/>
+      <c r="C10" s="67"/>
     </row>
     <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="26" t="s">
@@ -15911,22 +17674,22 @@
       <c r="C19" s="35"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="55" t="s">
+      <c r="A20" s="56" t="s">
         <v>543</v>
       </c>
       <c r="B20" s="36" t="s">
         <v>544</v>
       </c>
-      <c r="C20" s="57" t="s">
+      <c r="C20" s="58" t="s">
         <v>530</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="56"/>
+      <c r="A21" s="57"/>
       <c r="B21" s="16" t="s">
         <v>545</v>
       </c>
-      <c r="C21" s="58"/>
+      <c r="C21" s="59"/>
     </row>
     <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="32"/>

</xml_diff>

<commit_message>
2.	se documentaron:   versiono \00-Documentacion\Listado_Modulos2.xlsx "descriptivo- detalle a migrar f"
                       	 fmc_reporte
			cd_cd_email
			invent_salidas_entradas
			trading_diario_fact_det
			pedimentos_imar_ws
pedimentos_imar_ws
3	Se actualizaron de matriz de los command de acuerdo a lo documentado- se aplicaron cambios
                     (correo,liga,ftp,ws,txt,excel,xml,pdf,zip,otros)
                     versionador \00-Documentacion\Listado de reportes totales.xlsx
</commit_message>
<xml_diff>
--- a/00-Documentacion/Listado_Modulos2.xlsx
+++ b/00-Documentacion/Listado_Modulos2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\pc\raul\Net\migracion_spooler\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6514952-085C-4847-8B27-0E9316177F85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC9DCA40-AE4D-4988-9479-60931F866366}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="859" activeTab="3" xr2:uid="{9A494972-654C-41EC-A971-3BEDBD7DDBA9}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1825" uniqueCount="1040">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1854" uniqueCount="1046">
   <si>
     <t>Opción de Menú</t>
   </si>
@@ -3278,12 +3278,30 @@
   <si>
     <t>ftp_cfd_logis</t>
   </si>
+  <si>
+    <t>SQL_MVTO</t>
+  </si>
+  <si>
+    <t>SQL_INVENT</t>
+  </si>
+  <si>
+    <t>SQL_REFS</t>
+  </si>
+  <si>
+    <t>PUT_DATA</t>
+  </si>
+  <si>
+    <t>ws,correo,excel,xml</t>
+  </si>
+  <si>
+    <t>soap_env</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3380,6 +3398,13 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -3553,7 +3578,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -3750,6 +3775,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9727,13 +9753,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD54439F-40DB-4068-9758-9F0A5DA03583}">
-  <dimension ref="A1:O510"/>
+  <dimension ref="A1:O530"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F496" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F511" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F511" sqref="F511"/>
+      <selection pane="bottomRight" activeCell="D525" sqref="D525"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17087,7 +17113,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="497" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="497" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D497"/>
       <c r="E497"/>
       <c r="F497" t="s">
@@ -17097,7 +17123,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="498" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="498" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D498"/>
       <c r="E498"/>
       <c r="F498" t="s">
@@ -17107,7 +17133,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="499" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="499" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D499"/>
       <c r="E499"/>
       <c r="F499" t="s">
@@ -17120,7 +17146,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="500" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="500" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D500"/>
       <c r="E500"/>
       <c r="F500" t="s">
@@ -17133,7 +17159,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="501" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="501" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D501"/>
       <c r="E501"/>
       <c r="F501" t="s">
@@ -17143,7 +17169,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="502" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="502" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D502"/>
       <c r="E502"/>
       <c r="F502" t="s">
@@ -17153,7 +17179,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="503" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="503" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D503"/>
       <c r="E503"/>
       <c r="F503" t="s">
@@ -17163,7 +17189,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="504" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="504" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A504" s="9">
         <v>284</v>
       </c>
@@ -17179,14 +17205,14 @@
         <v>284</v>
       </c>
     </row>
-    <row r="505" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="505" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D505"/>
       <c r="E505"/>
       <c r="F505" t="s">
         <v>459</v>
       </c>
     </row>
-    <row r="506" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="506" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D506"/>
       <c r="E506"/>
       <c r="F506" t="s">
@@ -17196,7 +17222,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="507" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="507" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D507"/>
       <c r="E507"/>
       <c r="F507" t="s">
@@ -17206,7 +17232,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="508" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="508" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A508" s="9">
         <v>290</v>
       </c>
@@ -17225,14 +17251,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="509" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="509" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D509"/>
       <c r="E509"/>
       <c r="F509" t="s">
         <v>459</v>
       </c>
     </row>
-    <row r="510" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="510" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D510"/>
       <c r="E510"/>
       <c r="F510" t="s">
@@ -17240,6 +17266,305 @@
       </c>
       <c r="H510">
         <v>1</v>
+      </c>
+    </row>
+    <row r="511" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A511" s="9">
+        <v>246</v>
+      </c>
+      <c r="B511" s="9"/>
+      <c r="C511" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="D511" s="9"/>
+      <c r="E511" s="9" t="s">
+        <v>1030</v>
+      </c>
+      <c r="F511" t="s">
+        <v>571</v>
+      </c>
+      <c r="G511">
+        <v>1</v>
+      </c>
+      <c r="H511">
+        <v>1</v>
+      </c>
+      <c r="I511">
+        <v>1</v>
+      </c>
+      <c r="J511" s="68"/>
+    </row>
+    <row r="512" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A512" s="68"/>
+      <c r="B512" s="68"/>
+      <c r="C512" s="68"/>
+      <c r="D512" s="68"/>
+      <c r="E512" s="68"/>
+      <c r="F512" t="s">
+        <v>459</v>
+      </c>
+      <c r="I512">
+        <v>2</v>
+      </c>
+      <c r="J512" s="68"/>
+    </row>
+    <row r="513" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A513" s="68"/>
+      <c r="B513" s="68"/>
+      <c r="C513" s="68"/>
+      <c r="D513" s="68"/>
+      <c r="E513" s="68"/>
+      <c r="I513">
+        <v>3</v>
+      </c>
+      <c r="J513" s="68"/>
+    </row>
+    <row r="514" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A514" s="9">
+        <v>287</v>
+      </c>
+      <c r="B514" s="9"/>
+      <c r="C514" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="D514" s="9"/>
+      <c r="E514" s="9" t="s">
+        <v>1030</v>
+      </c>
+      <c r="F514" t="s">
+        <v>569</v>
+      </c>
+      <c r="G514">
+        <v>3</v>
+      </c>
+      <c r="H514">
+        <v>3</v>
+      </c>
+      <c r="I514">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="515" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D515"/>
+      <c r="E515"/>
+      <c r="F515" t="s">
+        <v>459</v>
+      </c>
+      <c r="I515">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="516" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D516"/>
+      <c r="E516"/>
+      <c r="F516" t="s">
+        <v>989</v>
+      </c>
+      <c r="I516">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="517" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A517" s="9">
+        <v>213</v>
+      </c>
+      <c r="B517" s="9"/>
+      <c r="C517" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="D517" s="9"/>
+      <c r="E517" s="9" t="s">
+        <v>794</v>
+      </c>
+      <c r="F517" t="s">
+        <v>566</v>
+      </c>
+      <c r="G517">
+        <v>5</v>
+      </c>
+      <c r="H517">
+        <v>1</v>
+      </c>
+      <c r="I517">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="518" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D518"/>
+      <c r="E518"/>
+      <c r="F518" t="s">
+        <v>459</v>
+      </c>
+      <c r="I518">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="519" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D519"/>
+      <c r="E519"/>
+      <c r="F519" t="s">
+        <v>750</v>
+      </c>
+      <c r="H519">
+        <v>1</v>
+      </c>
+      <c r="I519">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="520" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D520"/>
+      <c r="E520"/>
+      <c r="F520" t="s">
+        <v>1040</v>
+      </c>
+      <c r="H520">
+        <v>1</v>
+      </c>
+      <c r="I520">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="521" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D521"/>
+      <c r="E521"/>
+      <c r="F521" t="s">
+        <v>1041</v>
+      </c>
+      <c r="H521">
+        <v>1</v>
+      </c>
+      <c r="I521">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="522" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D522"/>
+      <c r="E522"/>
+      <c r="F522" t="s">
+        <v>1042</v>
+      </c>
+      <c r="H522">
+        <v>1</v>
+      </c>
+      <c r="I522">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="523" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A523" s="9">
+        <v>119</v>
+      </c>
+      <c r="B523" s="9"/>
+      <c r="C523" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="D523" s="9"/>
+      <c r="E523" s="9" t="s">
+        <v>1030</v>
+      </c>
+      <c r="F523" t="s">
+        <v>160</v>
+      </c>
+      <c r="G523">
+        <v>5</v>
+      </c>
+      <c r="H523">
+        <v>3</v>
+      </c>
+      <c r="I523">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="524" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D524"/>
+      <c r="E524"/>
+      <c r="F524" t="s">
+        <v>459</v>
+      </c>
+      <c r="I524">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="525" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D525"/>
+      <c r="E525"/>
+      <c r="F525" t="s">
+        <v>995</v>
+      </c>
+      <c r="H525">
+        <v>1</v>
+      </c>
+      <c r="I525">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="526" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D526"/>
+      <c r="E526"/>
+      <c r="F526" t="s">
+        <v>994</v>
+      </c>
+      <c r="H526">
+        <v>1</v>
+      </c>
+      <c r="I526">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="527" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D527"/>
+      <c r="E527"/>
+      <c r="F527" t="s">
+        <v>1043</v>
+      </c>
+      <c r="I527">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="528" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A528" s="9">
+        <v>181</v>
+      </c>
+      <c r="B528" s="9"/>
+      <c r="C528" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D528" s="9"/>
+      <c r="E528" s="9" t="s">
+        <v>1044</v>
+      </c>
+      <c r="F528" t="s">
+        <v>73</v>
+      </c>
+      <c r="G528">
+        <v>3</v>
+      </c>
+      <c r="H528">
+        <v>3</v>
+      </c>
+      <c r="I528">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="529" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D529"/>
+      <c r="E529"/>
+      <c r="F529" t="s">
+        <v>459</v>
+      </c>
+      <c r="I529">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="530" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D530"/>
+      <c r="E530"/>
+      <c r="F530" t="s">
+        <v>1045</v>
+      </c>
+      <c r="I530">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Estructura de actividades RGG 20240527
1.    se documentaron:   versiono \00-Documentacion\Listado_Modulos2.xlsx "descriptivo- detalle a migrar f"
	entregas_fuji
	supp_inv
	ped_invoices_tupperware
	cfd_generacion
	clean_report
	dict_resumen
	evidencias_urrea
	facturas_conceptos
	facturas_johnson
	ftp_digit_cp
	ftp_digit_sucursale
	ftp_envios_M
	ftp_evidencias
	ftp_seg_automotive
	invent_cedis
	italika_tracking
	lista_refs
	pedimentos_absormex
	pedimentos_pdf
	resumen_anom3
2 	Se actualizaron de matriz de los command de acuerdo a lo documentado- se aplicaron cambios
                     (correo,liga,ftp,ws,txt,excel,xml,pdf,zip,otros)
                     versionador \00-Documentacion\Listado de reportes totales.xlsx
3.	Se realizaron ajuste a los sql en aplicación (rep_dias_libres  confirma fecha confirma fecha2)
</commit_message>
<xml_diff>
--- a/00-Documentacion/Listado_Modulos2.xlsx
+++ b/00-Documentacion/Listado_Modulos2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\pc\raul\Net\migracion_spooler\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC9DCA40-AE4D-4988-9479-60931F866366}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{346F8793-CF5B-43C4-81FD-E8000E1E8913}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="859" activeTab="3" xr2:uid="{9A494972-654C-41EC-A971-3BEDBD7DDBA9}"/>
   </bookViews>
@@ -20,6 +20,9 @@
     <sheet name="Reportes Automáticos SMO" sheetId="6" r:id="rId5"/>
     <sheet name="REPORTES AICM " sheetId="7" r:id="rId6"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'descriptivo- detalle a migrar f'!$A$1:$O$580</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -39,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1854" uniqueCount="1046">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1974" uniqueCount="1076">
   <si>
     <t>Opción de Menú</t>
   </si>
@@ -3295,6 +3298,96 @@
   </si>
   <si>
     <t>soap_env</t>
+  </si>
+  <si>
+    <t>correo,excel,ftp</t>
+  </si>
+  <si>
+    <t>upload_sftp</t>
+  </si>
+  <si>
+    <t>upload_ftp</t>
+  </si>
+  <si>
+    <t>correo,excel, txt</t>
+  </si>
+  <si>
+    <t>correo, factura</t>
+  </si>
+  <si>
+    <t>clean_logs</t>
+  </si>
+  <si>
+    <t>excel,correo,txt</t>
+  </si>
+  <si>
+    <t>correo,transfiere,zip</t>
+  </si>
+  <si>
+    <t>ftp,correo,pdf</t>
+  </si>
+  <si>
+    <t>validar_evidencia_cp</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>ftp_servers</t>
+  </si>
+  <si>
+    <t>Create_Entire_Path</t>
+  </si>
+  <si>
+    <t>ftp,correo,pdf,txt</t>
+  </si>
+  <si>
+    <t>correo,ftp,bat,pdf,txt</t>
+  </si>
+  <si>
+    <t>ftp_envios_M</t>
+  </si>
+  <si>
+    <t>ftp,correo,pdf,xml</t>
+  </si>
+  <si>
+    <t>no se encontro la funcion en archivo main</t>
+  </si>
+  <si>
+    <t>ftp,correo</t>
+  </si>
+  <si>
+    <t>ws,correo,txt</t>
+  </si>
+  <si>
+    <t>correo, txt</t>
+  </si>
+  <si>
+    <t>zip,pdf,correo,excel</t>
+  </si>
+  <si>
+    <t>SQL_PEDTOS_Absormex</t>
+  </si>
+  <si>
+    <t>SQL_MANIF</t>
+  </si>
+  <si>
+    <t>GenerarNombreArchivo</t>
+  </si>
+  <si>
+    <t>SQL_Q</t>
+  </si>
+  <si>
+    <t>SQL_Cliente</t>
+  </si>
+  <si>
+    <t>SQL_EDOCUMENTS</t>
+  </si>
+  <si>
+    <t>EnvioCorreo</t>
+  </si>
+  <si>
+    <t>pdf,correo,excel,zip</t>
   </si>
 </sst>
 </file>
@@ -3578,7 +3671,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -3712,6 +3805,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3775,7 +3869,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9753,13 +9847,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD54439F-40DB-4068-9758-9F0A5DA03583}">
-  <dimension ref="A1:O530"/>
+  <dimension ref="A1:O610"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F511" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F526" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D525" sqref="D525"/>
+      <selection pane="bottomRight" activeCell="D534" sqref="D534"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17292,32 +17386,32 @@
       <c r="I511">
         <v>1</v>
       </c>
-      <c r="J511" s="68"/>
+      <c r="J511" s="47"/>
     </row>
     <row r="512" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A512" s="68"/>
-      <c r="B512" s="68"/>
-      <c r="C512" s="68"/>
-      <c r="D512" s="68"/>
-      <c r="E512" s="68"/>
+      <c r="A512" s="47"/>
+      <c r="B512" s="47"/>
+      <c r="C512" s="47"/>
+      <c r="D512" s="47"/>
+      <c r="E512" s="47"/>
       <c r="F512" t="s">
         <v>459</v>
       </c>
       <c r="I512">
         <v>2</v>
       </c>
-      <c r="J512" s="68"/>
+      <c r="J512" s="47"/>
     </row>
     <row r="513" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A513" s="68"/>
-      <c r="B513" s="68"/>
-      <c r="C513" s="68"/>
-      <c r="D513" s="68"/>
-      <c r="E513" s="68"/>
+      <c r="A513" s="47"/>
+      <c r="B513" s="47"/>
+      <c r="C513" s="47"/>
+      <c r="D513" s="47"/>
+      <c r="E513" s="47"/>
       <c r="I513">
         <v>3</v>
       </c>
-      <c r="J513" s="68"/>
+      <c r="J513" s="47"/>
     </row>
     <row r="514" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A514" s="9">
@@ -17547,7 +17641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="529" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="529" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D529"/>
       <c r="E529"/>
       <c r="F529" t="s">
@@ -17557,7 +17651,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="530" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="530" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D530"/>
       <c r="E530"/>
       <c r="F530" t="s">
@@ -17567,7 +17661,1165 @@
         <v>3</v>
       </c>
     </row>
+    <row r="531" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A531" s="9">
+        <v>221</v>
+      </c>
+      <c r="B531" s="9"/>
+      <c r="C531" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="D531" s="9"/>
+      <c r="E531" s="9" t="s">
+        <v>1046</v>
+      </c>
+      <c r="F531" t="s">
+        <v>106</v>
+      </c>
+      <c r="G531">
+        <v>11</v>
+      </c>
+      <c r="H531">
+        <v>4</v>
+      </c>
+      <c r="I531">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="532" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D532"/>
+      <c r="E532"/>
+      <c r="F532" t="s">
+        <v>459</v>
+      </c>
+      <c r="I532">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="533" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D533"/>
+      <c r="E533"/>
+      <c r="F533" t="s">
+        <v>615</v>
+      </c>
+      <c r="H533">
+        <v>1</v>
+      </c>
+      <c r="I533">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="534" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D534"/>
+      <c r="E534"/>
+      <c r="F534" t="s">
+        <v>1047</v>
+      </c>
+      <c r="H534">
+        <v>3</v>
+      </c>
+      <c r="I534">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="535" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D535"/>
+      <c r="E535"/>
+      <c r="F535" t="s">
+        <v>459</v>
+      </c>
+      <c r="I535">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="536" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D536"/>
+      <c r="E536"/>
+      <c r="F536" t="s">
+        <v>1048</v>
+      </c>
+      <c r="H536">
+        <v>3</v>
+      </c>
+      <c r="I536">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="537" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A537" s="9">
+        <v>25</v>
+      </c>
+      <c r="B537" s="9"/>
+      <c r="C537" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="D537" s="9"/>
+      <c r="E537" s="9" t="s">
+        <v>1052</v>
+      </c>
+      <c r="F537" t="s">
+        <v>392</v>
+      </c>
+      <c r="G537">
+        <v>1</v>
+      </c>
+      <c r="H537">
+        <v>1</v>
+      </c>
+      <c r="I537">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="538" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D538"/>
+      <c r="E538"/>
+      <c r="F538" t="s">
+        <v>459</v>
+      </c>
+      <c r="I538">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="539" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A539" s="9">
+        <v>194</v>
+      </c>
+      <c r="B539" s="9"/>
+      <c r="C539" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="D539" s="9"/>
+      <c r="E539" s="9" t="s">
+        <v>1049</v>
+      </c>
+      <c r="F539" t="s">
+        <v>220</v>
+      </c>
+      <c r="G539">
+        <v>15</v>
+      </c>
+      <c r="H539">
+        <v>15</v>
+      </c>
+      <c r="I539">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="540" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D540"/>
+      <c r="E540"/>
+      <c r="F540" t="s">
+        <v>459</v>
+      </c>
+      <c r="I540">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="541" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A541" s="9">
+        <v>179</v>
+      </c>
+      <c r="B541" s="9"/>
+      <c r="C541" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="D541" s="9"/>
+      <c r="E541" s="9" t="s">
+        <v>1050</v>
+      </c>
+      <c r="F541" t="s">
+        <v>98</v>
+      </c>
+      <c r="G541">
+        <v>1</v>
+      </c>
+      <c r="H541">
+        <v>1</v>
+      </c>
+      <c r="I541">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="542" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D542"/>
+      <c r="E542"/>
+      <c r="F542" t="s">
+        <v>459</v>
+      </c>
+      <c r="I542">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="543" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A543" s="9">
+        <v>40</v>
+      </c>
+      <c r="B543" s="9"/>
+      <c r="C543" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D543" s="9"/>
+      <c r="E543" s="9" t="s">
+        <v>1053</v>
+      </c>
+      <c r="F543" t="s">
+        <v>330</v>
+      </c>
+      <c r="G543">
+        <v>2</v>
+      </c>
+      <c r="I543">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="544" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D544"/>
+      <c r="E544"/>
+      <c r="F544" t="s">
+        <v>985</v>
+      </c>
+      <c r="H544">
+        <v>2</v>
+      </c>
+      <c r="I544">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="545" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D545"/>
+      <c r="E545"/>
+      <c r="F545" t="s">
+        <v>1051</v>
+      </c>
+      <c r="I545">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="546" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A546" s="9">
+        <v>75</v>
+      </c>
+      <c r="B546" s="9"/>
+      <c r="C546" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="D546" s="9"/>
+      <c r="E546" s="9" t="s">
+        <v>1030</v>
+      </c>
+      <c r="F546" t="s">
+        <v>391</v>
+      </c>
+      <c r="G546">
+        <v>17</v>
+      </c>
+      <c r="H546">
+        <v>17</v>
+      </c>
+      <c r="I546">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="547" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D547"/>
+      <c r="E547"/>
+      <c r="F547" t="s">
+        <v>459</v>
+      </c>
+      <c r="I547">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="548" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A548" s="9">
+        <v>288</v>
+      </c>
+      <c r="B548" s="9"/>
+      <c r="C548" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="D548" s="9"/>
+      <c r="E548" s="9" t="s">
+        <v>1046</v>
+      </c>
+      <c r="F548" t="s">
+        <v>92</v>
+      </c>
+      <c r="G548">
+        <v>5</v>
+      </c>
+      <c r="H548">
+        <v>5</v>
+      </c>
+      <c r="I548">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="549" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D549"/>
+      <c r="E549"/>
+      <c r="F549" t="s">
+        <v>459</v>
+      </c>
+      <c r="I549">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="550" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A550" s="9">
+        <v>184</v>
+      </c>
+      <c r="B550" s="9"/>
+      <c r="C550" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="D550" s="9"/>
+      <c r="E550" s="9" t="s">
+        <v>1030</v>
+      </c>
+      <c r="F550" t="s">
+        <v>404</v>
+      </c>
+      <c r="G550">
+        <v>15</v>
+      </c>
+      <c r="H550">
+        <v>3</v>
+      </c>
+      <c r="I550">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="551" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D551"/>
+      <c r="E551"/>
+      <c r="F551" t="s">
+        <v>459</v>
+      </c>
+      <c r="I551">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="552" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D552"/>
+      <c r="E552"/>
+      <c r="F552" t="s">
+        <v>755</v>
+      </c>
+      <c r="H552">
+        <v>3</v>
+      </c>
+      <c r="I552">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="553" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D553"/>
+      <c r="E553"/>
+      <c r="F553" t="s">
+        <v>993</v>
+      </c>
+      <c r="H553">
+        <v>1</v>
+      </c>
+      <c r="I553">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="554" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D554"/>
+      <c r="E554"/>
+      <c r="F554" t="s">
+        <v>995</v>
+      </c>
+      <c r="H554">
+        <v>1</v>
+      </c>
+      <c r="I554">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="555" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D555"/>
+      <c r="E555"/>
+      <c r="F555" t="s">
+        <v>996</v>
+      </c>
+      <c r="H555">
+        <v>3</v>
+      </c>
+      <c r="I555">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="556" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D556"/>
+      <c r="E556"/>
+      <c r="F556" t="s">
+        <v>994</v>
+      </c>
+      <c r="H556">
+        <v>4</v>
+      </c>
+      <c r="I556">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="557" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A557" s="9">
+        <v>180</v>
+      </c>
+      <c r="B557" s="9"/>
+      <c r="C557" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="D557" s="9"/>
+      <c r="E557" s="9" t="s">
+        <v>1030</v>
+      </c>
+      <c r="F557" t="s">
+        <v>210</v>
+      </c>
+      <c r="H557">
+        <v>1</v>
+      </c>
+      <c r="I557">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="558" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D558"/>
+      <c r="E558"/>
+      <c r="F558" t="s">
+        <v>459</v>
+      </c>
+      <c r="I558">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="559" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A559" s="9">
+        <v>228</v>
+      </c>
+      <c r="B559" s="9"/>
+      <c r="C559" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="D559" s="9"/>
+      <c r="E559" s="9" t="s">
+        <v>1059</v>
+      </c>
+      <c r="F559" t="s">
+        <v>119</v>
+      </c>
+      <c r="G559">
+        <v>7</v>
+      </c>
+      <c r="H559">
+        <v>3</v>
+      </c>
+      <c r="I559">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="560" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D560"/>
+      <c r="E560"/>
+      <c r="F560" t="s">
+        <v>459</v>
+      </c>
+      <c r="I560">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="561" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D561"/>
+      <c r="E561"/>
+      <c r="F561" t="s">
+        <v>1055</v>
+      </c>
+      <c r="H561">
+        <v>1</v>
+      </c>
+      <c r="I561">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="562" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D562"/>
+      <c r="E562"/>
+      <c r="F562" t="s">
+        <v>985</v>
+      </c>
+      <c r="H562">
+        <v>2</v>
+      </c>
+      <c r="I562">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="563" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D563"/>
+      <c r="E563"/>
+      <c r="F563" t="s">
+        <v>622</v>
+      </c>
+      <c r="I563">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="564" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D564"/>
+      <c r="E564"/>
+      <c r="F564" t="s">
+        <v>986</v>
+      </c>
+      <c r="I564">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="565" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D565"/>
+      <c r="E565"/>
+      <c r="F565" t="s">
+        <v>1056</v>
+      </c>
+      <c r="I565">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="566" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D566"/>
+      <c r="E566"/>
+      <c r="F566" t="s">
+        <v>460</v>
+      </c>
+      <c r="H566">
+        <v>1</v>
+      </c>
+      <c r="I566">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="567" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A567" s="9">
+        <v>142</v>
+      </c>
+      <c r="B567" s="9"/>
+      <c r="C567" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D567" s="9"/>
+      <c r="E567" s="9" t="s">
+        <v>1060</v>
+      </c>
+      <c r="F567" t="s">
+        <v>87</v>
+      </c>
+      <c r="G567">
+        <v>7</v>
+      </c>
+      <c r="I567">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="568" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D568"/>
+      <c r="E568"/>
+      <c r="F568" t="s">
+        <v>459</v>
+      </c>
+      <c r="I568">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="569" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D569"/>
+      <c r="E569"/>
+      <c r="F569" t="s">
+        <v>460</v>
+      </c>
+      <c r="H569">
+        <v>1</v>
+      </c>
+      <c r="I569">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="570" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D570"/>
+      <c r="E570"/>
+      <c r="F570" t="s">
+        <v>622</v>
+      </c>
+      <c r="I570">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="571" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D571"/>
+      <c r="E571"/>
+      <c r="F571" t="s">
+        <v>1057</v>
+      </c>
+      <c r="I571">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="572" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D572"/>
+      <c r="E572"/>
+      <c r="F572" t="s">
+        <v>1058</v>
+      </c>
+      <c r="I572">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="573" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D573"/>
+      <c r="E573"/>
+      <c r="F573" t="s">
+        <v>985</v>
+      </c>
+      <c r="I573">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="574" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D574"/>
+      <c r="E574"/>
+      <c r="F574" t="s">
+        <v>756</v>
+      </c>
+      <c r="H574">
+        <v>6</v>
+      </c>
+      <c r="I574">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="575" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A575" s="69">
+        <v>346</v>
+      </c>
+      <c r="B575" s="9"/>
+      <c r="C575" s="9" t="s">
+        <v>1061</v>
+      </c>
+      <c r="D575" s="9"/>
+      <c r="E575" s="9" t="s">
+        <v>1054</v>
+      </c>
+      <c r="I575">
+        <v>1</v>
+      </c>
+      <c r="K575" t="s">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="576" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A576" s="9">
+        <v>126</v>
+      </c>
+      <c r="B576" s="9"/>
+      <c r="C576" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="D576" s="9"/>
+      <c r="E576" s="9" t="s">
+        <v>1062</v>
+      </c>
+      <c r="F576" t="s">
+        <v>366</v>
+      </c>
+      <c r="G576">
+        <v>10</v>
+      </c>
+      <c r="H576">
+        <v>9</v>
+      </c>
+      <c r="I576">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="577" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D577"/>
+      <c r="E577"/>
+      <c r="F577" t="s">
+        <v>459</v>
+      </c>
+      <c r="I577">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="578" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D578"/>
+      <c r="E578"/>
+      <c r="F578" t="s">
+        <v>460</v>
+      </c>
+      <c r="H578">
+        <v>1</v>
+      </c>
+      <c r="I578">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="579" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D579"/>
+      <c r="E579"/>
+      <c r="F579" t="s">
+        <v>1058</v>
+      </c>
+      <c r="I579">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="580" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D580"/>
+      <c r="E580"/>
+      <c r="F580" t="s">
+        <v>985</v>
+      </c>
+      <c r="I580">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="581" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A581" s="9">
+        <v>345</v>
+      </c>
+      <c r="B581" s="9"/>
+      <c r="C581" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="D581" s="9"/>
+      <c r="E581" s="9" t="s">
+        <v>1064</v>
+      </c>
+      <c r="F581" t="s">
+        <v>699</v>
+      </c>
+      <c r="I581">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="582" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D582"/>
+      <c r="E582"/>
+      <c r="F582" t="s">
+        <v>459</v>
+      </c>
+      <c r="I582">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="583" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A583" s="9">
+        <v>169</v>
+      </c>
+      <c r="B583" s="9"/>
+      <c r="C583" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="D583" s="9"/>
+      <c r="E583" s="9" t="s">
+        <v>1049</v>
+      </c>
+      <c r="F583" t="s">
+        <v>452</v>
+      </c>
+      <c r="I583">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="584" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D584"/>
+      <c r="E584"/>
+      <c r="F584" t="s">
+        <v>459</v>
+      </c>
+      <c r="I584">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="585" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A585" s="9">
+        <v>118</v>
+      </c>
+      <c r="B585" s="9"/>
+      <c r="C585" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D585" s="9"/>
+      <c r="E585" s="9" t="s">
+        <v>1065</v>
+      </c>
+      <c r="F585" t="s">
+        <v>76</v>
+      </c>
+      <c r="G585">
+        <v>5</v>
+      </c>
+      <c r="H585">
+        <v>4</v>
+      </c>
+      <c r="I585">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="586" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D586"/>
+      <c r="E586"/>
+      <c r="F586" t="s">
+        <v>459</v>
+      </c>
+      <c r="I586">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="587" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D587"/>
+      <c r="E587"/>
+      <c r="F587" t="s">
+        <v>643</v>
+      </c>
+      <c r="H587">
+        <v>1</v>
+      </c>
+      <c r="I587">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="588" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A588" s="9">
+        <v>144</v>
+      </c>
+      <c r="B588" s="9"/>
+      <c r="C588" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="D588" s="9"/>
+      <c r="E588" s="9" t="s">
+        <v>1066</v>
+      </c>
+      <c r="F588" t="s">
+        <v>181</v>
+      </c>
+      <c r="G588">
+        <v>1</v>
+      </c>
+      <c r="H588">
+        <v>1</v>
+      </c>
+      <c r="I588">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="589" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D589"/>
+      <c r="E589"/>
+      <c r="F589" t="s">
+        <v>459</v>
+      </c>
+      <c r="I589">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="590" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A590" s="9">
+        <v>332</v>
+      </c>
+      <c r="B590" s="9"/>
+      <c r="C590" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D590" s="9"/>
+      <c r="E590" s="9" t="s">
+        <v>1067</v>
+      </c>
+      <c r="F590" t="s">
+        <v>74</v>
+      </c>
+      <c r="G590">
+        <v>12</v>
+      </c>
+      <c r="H590">
+        <v>2</v>
+      </c>
+      <c r="I590">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="591" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D591"/>
+      <c r="E591"/>
+      <c r="F591" t="s">
+        <v>459</v>
+      </c>
+      <c r="H591">
+        <v>1</v>
+      </c>
+      <c r="I591">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="592" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D592"/>
+      <c r="E592"/>
+      <c r="F592" t="s">
+        <v>1068</v>
+      </c>
+      <c r="H592">
+        <v>1</v>
+      </c>
+      <c r="I592">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="593" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D593"/>
+      <c r="E593"/>
+      <c r="F593" t="s">
+        <v>1069</v>
+      </c>
+      <c r="H593">
+        <v>1</v>
+      </c>
+      <c r="I593">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="594" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D594"/>
+      <c r="E594"/>
+      <c r="F594" t="s">
+        <v>1070</v>
+      </c>
+      <c r="I594">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="595" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D595"/>
+      <c r="E595"/>
+      <c r="F595" t="s">
+        <v>466</v>
+      </c>
+      <c r="H595">
+        <v>1</v>
+      </c>
+      <c r="I595">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="596" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D596"/>
+      <c r="E596"/>
+      <c r="F596" t="s">
+        <v>1071</v>
+      </c>
+      <c r="H596">
+        <v>1</v>
+      </c>
+      <c r="I596">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="597" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D597"/>
+      <c r="E597"/>
+      <c r="F597" t="s">
+        <v>468</v>
+      </c>
+      <c r="H597">
+        <v>1</v>
+      </c>
+      <c r="I597">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="598" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D598"/>
+      <c r="E598"/>
+      <c r="F598" t="s">
+        <v>982</v>
+      </c>
+      <c r="I598">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="599" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D599"/>
+      <c r="E599"/>
+      <c r="F599" t="s">
+        <v>1072</v>
+      </c>
+      <c r="H599">
+        <v>1</v>
+      </c>
+      <c r="I599">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="600" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D600"/>
+      <c r="E600"/>
+      <c r="F600" t="s">
+        <v>836</v>
+      </c>
+      <c r="H600">
+        <v>1</v>
+      </c>
+      <c r="I600">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="601" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D601"/>
+      <c r="E601"/>
+      <c r="F601" t="s">
+        <v>1073</v>
+      </c>
+      <c r="H601">
+        <v>1</v>
+      </c>
+      <c r="I601">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="602" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D602"/>
+      <c r="E602"/>
+      <c r="F602" t="s">
+        <v>1074</v>
+      </c>
+      <c r="H602">
+        <v>1</v>
+      </c>
+      <c r="I602">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="603" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A603" s="9">
+        <v>104</v>
+      </c>
+      <c r="B603" s="9"/>
+      <c r="C603" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D603" s="9"/>
+      <c r="E603" s="9" t="s">
+        <v>1075</v>
+      </c>
+      <c r="F603" t="s">
+        <v>67</v>
+      </c>
+      <c r="G603">
+        <v>8</v>
+      </c>
+      <c r="H603">
+        <v>3</v>
+      </c>
+      <c r="I603">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="604" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D604"/>
+      <c r="E604"/>
+      <c r="F604" t="s">
+        <v>459</v>
+      </c>
+      <c r="I604">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="605" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D605"/>
+      <c r="E605"/>
+      <c r="F605" t="s">
+        <v>792</v>
+      </c>
+      <c r="I605">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="606" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D606"/>
+      <c r="E606"/>
+      <c r="F606" t="s">
+        <v>228</v>
+      </c>
+      <c r="H606">
+        <v>5</v>
+      </c>
+      <c r="I606">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="607" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D607"/>
+      <c r="E607"/>
+      <c r="F607" t="s">
+        <v>459</v>
+      </c>
+      <c r="I607">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="608" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A608" s="9">
+        <v>19</v>
+      </c>
+      <c r="B608" s="9"/>
+      <c r="C608" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D608" s="9"/>
+      <c r="E608" s="9" t="s">
+        <v>1030</v>
+      </c>
+      <c r="F608" t="s">
+        <v>4</v>
+      </c>
+      <c r="G608">
+        <v>53</v>
+      </c>
+      <c r="H608">
+        <v>37</v>
+      </c>
+      <c r="I608">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="609" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D609"/>
+      <c r="E609"/>
+      <c r="F609" t="s">
+        <v>459</v>
+      </c>
+      <c r="H609">
+        <v>15</v>
+      </c>
+      <c r="I609">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="610" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D610"/>
+      <c r="E610"/>
+      <c r="F610" t="s">
+        <v>980</v>
+      </c>
+      <c r="I610">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:O580" xr:uid="{AD54439F-40DB-4068-9758-9F0A5DA03583}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -17589,11 +18841,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="51" t="s">
         <v>495</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="52"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="53"/>
     </row>
     <row r="2" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
@@ -17621,9 +18873,9 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="53"/>
-      <c r="B4" s="54"/>
-      <c r="C4" s="55"/>
+      <c r="A4" s="54"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="56"/>
     </row>
     <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
@@ -17659,9 +18911,9 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="53"/>
-      <c r="B8" s="54"/>
-      <c r="C8" s="55"/>
+      <c r="A8" s="54"/>
+      <c r="B8" s="55"/>
+      <c r="C8" s="56"/>
     </row>
     <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
@@ -17678,9 +18930,9 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="53"/>
-      <c r="B10" s="54"/>
-      <c r="C10" s="55"/>
+      <c r="A10" s="54"/>
+      <c r="B10" s="55"/>
+      <c r="C10" s="56"/>
     </row>
     <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
@@ -17697,9 +18949,9 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="53"/>
-      <c r="B12" s="54"/>
-      <c r="C12" s="55"/>
+      <c r="A12" s="54"/>
+      <c r="B12" s="55"/>
+      <c r="C12" s="56"/>
     </row>
     <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="13" t="s">
@@ -17713,9 +18965,9 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="53"/>
-      <c r="B14" s="54"/>
-      <c r="C14" s="55"/>
+      <c r="A14" s="54"/>
+      <c r="B14" s="55"/>
+      <c r="C14" s="56"/>
     </row>
     <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="21" t="s">
@@ -17729,9 +18981,9 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="47"/>
-      <c r="B16" s="48"/>
-      <c r="C16" s="49"/>
+      <c r="A16" s="48"/>
+      <c r="B16" s="49"/>
+      <c r="C16" s="50"/>
     </row>
     <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="13" t="s">
@@ -17745,9 +18997,9 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="47"/>
-      <c r="B18" s="48"/>
-      <c r="C18" s="49"/>
+      <c r="A18" s="48"/>
+      <c r="B18" s="49"/>
+      <c r="C18" s="50"/>
     </row>
     <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="13" t="s">
@@ -17761,9 +19013,9 @@
       </c>
     </row>
     <row r="20" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="47"/>
-      <c r="B20" s="48"/>
-      <c r="C20" s="49"/>
+      <c r="A20" s="48"/>
+      <c r="B20" s="49"/>
+      <c r="C20" s="50"/>
     </row>
     <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="13" t="s">
@@ -17777,9 +19029,9 @@
       </c>
     </row>
     <row r="22" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="47"/>
-      <c r="B22" s="48"/>
-      <c r="C22" s="49"/>
+      <c r="A22" s="48"/>
+      <c r="B22" s="49"/>
+      <c r="C22" s="50"/>
     </row>
     <row r="23" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="13" t="s">
@@ -17825,11 +19077,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="51" t="s">
         <v>517</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="52"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="53"/>
     </row>
     <row r="2" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
@@ -17850,13 +19102,13 @@
       <c r="C3" s="23"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="60" t="s">
+      <c r="A4" s="61" t="s">
         <v>521</v>
       </c>
       <c r="B4" s="24" t="s">
         <v>522</v>
       </c>
-      <c r="C4" s="62" t="s">
+      <c r="C4" s="63" t="s">
         <v>523</v>
       </c>
       <c r="D4" s="7">
@@ -17864,11 +19116,11 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="61"/>
+      <c r="A5" s="62"/>
       <c r="B5" s="25" t="s">
         <v>524</v>
       </c>
-      <c r="C5" s="63"/>
+      <c r="C5" s="64"/>
     </row>
     <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="26" t="s">
@@ -17882,40 +19134,40 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="64" t="s">
+      <c r="A7" s="65" t="s">
         <v>528</v>
       </c>
       <c r="B7" s="29" t="s">
         <v>529</v>
       </c>
-      <c r="C7" s="66" t="s">
+      <c r="C7" s="67" t="s">
         <v>530</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="65"/>
+      <c r="A8" s="66"/>
       <c r="B8" s="30" t="s">
         <v>531</v>
       </c>
-      <c r="C8" s="67"/>
+      <c r="C8" s="68"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="64" t="s">
+      <c r="A9" s="65" t="s">
         <v>532</v>
       </c>
       <c r="B9" s="29" t="s">
         <v>529</v>
       </c>
-      <c r="C9" s="66" t="s">
+      <c r="C9" s="67" t="s">
         <v>530</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="65"/>
+      <c r="A10" s="66"/>
       <c r="B10" s="30" t="s">
         <v>531</v>
       </c>
-      <c r="C10" s="67"/>
+      <c r="C10" s="68"/>
     </row>
     <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="26" t="s">
@@ -17999,22 +19251,22 @@
       <c r="C19" s="35"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="56" t="s">
+      <c r="A20" s="57" t="s">
         <v>543</v>
       </c>
       <c r="B20" s="36" t="s">
         <v>544</v>
       </c>
-      <c r="C20" s="58" t="s">
+      <c r="C20" s="59" t="s">
         <v>530</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="57"/>
+      <c r="A21" s="58"/>
       <c r="B21" s="16" t="s">
         <v>545</v>
       </c>
-      <c r="C21" s="59"/>
+      <c r="C21" s="60"/>
     </row>
     <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="32"/>

</xml_diff>